<commit_message>
Adding ADBE ADI AGCO AL ALB
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD5A4A-4EE6-437C-816B-B07029FD7C21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BEF468-F4CA-42D1-BB0F-2717622B0560}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="369">
   <si>
     <t>SCVL</t>
   </si>
@@ -1128,6 +1128,12 @@
   </si>
   <si>
     <t xml:space="preserve">See the huge drop - Asking Ann about it </t>
+  </si>
+  <si>
+    <t>Seems like a nice growth ahead - Ann's adjusted analyst lines are flatter than the actual analysts. Understand why</t>
+  </si>
+  <si>
+    <t>One stock that reports whose fiscal is Oct-Oct. Use this as an experiment case</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1698,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2074,6 +2080,12 @@
       <c r="B28" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H28" s="3">
+        <v>43690</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
@@ -2082,6 +2094,12 @@
       <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H29" s="3">
+        <v>43690</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
@@ -2090,6 +2108,9 @@
       <c r="B30" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H30" s="3">
+        <v>43690</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
@@ -2098,6 +2119,9 @@
       <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H31" s="3">
+        <v>43690</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -2105,6 +2129,9 @@
       </c>
       <c r="B32" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="H32" s="3">
+        <v>43690</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -4583,25 +4610,25 @@
     <cfRule type="duplicateValues" dxfId="17" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D341:D343">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D344">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D345:D347">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D346:D347">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D346:D347">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D348:D358">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D348:D358">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7287,34 +7314,34 @@
     <sortCondition ref="A1:A331"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H4">
-    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H8">
-    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136:B330">
-    <cfRule type="duplicateValues" dxfId="7" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding ALGN ALOT ALSN AMAT AME
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BEF468-F4CA-42D1-BB0F-2717622B0560}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E16D55-13C3-4617-8456-BC1B451D7331}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="370">
   <si>
     <t>SCVL</t>
   </si>
@@ -1134,6 +1134,9 @@
   </si>
   <si>
     <t>One stock that reports whose fiscal is Oct-Oct. Use this as an experiment case</t>
+  </si>
+  <si>
+    <t>Something wrong with my chart - need to compare Ann w/mine to see what is going on</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1700,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2134,47 +2137,65 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H33" s="3">
+        <v>43690</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>195</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H34" s="3">
+        <v>43690</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>196</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H35" s="3">
+        <v>43690</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>197</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H36" s="3">
+        <v>43690</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>198</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H37" s="3">
+        <v>43690</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>199</v>
       </c>
@@ -2182,7 +2203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>200</v>
       </c>
@@ -2190,7 +2211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>201</v>
       </c>
@@ -2198,7 +2219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>202</v>
       </c>
@@ -2206,7 +2227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>76</v>
       </c>
@@ -2214,7 +2235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>203</v>
       </c>
@@ -2222,7 +2243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>69</v>
       </c>
@@ -2230,7 +2251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>62</v>
       </c>
@@ -2238,12 +2259,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>204</v>
       </c>
@@ -2251,7 +2272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>205</v>
       </c>

</xml_diff>

<commit_message>
More stuff for ALOT
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E16D55-13C3-4617-8456-BC1B451D7331}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75D0609-31A3-4F6F-801C-93641CFFFF3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1136,7 +1136,7 @@
     <t>One stock that reports whose fiscal is Oct-Oct. Use this as an experiment case</t>
   </si>
   <si>
-    <t>Something wrong with my chart - need to compare Ann w/mine to see what is going on</t>
+    <t xml:space="preserve">This does not plot correctly with xtick and xticklabels on…not sure what is wrong though. If plotted without labels, it plots correctly </t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1701,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding AMOT ANET ANSS ANTM
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75D0609-31A3-4F6F-801C-93641CFFFF3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DE4335-38F4-4473-AE5C-F14B726EA16B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="371">
   <si>
     <t>SCVL</t>
   </si>
@@ -1137,6 +1137,9 @@
   </si>
   <si>
     <t xml:space="preserve">This does not plot correctly with xtick and xticklabels on…not sure what is wrong though. If plotted without labels, it plots correctly </t>
+  </si>
+  <si>
+    <t>Ann does not have this chart???</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1704,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2202,6 +2205,9 @@
       <c r="B38" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H38" s="3">
+        <v>43691</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -2210,6 +2216,9 @@
       <c r="B39" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H39" s="3">
+        <v>43691</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -2218,6 +2227,12 @@
       <c r="B40" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H40" s="3">
+        <v>43691</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
@@ -2226,6 +2241,9 @@
       <c r="B41" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H41" s="3">
+        <v>43691</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -2233,6 +2251,9 @@
       </c>
       <c r="B42" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="H42" s="3">
+        <v>43691</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding AOS APH ASGN ATHM ATVI AUDC AVAV AVGO AXP AYI AZPN
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DE4335-38F4-4473-AE5C-F14B726EA16B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF285CA6-568F-4A9D-976E-68CB2BF2FE44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2799" uniqueCount="373">
   <si>
     <t>SCVL</t>
   </si>
@@ -1140,6 +1140,12 @@
   </si>
   <si>
     <t>Ann does not have this chart???</t>
+  </si>
+  <si>
+    <t>Not found???</t>
+  </si>
+  <si>
+    <t>This one looks good</t>
   </si>
 </sst>
 </file>
@@ -1186,12 +1192,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1206,7 +1218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1228,6 +1240,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,11 +1714,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L358"/>
+  <dimension ref="A1:L357"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2263,172 +2277,211 @@
       <c r="B43" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H43" s="3">
+        <v>43693</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H44" s="3">
+        <v>43693</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H45" s="3">
+        <v>43693</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>127</v>
+      <c r="A46" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="3">
+        <v>43693</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H47" s="3">
+        <v>43693</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>205</v>
+      <c r="A48" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H48" s="3">
+        <v>43693</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>207</v>
+      <c r="H49" s="3">
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>169</v>
+      <c r="H50" s="3">
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>104</v>
+      <c r="H51" s="3">
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H52" s="3">
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>170</v>
       </c>
+      <c r="B55" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="B56" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>128</v>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>210</v>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>122</v>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>211</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>211</v>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>94</v>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>212</v>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>34</v>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>213</v>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>75</v>
+      <c r="A65" s="10" t="s">
+        <v>214</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>15</v>
@@ -2436,7 +2489,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>15</v>
@@ -2444,31 +2497,31 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
-        <v>216</v>
+      <c r="A68" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>217</v>
+      <c r="A69" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>72</v>
+      <c r="A70" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>15</v>
@@ -2476,7 +2529,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>15</v>
@@ -2484,23 +2537,23 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>220</v>
+      <c r="A73" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
-        <v>171</v>
+      <c r="A74" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>15</v>
@@ -2508,36 +2561,36 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>33</v>
+      <c r="A76" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>222</v>
+      <c r="A78" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>87</v>
+      <c r="A79" s="11" t="s">
+        <v>172</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>15</v>
@@ -2545,7 +2598,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>15</v>
@@ -2553,7 +2606,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>15</v>
@@ -2561,23 +2614,23 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
-        <v>173</v>
+      <c r="A83" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>135</v>
+      <c r="A84" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>15</v>
@@ -2585,23 +2638,23 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
-        <v>226</v>
+      <c r="A86" s="9" t="s">
+        <v>227</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
-        <v>227</v>
+      <c r="A87" s="11" t="s">
+        <v>228</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>15</v>
@@ -2609,15 +2662,15 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
-        <v>229</v>
+      <c r="A89" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>15</v>
@@ -2625,7 +2678,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>15</v>
@@ -2633,7 +2686,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>15</v>
@@ -2641,7 +2694,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>15</v>
@@ -2649,7 +2702,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>15</v>
@@ -2657,20 +2710,20 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>60</v>
+        <v>32</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>32</v>
+      <c r="A96" s="11" t="s">
+        <v>230</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>15</v>
@@ -2678,7 +2731,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>15</v>
@@ -2686,15 +2739,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
-        <v>232</v>
+      <c r="A99" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>15</v>
@@ -2702,23 +2755,23 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>79</v>
+      <c r="A101" s="9" t="s">
+        <v>233</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
-        <v>233</v>
+      <c r="A102" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>15</v>
@@ -2726,47 +2779,47 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
-        <v>235</v>
+      <c r="A104" s="9" t="s">
+        <v>236</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
-        <v>236</v>
+      <c r="A105" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>137</v>
+      <c r="A106" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
-        <v>237</v>
+      <c r="A107" s="9" t="s">
+        <v>238</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
-        <v>238</v>
+      <c r="A108" s="11" t="s">
+        <v>239</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>15</v>
@@ -2774,7 +2827,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>15</v>
@@ -2782,7 +2835,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>15</v>
@@ -2790,7 +2843,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>15</v>
@@ -2798,7 +2851,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>15</v>
@@ -2806,7 +2859,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>15</v>
@@ -2814,15 +2867,15 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="11" t="s">
-        <v>245</v>
+      <c r="A115" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>15</v>
@@ -2830,7 +2883,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>15</v>
@@ -2838,47 +2891,47 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>80</v>
+      <c r="A118" s="10" t="s">
+        <v>246</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="s">
-        <v>246</v>
+      <c r="A119" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>43</v>
+      <c r="A120" s="11" t="s">
+        <v>247</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="11" t="s">
-        <v>247</v>
+      <c r="A121" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
-        <v>248</v>
+      <c r="A122" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>15</v>
@@ -2886,63 +2939,63 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>68</v>
+      <c r="A124" s="11" t="s">
+        <v>174</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="11" t="s">
-        <v>174</v>
+      <c r="A125" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>64</v>
+      <c r="A126" s="7" t="s">
+        <v>175</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
-        <v>175</v>
+      <c r="A127" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>25</v>
+      <c r="A128" s="11" t="s">
+        <v>249</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="11" t="s">
-        <v>249</v>
+      <c r="A129" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="9" t="s">
-        <v>250</v>
+      <c r="A130" s="11" t="s">
+        <v>251</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>15</v>
@@ -2950,7 +3003,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>15</v>
@@ -2958,7 +3011,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>15</v>
@@ -2966,7 +3019,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
-        <v>253</v>
+        <v>176</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>15</v>
@@ -2974,7 +3027,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>176</v>
+        <v>254</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>15</v>
@@ -2982,68 +3035,68 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="11" t="s">
-        <v>255</v>
+      <c r="A136" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="9" t="s">
-        <v>177</v>
+      <c r="A137" s="11" t="s">
+        <v>256</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="11" t="s">
-        <v>256</v>
+      <c r="A138" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>31</v>
+      <c r="A139" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>15</v>
+      <c r="A140" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>111</v>
+      <c r="A141" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="11" t="s">
-        <v>259</v>
+      <c r="A143" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>15</v>
@@ -3051,7 +3104,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>15</v>
@@ -3059,31 +3112,31 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>42</v>
+      <c r="A146" s="11" t="s">
+        <v>260</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="11" t="s">
-        <v>260</v>
+      <c r="A147" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="9" t="s">
-        <v>178</v>
+      <c r="A148" s="11" t="s">
+        <v>261</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>15</v>
@@ -3091,39 +3144,39 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="11" t="s">
-        <v>262</v>
+      <c r="A150" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>117</v>
+      <c r="A151" s="11" t="s">
+        <v>263</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="11" t="s">
-        <v>263</v>
+      <c r="A152" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>100</v>
+      <c r="A153" s="11" t="s">
+        <v>264</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>15</v>
@@ -3131,15 +3184,15 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="11" t="s">
-        <v>265</v>
+      <c r="A155" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>15</v>
@@ -3147,28 +3200,28 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>123</v>
+      <c r="A157" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="11" t="s">
-        <v>266</v>
+      <c r="A158" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
-        <v>27</v>
+      <c r="A159" s="9" t="s">
+        <v>267</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>15</v>
@@ -3176,44 +3229,44 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="9" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>15</v>
+      <c r="A161" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>30</v>
+      <c r="A162" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="11" t="s">
-        <v>269</v>
+      <c r="A163" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="2" t="s">
-        <v>58</v>
+      <c r="A164" s="11" t="s">
+        <v>270</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="11" t="s">
-        <v>270</v>
+      <c r="A165" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>15</v>
@@ -3221,23 +3274,23 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
-        <v>109</v>
+      <c r="A167" s="10" t="s">
+        <v>271</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="10" t="s">
-        <v>271</v>
+      <c r="A168" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>15</v>
@@ -3245,23 +3298,23 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="11" t="s">
-        <v>273</v>
+      <c r="A170" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>138</v>
+      <c r="A171" s="11" t="s">
+        <v>274</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>15</v>
@@ -3269,7 +3322,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>15</v>
@@ -3277,15 +3330,15 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="11" t="s">
-        <v>276</v>
+      <c r="A174" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>15</v>
@@ -3293,23 +3346,23 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>70</v>
+      <c r="A176" s="11" t="s">
+        <v>277</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="11" t="s">
-        <v>277</v>
+      <c r="A177" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>15</v>
@@ -3317,31 +3370,31 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="9" t="s">
-        <v>179</v>
+        <v>278</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="9" t="s">
-        <v>278</v>
+      <c r="A179" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>41</v>
+      <c r="A180" s="11" t="s">
+        <v>279</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="11" t="s">
-        <v>279</v>
+      <c r="A181" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>15</v>
@@ -3349,20 +3402,20 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="2" t="s">
-        <v>24</v>
+      <c r="A183" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="10" t="s">
-        <v>280</v>
+      <c r="A184" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>15</v>
@@ -3370,15 +3423,15 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
-        <v>57</v>
+      <c r="A186" s="11" t="s">
+        <v>281</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>15</v>
@@ -3386,47 +3439,47 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="11" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="11" t="s">
-        <v>282</v>
+      <c r="A188" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
-        <v>49</v>
+      <c r="A189" s="9" t="s">
+        <v>180</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="9" t="s">
-        <v>180</v>
+      <c r="A190" s="11" t="s">
+        <v>283</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="11" t="s">
-        <v>283</v>
+      <c r="A191" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>40</v>
+      <c r="A192" s="11" t="s">
+        <v>284</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>15</v>
@@ -3434,7 +3487,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>15</v>
@@ -3442,7 +3495,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>15</v>
@@ -3450,7 +3503,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>15</v>
@@ -3458,7 +3511,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>15</v>
@@ -3466,23 +3519,23 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="11" t="s">
-        <v>289</v>
+      <c r="A198" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="9" t="s">
-        <v>290</v>
+      <c r="A199" s="11" t="s">
+        <v>291</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>15</v>
@@ -3490,15 +3543,15 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="11" t="s">
-        <v>292</v>
+      <c r="A201" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>15</v>
@@ -3506,31 +3559,31 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
-        <v>56</v>
+      <c r="A203" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="11" t="s">
-        <v>293</v>
+      <c r="A204" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
-        <v>108</v>
+      <c r="A205" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>15</v>
@@ -3538,39 +3591,39 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="11" t="s">
-        <v>181</v>
+        <v>294</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="11" t="s">
-        <v>294</v>
+      <c r="A207" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>116</v>
+      <c r="A208" s="11" t="s">
+        <v>295</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="11" t="s">
-        <v>295</v>
+      <c r="A209" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
-        <v>92</v>
+      <c r="A210" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>15</v>
@@ -3578,23 +3631,23 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="11" t="s">
-        <v>182</v>
+        <v>296</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="11" t="s">
-        <v>296</v>
+      <c r="A212" s="9" t="s">
+        <v>297</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="9" t="s">
-        <v>297</v>
+      <c r="A213" s="11" t="s">
+        <v>298</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>15</v>
@@ -3602,15 +3655,15 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="11" t="s">
-        <v>299</v>
+      <c r="A215" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>15</v>
@@ -3618,7 +3671,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>15</v>
@@ -3626,23 +3679,23 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>124</v>
+        <v>66</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
-        <v>66</v>
+      <c r="A218" s="9" t="s">
+        <v>300</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="9" t="s">
-        <v>300</v>
+      <c r="A219" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>15</v>
@@ -3650,15 +3703,15 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="11" t="s">
-        <v>302</v>
+      <c r="A221" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>15</v>
@@ -3666,15 +3719,15 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
-        <v>98</v>
+      <c r="A223" s="11" t="s">
+        <v>303</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>15</v>
@@ -3682,7 +3735,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="11" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>15</v>
@@ -3690,7 +3743,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>15</v>
@@ -3698,31 +3751,31 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="11" t="s">
-        <v>306</v>
+      <c r="A227" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
-        <v>55</v>
+      <c r="A228" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="9" t="s">
-        <v>183</v>
+      <c r="A229" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>15</v>
@@ -3730,28 +3783,28 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
-        <v>106</v>
+      <c r="A231" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="11" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="11" t="s">
-        <v>308</v>
+      <c r="A233" s="9" t="s">
+        <v>309</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>15</v>
@@ -3759,15 +3812,15 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="9" t="s">
-        <v>310</v>
+      <c r="A235" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>15</v>
@@ -3775,20 +3828,20 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
-        <v>136</v>
+      <c r="A237" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="11" t="s">
-        <v>311</v>
+        <v>184</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>15</v>
@@ -3796,7 +3849,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="11" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>15</v>
@@ -3804,15 +3857,15 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="11" t="s">
-        <v>313</v>
+      <c r="A241" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>15</v>
@@ -3820,20 +3873,20 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="2" t="s">
-        <v>50</v>
+      <c r="A243" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="11" t="s">
-        <v>185</v>
+      <c r="A244" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>15</v>
@@ -3841,79 +3894,79 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>54</v>
+      <c r="A246" s="11" t="s">
+        <v>314</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="11" t="s">
-        <v>314</v>
+      <c r="A247" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="7" t="s">
-        <v>186</v>
+      <c r="A248" s="10" t="s">
+        <v>315</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="10" t="s">
-        <v>315</v>
+      <c r="A249" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
-        <v>53</v>
+      <c r="A250" s="11" t="s">
+        <v>316</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="11" t="s">
-        <v>316</v>
+      <c r="A251" s="9" t="s">
+        <v>317</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="9" t="s">
-        <v>317</v>
+      <c r="A252" s="11" t="s">
+        <v>318</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="11" t="s">
-        <v>318</v>
+      <c r="A253" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
-        <v>102</v>
+      <c r="A254" s="11" t="s">
+        <v>319</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>15</v>
@@ -3921,15 +3974,15 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="11" t="s">
-        <v>320</v>
+      <c r="A256" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>15</v>
@@ -3937,7 +3990,7 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>15</v>
@@ -3945,7 +3998,7 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>15</v>
@@ -3953,31 +4006,31 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A260" s="2" t="s">
-        <v>39</v>
+      <c r="A260" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A261" s="9" t="s">
-        <v>321</v>
+      <c r="A261" s="11" t="s">
+        <v>322</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A262" s="11" t="s">
-        <v>322</v>
+      <c r="A262" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>15</v>
@@ -3985,7 +4038,7 @@
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>15</v>
@@ -3993,7 +4046,7 @@
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>15</v>
@@ -4001,23 +4054,23 @@
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
-        <v>28</v>
+      <c r="A266" s="11" t="s">
+        <v>323</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A267" s="11" t="s">
-        <v>323</v>
+      <c r="A267" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>15</v>
@@ -4025,56 +4078,56 @@
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="J268" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K268" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L268" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
-        <v>0</v>
+      <c r="A269" s="11" t="s">
+        <v>324</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J269" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K269" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L269" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A270" s="11" t="s">
-        <v>324</v>
+      <c r="A270" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
-        <v>29</v>
+      <c r="A271" s="11" t="s">
+        <v>325</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A272" s="11" t="s">
-        <v>325</v>
+      <c r="A272" s="9" t="s">
+        <v>326</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="9" t="s">
-        <v>326</v>
+      <c r="A273" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>15</v>
@@ -4082,15 +4135,15 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>119</v>
+        <v>22</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2" t="s">
-        <v>22</v>
+      <c r="A275" s="11" t="s">
+        <v>327</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>15</v>
@@ -4098,7 +4151,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>15</v>
@@ -4106,41 +4159,41 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>15</v>
+      <c r="A278" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2" t="s">
-        <v>48</v>
+      <c r="A280" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="9" t="s">
-        <v>330</v>
+      <c r="A281" s="11" t="s">
+        <v>331</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="11" t="s">
-        <v>331</v>
+      <c r="A282" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>15</v>
@@ -4148,15 +4201,15 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2" t="s">
-        <v>101</v>
+      <c r="A284" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>15</v>
@@ -4164,31 +4217,31 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="11" t="s">
-        <v>333</v>
+      <c r="A286" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2" t="s">
-        <v>126</v>
+      <c r="A287" s="9" t="s">
+        <v>334</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="9" t="s">
-        <v>334</v>
+      <c r="A288" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>15</v>
@@ -4196,15 +4249,15 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2" t="s">
-        <v>99</v>
+      <c r="A290" s="11" t="s">
+        <v>335</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>15</v>
@@ -4212,7 +4265,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>15</v>
@@ -4220,31 +4273,31 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="11" t="s">
-        <v>337</v>
+      <c r="A293" s="10" t="s">
+        <v>338</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="10" t="s">
-        <v>338</v>
+      <c r="A294" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="11" t="s">
-        <v>339</v>
+      <c r="A295" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>15</v>
@@ -4252,7 +4305,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>15</v>
@@ -4260,15 +4313,15 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2" t="s">
-        <v>37</v>
+      <c r="A298" s="11" t="s">
+        <v>340</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>15</v>
@@ -4276,7 +4329,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>15</v>
@@ -4284,7 +4337,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>15</v>
@@ -4292,7 +4345,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>15</v>
@@ -4300,7 +4353,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>15</v>
@@ -4308,44 +4361,44 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="11" t="s">
-        <v>345</v>
+      <c r="A304" s="9" t="s">
+        <v>346</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="B305" s="2" t="s">
-        <v>15</v>
+      <c r="A305" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
-        <v>83</v>
+        <v>129</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="2" t="s">
-        <v>130</v>
+      <c r="A308" s="9" t="s">
+        <v>347</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>15</v>
@@ -4353,23 +4406,23 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="9" t="s">
-        <v>348</v>
+      <c r="A310" s="11" t="s">
+        <v>349</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="11" t="s">
-        <v>349</v>
+      <c r="A311" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>15</v>
@@ -4377,7 +4430,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>15</v>
@@ -4385,7 +4438,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>15</v>
@@ -4393,54 +4446,54 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B314" s="2" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="2" t="s">
-        <v>85</v>
+      <c r="A315" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="11" t="s">
-        <v>187</v>
+      <c r="A316" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="2" t="s">
-        <v>84</v>
+      <c r="A317" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>15</v>
+      <c r="A318" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="2" t="s">
-        <v>36</v>
+      <c r="A321" s="11" t="s">
+        <v>350</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>15</v>
@@ -4448,7 +4501,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="11" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>15</v>
@@ -4456,7 +4509,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>15</v>
@@ -4464,23 +4517,23 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="11" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="11" t="s">
-        <v>353</v>
+      <c r="A325" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="s">
-        <v>105</v>
+      <c r="A326" s="11" t="s">
+        <v>354</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>15</v>
@@ -4488,7 +4541,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>15</v>
@@ -4496,52 +4549,52 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="11" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="11" t="s">
-        <v>356</v>
+      <c r="A329" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="2" t="s">
-        <v>97</v>
+      <c r="A330" s="11" t="s">
+        <v>357</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="11" t="s">
-        <v>357</v>
+      <c r="A331" s="9" t="s">
+        <v>358</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="B332" s="2" t="s">
-        <v>15</v>
+      <c r="A332" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="s">
-        <v>46</v>
+      <c r="A333" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="12" t="s">
-        <v>359</v>
+      <c r="A334" s="11" t="s">
+        <v>360</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>15</v>
@@ -4549,7 +4602,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>15</v>
@@ -4557,7 +4610,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>15</v>
@@ -4565,7 +4618,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>15</v>
@@ -4573,19 +4626,14 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="B339" s="2" t="s">
-        <v>15</v>
-      </c>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D340" s="8"/>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D341" s="8"/>
@@ -4638,38 +4686,35 @@
     <row r="357" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D357" s="8"/>
     </row>
-    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D358" s="8"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L358">
-    <sortCondition ref="H2:H358"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L357">
+    <sortCondition ref="H2:H357"/>
   </sortState>
-  <conditionalFormatting sqref="A142:A339">
+  <conditionalFormatting sqref="A141:A338">
     <cfRule type="duplicateValues" dxfId="18" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A142:A339">
+  <conditionalFormatting sqref="A141:A338">
     <cfRule type="duplicateValues" dxfId="17" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D341:D343">
+  <conditionalFormatting sqref="D340:D342">
     <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D344">
+  <conditionalFormatting sqref="D343">
     <cfRule type="duplicateValues" dxfId="15" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D345:D347">
+  <conditionalFormatting sqref="D344:D346">
     <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D346:D347">
+  <conditionalFormatting sqref="D345:D346">
     <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D346:D347">
+  <conditionalFormatting sqref="D345:D346">
     <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D348:D358">
+  <conditionalFormatting sqref="D347:D357">
     <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D348:D358">
+  <conditionalFormatting sqref="D347:D357">
     <cfRule type="duplicateValues" dxfId="10" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding BA BABA BAC BBSI BBT BBY BIIB BKNG BOOM BR BSX BZUN
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF285CA6-568F-4A9D-976E-68CB2BF2FE44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45907C12-3B8A-4FD6-BFB7-59334B9CC90D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2799" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="374">
   <si>
     <t>SCVL</t>
   </si>
@@ -1146,6 +1146,9 @@
   </si>
   <si>
     <t>This one looks good</t>
+  </si>
+  <si>
+    <t>What a chart - what a growth - Ask Ann</t>
   </si>
 </sst>
 </file>
@@ -1717,8 +1720,8 @@
   <dimension ref="A1:L357"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2393,11 +2396,17 @@
       <c r="B53" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H53" s="3">
+        <v>43693</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="H54" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
@@ -2406,6 +2415,9 @@
       <c r="B55" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H55" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
@@ -2414,6 +2426,9 @@
       <c r="B56" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H56" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
@@ -2422,6 +2437,9 @@
       <c r="B57" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H57" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -2430,6 +2448,9 @@
       <c r="B58" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H58" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
@@ -2438,6 +2459,9 @@
       <c r="B59" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H59" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -2446,6 +2470,9 @@
       <c r="B60" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H60" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
@@ -2454,6 +2481,9 @@
       <c r="B61" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H61" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
@@ -2462,6 +2492,9 @@
       <c r="B62" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H62" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
@@ -2470,6 +2503,9 @@
       <c r="B63" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H63" s="3">
+        <v>43694</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -2478,16 +2514,25 @@
       <c r="B64" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H64" s="3">
+        <v>43694</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>214</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H65" s="3">
+        <v>43694</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>215</v>
       </c>
@@ -2495,7 +2540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>216</v>
       </c>
@@ -2503,7 +2548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>217</v>
       </c>
@@ -2511,7 +2556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
@@ -2519,7 +2564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>218</v>
       </c>
@@ -2527,7 +2572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>219</v>
       </c>
@@ -2535,7 +2580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>220</v>
       </c>
@@ -2543,7 +2588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>171</v>
       </c>
@@ -2551,7 +2596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>103</v>
       </c>
@@ -2559,12 +2604,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>221</v>
       </c>
@@ -2572,7 +2617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>222</v>
       </c>
@@ -2580,7 +2625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>87</v>
       </c>
@@ -2588,7 +2633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>172</v>
       </c>
@@ -2596,7 +2641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>223</v>
       </c>

</xml_diff>

<commit_message>
More experiments with Red lines
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45907C12-3B8A-4FD6-BFB7-59334B9CC90D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DFD926-17A0-41BE-BB4B-5CBA581ABA40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,9 @@
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$361</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="376">
   <si>
     <t>SCVL</t>
   </si>
@@ -1149,6 +1152,12 @@
   </si>
   <si>
     <t>What a chart - what a growth - Ask Ann</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>Chaff</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1258,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1717,11 +1826,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L357"/>
+  <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H319" sqref="H319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2539,6 +2648,7 @@
       <c r="B66" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H66" s="3"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
@@ -2547,6 +2657,7 @@
       <c r="B67" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H67" s="3"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -2555,14 +2666,16 @@
       <c r="B68" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
@@ -2571,6 +2684,7 @@
       <c r="B70" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
@@ -2579,6 +2693,7 @@
       <c r="B71" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
@@ -2587,6 +2702,7 @@
       <c r="B72" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
@@ -2595,19 +2711,22 @@
       <c r="B73" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="15" t="s">
         <v>103</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="15" t="s">
         <v>33</v>
       </c>
+      <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
@@ -2616,6 +2735,7 @@
       <c r="B76" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
@@ -2624,14 +2744,16 @@
       <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H77" s="3"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="15" t="s">
         <v>87</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H78" s="3"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
@@ -2640,6 +2762,7 @@
       <c r="B79" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H79" s="3"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
@@ -2649,7 +2772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>224</v>
       </c>
@@ -2657,118 +2780,127 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>173</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H82" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H83" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="B84" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+      <c r="B85" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+      <c r="B86" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+      <c r="B87" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
+      <c r="B88" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+      <c r="B89" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="B90" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="B91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="B92" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="B93" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="B94" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>230</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>15</v>
@@ -2776,7 +2908,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>15</v>
@@ -2784,15 +2916,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>15</v>
@@ -2800,23 +2932,23 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
+      <c r="B101" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="11" t="s">
-        <v>234</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>15</v>
@@ -2824,47 +2956,47 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
+      <c r="B104" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+      <c r="B105" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="11" t="s">
+      <c r="B106" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
+      <c r="B107" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
         <v>238</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>15</v>
@@ -2872,7 +3004,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>15</v>
@@ -2880,7 +3012,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>15</v>
@@ -2888,7 +3020,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>15</v>
@@ -2896,7 +3028,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>15</v>
@@ -2904,7 +3036,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>15</v>
@@ -2912,15 +3044,15 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>15</v>
@@ -2928,7 +3060,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>15</v>
@@ -2936,47 +3068,47 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="10" t="s">
+      <c r="B118" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+      <c r="B119" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="11" t="s">
+      <c r="B120" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="9" t="s">
+      <c r="B121" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
         <v>248</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>15</v>
@@ -2984,63 +3116,63 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="11" t="s">
+      <c r="B124" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+      <c r="B125" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B125" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="7" t="s">
+      <c r="B126" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+      <c r="B127" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="11" t="s">
+      <c r="B128" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="9" t="s">
+      <c r="B129" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="11" t="s">
-        <v>251</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>15</v>
@@ -3048,7 +3180,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>15</v>
@@ -3056,7 +3188,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>15</v>
@@ -3064,7 +3196,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
-        <v>176</v>
+        <v>253</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>15</v>
@@ -3072,7 +3204,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>254</v>
+        <v>176</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>15</v>
@@ -3080,68 +3212,68 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="9" t="s">
+      <c r="B136" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="11" t="s">
+      <c r="B137" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+      <c r="B138" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="11" t="s">
+      <c r="B139" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
+      <c r="B140" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="11" t="s">
         <v>259</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>15</v>
@@ -3149,526 +3281,538 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
+      <c r="B145" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="11" t="s">
+      <c r="B146" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="9" t="s">
+      <c r="B147" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="11" t="s">
+      <c r="B148" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H148" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="11" t="s">
+      <c r="B149" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
+      <c r="B150" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B150" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="11" t="s">
+      <c r="B151" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="B151" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
+      <c r="B152" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B152" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="11" t="s">
+      <c r="B153" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="11" t="s">
+      <c r="B154" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
+      <c r="B155" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B155" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
+      <c r="B156" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="11" t="s">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="B157" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
+      <c r="B158" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B158" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="9" t="s">
+      <c r="B159" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="9" t="s">
+      <c r="B160" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B160" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
+      <c r="B161" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="11" t="s">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
+      <c r="B163" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="11" t="s">
+      <c r="B164" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
+      <c r="B165" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B165" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
+      <c r="B166" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="10" t="s">
+      <c r="B167" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="B167" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="11" t="s">
+      <c r="B168" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="B168" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="11" t="s">
+      <c r="B169" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="B169" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
+      <c r="B170" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B170" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="11" t="s">
+      <c r="B171" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="B171" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="11" t="s">
+      <c r="B172" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="11" t="s">
+      <c r="B173" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
+      <c r="B174" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B174" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+      <c r="B175" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="11" t="s">
+      <c r="B176" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H176" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="9" t="s">
+      <c r="B177" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="9" t="s">
+      <c r="B178" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="B178" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
+      <c r="B179" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B179" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="11" t="s">
+      <c r="B180" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
+      <c r="B181" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
+      <c r="B182" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="10" t="s">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+      <c r="B184" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B184" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
+      <c r="B185" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="11" t="s">
+      <c r="B186" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="11" t="s">
+      <c r="B187" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
+      <c r="B188" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="9" t="s">
+      <c r="B189" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="11" t="s">
+      <c r="B190" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H190" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
+      <c r="B191" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="11" t="s">
+      <c r="B192" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="11" t="s">
+      <c r="B193" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="11" t="s">
+      <c r="B194" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A195" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="11" t="s">
+      <c r="B195" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A196" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="11" t="s">
+      <c r="B196" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A197" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="11" t="s">
+      <c r="B197" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A198" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="B197" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="9" t="s">
+      <c r="B198" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="11" t="s">
+      <c r="B199" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A200" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="B199" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="11" t="s">
+      <c r="B200" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A201" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="B200" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
+      <c r="B201" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
+      <c r="B202" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="11" t="s">
+      <c r="B203" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A204" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="B203" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
+      <c r="B204" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="11" t="s">
+      <c r="B205" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="11" t="s">
+      <c r="B206" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H206" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="B206" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
+      <c r="B207" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B207" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="11" t="s">
+      <c r="B208" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
+      <c r="B209" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>15</v>
@@ -3676,23 +3820,23 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="B211" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="9" t="s">
+      <c r="B212" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="9" t="s">
         <v>297</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="11" t="s">
-        <v>298</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>15</v>
@@ -3700,15 +3844,15 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="11" t="s">
         <v>299</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>15</v>
@@ -3716,7 +3860,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>15</v>
@@ -3724,23 +3868,23 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="9" t="s">
+      <c r="B218" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="11" t="s">
-        <v>301</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>15</v>
@@ -3748,15 +3892,15 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>15</v>
@@ -3764,15 +3908,15 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="11" t="s">
-        <v>303</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>15</v>
@@ -3780,137 +3924,140 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="B224" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="11" t="s">
+      <c r="B225" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A226" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="B225" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="11" t="s">
+      <c r="B226" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A227" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
+      <c r="B227" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B227" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="9" t="s">
+      <c r="B228" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B228" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
+      <c r="B229" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B229" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
+      <c r="B230" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="11" t="s">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="B231" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="11" t="s">
+      <c r="B232" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="B232" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="9" t="s">
+      <c r="B233" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="B233" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="9" t="s">
+      <c r="B234" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="B234" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
+      <c r="B235" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B235" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
+      <c r="B236" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="11" t="s">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="B237" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="11" t="s">
+      <c r="B238" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B238" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="11" t="s">
+      <c r="B239" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H239" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="B239" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="11" t="s">
+      <c r="B240" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="11" t="s">
         <v>313</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>15</v>
@@ -3918,20 +4065,20 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="11" t="s">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>15</v>
@@ -3939,79 +4086,79 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B245" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="11" t="s">
+      <c r="B246" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="B246" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="7" t="s">
+      <c r="B247" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B247" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="10" t="s">
+      <c r="B248" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="B248" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="2" t="s">
+      <c r="B249" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B249" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="11" t="s">
+      <c r="B250" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="B250" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="9" t="s">
+      <c r="B251" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="B251" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="11" t="s">
+      <c r="B252" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="B252" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
+      <c r="B253" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="11" t="s">
-        <v>319</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>15</v>
@@ -4019,15 +4166,15 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="11" t="s">
         <v>320</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>15</v>
@@ -4035,7 +4182,7 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>15</v>
@@ -4043,7 +4190,7 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>15</v>
@@ -4051,31 +4198,31 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B259" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A260" s="9" t="s">
+      <c r="B260" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A261" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B260" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A261" s="11" t="s">
+      <c r="B261" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A262" s="11" t="s">
         <v>322</v>
-      </c>
-      <c r="B261" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A262" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>15</v>
@@ -4083,7 +4230,7 @@
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>15</v>
@@ -4091,7 +4238,7 @@
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>15</v>
@@ -4099,23 +4246,23 @@
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B265" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A266" s="11" t="s">
+      <c r="B266" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A267" s="11" t="s">
         <v>323</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A267" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>15</v>
@@ -4123,56 +4270,56 @@
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B268" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J268" s="2" t="s">
+      <c r="B269" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J269" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K268" s="2" t="s">
+      <c r="K269" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L268" s="2" t="s">
+      <c r="L269" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A269" s="11" t="s">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A270" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="B269" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
+      <c r="B270" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B270" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A271" s="11" t="s">
+      <c r="B271" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A272" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="B271" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A272" s="9" t="s">
+      <c r="B272" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="9" t="s">
         <v>326</v>
-      </c>
-      <c r="B272" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>15</v>
@@ -4180,15 +4327,15 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B274" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="11" t="s">
-        <v>327</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>15</v>
@@ -4196,7 +4343,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>15</v>
@@ -4204,41 +4351,41 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B277" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2" t="s">
-        <v>112</v>
+      <c r="B278" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="9" t="s">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="B280" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="11" t="s">
+      <c r="B281" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="11" t="s">
         <v>331</v>
-      </c>
-      <c r="B281" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>15</v>
@@ -4246,15 +4393,15 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B283" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="11" t="s">
-        <v>332</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>15</v>
@@ -4262,31 +4409,31 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="B285" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="2" t="s">
+      <c r="B286" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B286" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="9" t="s">
+      <c r="B287" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="9" t="s">
         <v>334</v>
-      </c>
-      <c r="B287" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>15</v>
@@ -4294,15 +4441,15 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B289" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="11" t="s">
-        <v>335</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>15</v>
@@ -4310,7 +4457,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>15</v>
@@ -4318,31 +4465,31 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="B292" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="10" t="s">
+      <c r="B293" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="B293" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="11" t="s">
+      <c r="B294" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="11" t="s">
         <v>339</v>
-      </c>
-      <c r="B294" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>15</v>
@@ -4350,7 +4497,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>15</v>
@@ -4358,15 +4505,15 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B297" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="11" t="s">
-        <v>340</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>15</v>
@@ -4374,7 +4521,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>15</v>
@@ -4382,7 +4529,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>15</v>
@@ -4390,7 +4537,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>15</v>
@@ -4398,7 +4545,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>15</v>
@@ -4406,139 +4553,142 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="B303" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="9" t="s">
+      <c r="B304" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A305" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="B304" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" s="2" t="s">
+      <c r="B305" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" s="2" t="s">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A307" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B306" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" s="2" t="s">
+      <c r="B307" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A308" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B307" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" s="9" t="s">
+      <c r="B308" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A309" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="B308" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" s="9" t="s">
+      <c r="B309" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A310" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="B309" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" s="11" t="s">
+      <c r="B310" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A311" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="B310" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="2" t="s">
+      <c r="B311" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A312" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B311" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" s="2" t="s">
+      <c r="B312" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A313" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B312" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" s="2" t="s">
+      <c r="B313" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A314" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B313" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" s="2" t="s">
+      <c r="B314" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A315" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" s="11" t="s">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A316" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B315" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" s="2" t="s">
+      <c r="B316" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A317" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B316" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" s="11" t="s">
+      <c r="B317" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A318" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B317" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" s="2" t="s">
+      <c r="B318" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H318" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A319" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" s="2" t="s">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A320" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" s="2" t="s">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B320" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" s="11" t="s">
-        <v>350</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>15</v>
@@ -4546,7 +4696,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>15</v>
@@ -4554,7 +4704,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>15</v>
@@ -4562,23 +4712,23 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="B324" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="2" t="s">
+      <c r="B325" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B325" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="11" t="s">
-        <v>354</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>15</v>
@@ -4586,7 +4736,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>15</v>
@@ -4594,52 +4744,52 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="B328" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="2" t="s">
+      <c r="B329" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B329" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" s="11" t="s">
+      <c r="B330" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="B330" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="9" t="s">
+      <c r="B331" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B331" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="2" t="s">
+      <c r="B332" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="12" t="s">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="12" t="s">
         <v>359</v>
-      </c>
-      <c r="B333" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="11" t="s">
-        <v>360</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>15</v>
@@ -4647,7 +4797,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>15</v>
@@ -4655,7 +4805,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>15</v>
@@ -4663,7 +4813,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>15</v>
@@ -4671,14 +4821,19 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="B338" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D340" s="8"/>
+      <c r="B339" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D341" s="8"/>
@@ -4731,36 +4886,43 @@
     <row r="357" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D357" s="8"/>
     </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D358" s="8"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L357">
-    <sortCondition ref="H2:H357"/>
+  <autoFilter ref="A1:A361" xr:uid="{BADA2078-8350-4D40-AA7E-30CA3E8A707E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M71:M80">
+    <sortCondition ref="M71:M80"/>
   </sortState>
-  <conditionalFormatting sqref="A141:A338">
+  <conditionalFormatting sqref="A142:A339">
+    <cfRule type="duplicateValues" dxfId="19" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A142:A339">
     <cfRule type="duplicateValues" dxfId="18" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A141:A338">
+  <conditionalFormatting sqref="D341:D343">
     <cfRule type="duplicateValues" dxfId="17" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D340:D342">
+  <conditionalFormatting sqref="D344">
     <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D343">
+  <conditionalFormatting sqref="D345:D347">
     <cfRule type="duplicateValues" dxfId="15" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D344:D346">
+  <conditionalFormatting sqref="D346:D347">
     <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D345:D346">
+  <conditionalFormatting sqref="D346:D347">
     <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D345:D346">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+  <conditionalFormatting sqref="D348:D358">
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D347:D357">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+  <conditionalFormatting sqref="D348:D358">
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D347:D357">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding CAT CBRE CDW CELG CFG CHE CHRW
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DFD926-17A0-41BE-BB4B-5CBA581ABA40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC940667-FF92-4208-AA98-A28987AF942C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="377">
   <si>
     <t>SCVL</t>
   </si>
@@ -1158,6 +1158,9 @@
   </si>
   <si>
     <t>Chaff</t>
+  </si>
+  <si>
+    <t>Not found</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1214,6 +1217,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1230,7 +1239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1254,101 +1263,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1829,8 +1749,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H319" sqref="H319"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2648,7 +2568,9 @@
       <c r="B66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H66" s="3"/>
+      <c r="H66" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
@@ -2657,7 +2579,9 @@
       <c r="B67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H67" s="3"/>
+      <c r="H67" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -2666,7 +2590,9 @@
       <c r="B68" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H68" s="3"/>
+      <c r="H68" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
@@ -2675,7 +2601,9 @@
       <c r="B69" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
@@ -2684,16 +2612,23 @@
       <c r="B70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H70" s="3"/>
+      <c r="H70" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="17" t="s">
         <v>219</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H71" s="3"/>
+      <c r="H71" s="3">
+        <v>43703</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
@@ -2702,7 +2637,9 @@
       <c r="B72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H72" s="3"/>
+      <c r="H72" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
@@ -2711,7 +2648,9 @@
       <c r="B73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H73" s="3"/>
+      <c r="H73" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
@@ -2720,13 +2659,17 @@
       <c r="B74" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H74" s="3"/>
+      <c r="H74" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H75" s="3"/>
+      <c r="H75" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
@@ -2735,7 +2678,9 @@
       <c r="B76" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H76" s="3"/>
+      <c r="H76" s="3">
+        <v>43703</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">

</xml_diff>

<commit_message>
Adding CP CPRT CRM CRS CRVL CSCO CSFL
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5C0AB4-CD0D-4ACB-B1C4-E0DBA4DFFD23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -18,18 +19,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="380">
   <si>
     <t>SCVL</t>
   </si>
@@ -1163,12 +1158,18 @@
   </si>
   <si>
     <t>Problem with the diamonds not matching with pink dots…Oct quarter….Need to figure out what is wroing</t>
+  </si>
+  <si>
+    <t>Problem with the diamonds not matching with pink dots…Dec quarter….Need to figure out what is wroing</t>
+  </si>
+  <si>
+    <t>Problem with the diamonds not matching with pink dots…Jan quarter….Need to figure out what is wroing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1209,7 +1210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1228,6 +1229,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1241,7 +1248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1266,7 +1273,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1747,13 +1755,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I83" sqref="I83"/>
+      <selection pane="bottomLeft" activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2686,7 +2694,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="18" t="s">
         <v>222</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -2697,7 +2705,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="19" t="s">
         <v>87</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -2708,7 +2716,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="18" t="s">
         <v>172</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -2719,7 +2727,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="18" t="s">
         <v>223</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -2732,8 +2740,8 @@
         <v>377</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
         <v>224</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -2743,8 +2751,8 @@
         <v>43705</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
         <v>173</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -2754,7 +2762,7 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>374</v>
       </c>
@@ -2765,63 +2773,90 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="3">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>225</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="3">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>226</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="3">
+        <v>43706</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>227</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="3">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>228</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="3">
+        <v>43706</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>229</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="3">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="3">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>88</v>
       </c>
@@ -2832,7 +2867,7 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>134</v>
       </c>
@@ -2840,7 +2875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>133</v>
       </c>
@@ -2848,7 +2883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>61</v>
       </c>
@@ -2856,12 +2891,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>32</v>
       </c>
@@ -4853,8 +4888,8 @@
       <c r="D358" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A361"/>
-  <sortState ref="M71:M80">
+  <autoFilter ref="A1:A361" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M71:M80">
     <sortCondition ref="M71:M80"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
@@ -4893,7 +4928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
@@ -7567,7 +7602,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A331">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A331">
     <sortCondition ref="A1:A331"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Adding CSX CTAS CTXS CVTI
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5C0AB4-CD0D-4ACB-B1C4-E0DBA4DFFD23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A662EE17-3824-4E4F-8A55-BD73D794075E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="382">
   <si>
     <t>SCVL</t>
   </si>
@@ -1164,6 +1164,12 @@
   </si>
   <si>
     <t>Problem with the diamonds not matching with pink dots…Jan quarter….Need to figure out what is wroing</t>
+  </si>
+  <si>
+    <t>Projections have come down significantly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have a purchase offer by some compnay </t>
   </si>
 </sst>
 </file>
@@ -1760,8 +1766,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L87" sqref="L87"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1822,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="3">
-        <v>43672</v>
+        <v>43712</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2874,6 +2883,9 @@
       <c r="B92" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H92" s="3">
+        <v>43713</v>
+      </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
@@ -2882,6 +2894,9 @@
       <c r="B93" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H93" s="3">
+        <v>43713</v>
+      </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
@@ -2890,11 +2905,17 @@
       <c r="B94" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H94" s="3">
+        <v>43713</v>
+      </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="H95" s="3">
+        <v>43713</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
@@ -2902,6 +2923,9 @@
       </c>
       <c r="B96" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding DAL DBX DECK  DFS DG DHI DIS DNKN DPZ
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DADC7AA-3512-4EAC-A864-6CD7682BA760}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E64394C-CF57-46C8-8C4F-7C47950DB104}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="381">
   <si>
     <t>SCVL</t>
   </si>
@@ -1164,6 +1164,9 @@
   </si>
   <si>
     <t>Projections have come down</t>
+  </si>
+  <si>
+    <t>Projections have gone up</t>
   </si>
 </sst>
 </file>
@@ -1760,8 +1763,8 @@
   <dimension ref="A1:J358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2924,87 +2927,121 @@
         <v>377</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>226</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F97" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>227</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F98" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>228</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F100" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F101" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>229</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F102" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>230</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F103" s="3">
+        <v>43714</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>231</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F104" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>232</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F105" s="3">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F106" s="3">
+        <v>43714</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>233</v>
       </c>
@@ -3012,7 +3049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>234</v>
       </c>
@@ -3020,7 +3057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>235</v>
       </c>
@@ -3028,7 +3065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>236</v>
       </c>
@@ -3036,7 +3073,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>237</v>
       </c>
@@ -3044,7 +3081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>238</v>
       </c>

</xml_diff>

<commit_message>
Adding support for Parsing Master Tracklist
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E64394C-CF57-46C8-8C4F-7C47950DB104}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756F46F1-3F4A-49F6-BC0F-5221F67BF855}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="382">
   <si>
     <t>SCVL</t>
   </si>
@@ -1167,6 +1167,9 @@
   </si>
   <si>
     <t>Projections have gone up</t>
+  </si>
+  <si>
+    <t>Last_Earnings_Date</t>
   </si>
 </sst>
 </file>
@@ -1760,25 +1763,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J358"/>
+  <dimension ref="A1:K358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17" style="2" customWidth="1"/>
-    <col min="9" max="9" width="98.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="139.85546875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="15.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17" style="2" customWidth="1"/>
+    <col min="10" max="10" width="98.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="139.85546875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1795,287 +1798,291 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>43712</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="J2" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>43712</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>43712</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>43712</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>43674</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>43674</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>43676</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>43678</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>43684</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>43684</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>43686</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>43686</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>43686</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>43686</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>155</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>43686</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>43686</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>43686</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>43686</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>160</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>43686</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>161</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>43686</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>185</v>
       </c>
@@ -2083,965 +2090,965 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>43689</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>163</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="3">
+      <c r="G24" s="3">
         <v>43689</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="3">
+      <c r="G25" s="3">
         <v>43689</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="3">
+      <c r="G26" s="3">
         <v>43689</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>186</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="3">
+      <c r="G27" s="3">
         <v>43689</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>187</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="3">
+      <c r="G28" s="3">
         <v>43690</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>188</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="3">
+      <c r="G29" s="3">
         <v>43690</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>189</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="3">
+      <c r="G30" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>164</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="3">
+      <c r="G31" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>190</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="3">
+      <c r="G32" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="3">
+      <c r="G33" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>191</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="3">
+      <c r="G34" s="3">
         <v>43690</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>192</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="3">
+      <c r="G35" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>193</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="3">
+      <c r="G36" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>194</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="3">
+      <c r="G37" s="3">
         <v>43690</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>195</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="3">
+      <c r="G38" s="3">
         <v>43691</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>196</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="3">
+      <c r="G39" s="3">
         <v>43691</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>197</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="3">
+      <c r="G40" s="3">
         <v>43691</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>198</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="3">
+      <c r="G41" s="3">
         <v>43691</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="3">
+      <c r="G42" s="3">
         <v>43691</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>199</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="3">
+      <c r="G43" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="3">
+      <c r="G44" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="3">
+      <c r="G45" s="3">
         <v>43693</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>200</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="3">
+      <c r="G46" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>201</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F47" s="3">
+      <c r="G47" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>202</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="3">
+      <c r="G48" s="3">
         <v>43693</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="3">
+      <c r="G49" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>165</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="3">
+      <c r="G50" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="3">
+      <c r="G51" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>204</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="3">
+      <c r="G52" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>205</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="3">
+      <c r="G53" s="3">
         <v>43693</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="3">
+      <c r="G54" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>166</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="3">
+      <c r="G55" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="3">
+      <c r="G56" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>206</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="3">
+      <c r="G57" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="3">
+      <c r="G58" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>207</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="3">
+      <c r="G59" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="3">
+      <c r="G60" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>208</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="3">
+      <c r="G61" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="3">
+      <c r="G62" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>209</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F63" s="3">
+      <c r="G63" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F64" s="3">
+      <c r="G64" s="3">
         <v>43694</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>210</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="3">
+      <c r="G65" s="3">
         <v>43694</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>211</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="3">
+      <c r="G66" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>212</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="3">
+      <c r="G67" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>213</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="3">
+      <c r="G68" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F69" s="3">
+      <c r="G69" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>214</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F70" s="3">
+      <c r="G70" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>215</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="3">
+      <c r="G71" s="3">
         <v>43703</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>216</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="3">
+      <c r="G72" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>167</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F73" s="3">
+      <c r="G73" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>101</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F74" s="3">
+      <c r="G74" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F75" s="3">
+      <c r="G75" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>217</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F76" s="3">
+      <c r="G76" s="3">
         <v>43703</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>218</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F77" s="3">
+      <c r="G77" s="3">
         <v>43705</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>85</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="3">
+      <c r="G78" s="3">
         <v>43705</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>168</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F79" s="3">
+      <c r="G79" s="3">
         <v>43705</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>219</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F80" s="3">
+      <c r="G80" s="3">
         <v>43705</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="J80" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
         <v>220</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F81" s="3">
+      <c r="G81" s="3">
         <v>43705</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F82" s="3">
+      <c r="G82" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>370</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="F83" s="3">
+      <c r="G83" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F84" s="3">
+      <c r="G84" s="3">
         <v>43706</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F85" s="3">
+      <c r="G85" s="3">
         <v>43706</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F86" s="3">
+      <c r="G86" s="3">
         <v>43706</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="J86" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>223</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F87" s="3">
+      <c r="G87" s="3">
         <v>43706</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>224</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F88" s="3">
+      <c r="G88" s="3">
         <v>43706</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="J88" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>225</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F89" s="3">
+      <c r="G89" s="3">
         <v>43706</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F90" s="3">
+      <c r="G90" s="3">
         <v>43706</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F91" s="3">
+      <c r="G91" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F92" s="3">
+      <c r="G92" s="3">
         <v>43713</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F93" s="3">
+      <c r="G93" s="3">
         <v>43713</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F94" s="3">
+      <c r="G94" s="3">
         <v>43713</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F95" s="3">
+      <c r="G95" s="3">
         <v>43713</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I96" s="2" t="s">
+      <c r="J96" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>226</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F97" s="3">
+      <c r="G97" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>227</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F98" s="3">
+      <c r="G98" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>228</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F100" s="3">
+      <c r="G100" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F101" s="3">
+      <c r="G101" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>229</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F102" s="3">
+      <c r="G102" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>230</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F103" s="3">
+      <c r="G103" s="3">
         <v>43714</v>
       </c>
-      <c r="I103" s="2" t="s">
+      <c r="J103" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>231</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="3">
+      <c r="G104" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>232</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F105" s="3">
+      <c r="G105" s="3">
         <v>43714</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F106" s="3">
+      <c r="G106" s="3">
         <v>43714</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="J106" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>233</v>
       </c>
@@ -3049,7 +3056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>234</v>
       </c>
@@ -3057,7 +3064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>235</v>
       </c>
@@ -3065,7 +3072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>236</v>
       </c>
@@ -3073,7 +3080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>237</v>
       </c>
@@ -3081,7 +3088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>238</v>
       </c>
@@ -3342,7 +3349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>65</v>
       </c>
@@ -3350,7 +3357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>40</v>
       </c>
@@ -3358,7 +3365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
         <v>256</v>
       </c>
@@ -3366,18 +3373,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
         <v>174</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F148" s="3">
+      <c r="G148" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
         <v>257</v>
       </c>
@@ -3385,7 +3392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
         <v>258</v>
       </c>
@@ -3393,7 +3400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>115</v>
       </c>
@@ -3401,7 +3408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
         <v>259</v>
       </c>
@@ -3409,7 +3416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>98</v>
       </c>
@@ -3417,7 +3424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>260</v>
       </c>
@@ -3425,7 +3432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
         <v>261</v>
       </c>
@@ -3433,7 +3440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>130</v>
       </c>
@@ -3441,12 +3448,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
         <v>262</v>
       </c>
@@ -3454,7 +3461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>25</v>
       </c>
@@ -3462,7 +3469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="9" t="s">
         <v>263</v>
       </c>
@@ -3470,7 +3477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="9" t="s">
         <v>264</v>
       </c>
@@ -3478,12 +3485,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
         <v>265</v>
       </c>
@@ -3491,7 +3498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>56</v>
       </c>
@@ -3499,7 +3506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="11" t="s">
         <v>266</v>
       </c>
@@ -3507,7 +3514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>84</v>
       </c>
@@ -3515,7 +3522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>107</v>
       </c>
@@ -3523,7 +3530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="10" t="s">
         <v>267</v>
       </c>
@@ -3531,7 +3538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
         <v>268</v>
       </c>
@@ -3539,7 +3546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>269</v>
       </c>
@@ -3547,7 +3554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>136</v>
       </c>
@@ -3555,7 +3562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>270</v>
       </c>
@@ -3563,7 +3570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
         <v>271</v>
       </c>
@@ -3571,7 +3578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>272</v>
       </c>
@@ -3579,7 +3586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>91</v>
       </c>
@@ -3587,18 +3594,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F176" s="3">
+      <c r="G176" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
         <v>273</v>
       </c>
@@ -3606,7 +3613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="9" t="s">
         <v>175</v>
       </c>
@@ -3614,7 +3621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="9" t="s">
         <v>274</v>
       </c>
@@ -3622,7 +3629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>39</v>
       </c>
@@ -3630,7 +3637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
         <v>275</v>
       </c>
@@ -3638,7 +3645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>87</v>
       </c>
@@ -3646,12 +3653,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
         <v>276</v>
       </c>
@@ -3659,7 +3666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>33</v>
       </c>
@@ -3667,7 +3674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>55</v>
       </c>
@@ -3675,7 +3682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="11" t="s">
         <v>277</v>
       </c>
@@ -3683,7 +3690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
         <v>278</v>
       </c>
@@ -3691,7 +3698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>47</v>
       </c>
@@ -3699,18 +3706,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="9" t="s">
         <v>176</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F190" s="3">
+      <c r="G190" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="11" t="s">
         <v>279</v>
       </c>
@@ -3718,7 +3725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>38</v>
       </c>
@@ -3726,7 +3733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
         <v>280</v>
       </c>
@@ -3734,7 +3741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
         <v>281</v>
       </c>
@@ -3742,7 +3749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="11" t="s">
         <v>282</v>
       </c>
@@ -3750,7 +3757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
         <v>283</v>
       </c>
@@ -3758,7 +3765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
         <v>284</v>
       </c>
@@ -3766,7 +3773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="11" t="s">
         <v>285</v>
       </c>
@@ -3774,7 +3781,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="9" t="s">
         <v>286</v>
       </c>
@@ -3782,7 +3789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
         <v>287</v>
       </c>
@@ -3790,7 +3797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="11" t="s">
         <v>288</v>
       </c>
@@ -3798,7 +3805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>118</v>
       </c>
@@ -3806,7 +3813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>54</v>
       </c>
@@ -3814,7 +3821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>289</v>
       </c>
@@ -3822,7 +3829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>106</v>
       </c>
@@ -3830,18 +3837,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="11" t="s">
         <v>177</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F206" s="3">
+      <c r="G206" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="11" t="s">
         <v>290</v>
       </c>
@@ -3849,7 +3856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>114</v>
       </c>
@@ -3985,7 +3992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="11" t="s">
         <v>300</v>
       </c>
@@ -3993,7 +4000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="11" t="s">
         <v>301</v>
       </c>
@@ -4001,7 +4008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="11" t="s">
         <v>302</v>
       </c>
@@ -4009,7 +4016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>53</v>
       </c>
@@ -4017,7 +4024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="9" t="s">
         <v>179</v>
       </c>
@@ -4025,7 +4032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>88</v>
       </c>
@@ -4033,12 +4040,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="11" t="s">
         <v>303</v>
       </c>
@@ -4046,7 +4053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="11" t="s">
         <v>304</v>
       </c>
@@ -4054,7 +4061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="9" t="s">
         <v>305</v>
       </c>
@@ -4062,7 +4069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="9" t="s">
         <v>306</v>
       </c>
@@ -4070,7 +4077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>89</v>
       </c>
@@ -4078,12 +4085,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="11" t="s">
         <v>307</v>
       </c>
@@ -4091,18 +4098,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="11" t="s">
         <v>180</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F239" s="3">
+      <c r="G239" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
         <v>308</v>
       </c>
@@ -4235,7 +4242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>50</v>
       </c>
@@ -4243,7 +4250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>21</v>
       </c>
@@ -4251,7 +4258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>43</v>
       </c>
@@ -4259,7 +4266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>37</v>
       </c>
@@ -4267,7 +4274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="9" t="s">
         <v>317</v>
       </c>
@@ -4275,7 +4282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="11" t="s">
         <v>318</v>
       </c>
@@ -4283,7 +4290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>36</v>
       </c>
@@ -4291,7 +4298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>49</v>
       </c>
@@ -4299,7 +4306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>108</v>
       </c>
@@ -4307,7 +4314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>26</v>
       </c>
@@ -4315,7 +4322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="11" t="s">
         <v>319</v>
       </c>
@@ -4323,7 +4330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>129</v>
       </c>
@@ -4331,21 +4338,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H269" s="2" t="s">
+      <c r="I269" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I269" s="2" t="s">
+      <c r="J269" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="11" t="s">
         <v>320</v>
       </c>
@@ -4353,7 +4360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>27</v>
       </c>
@@ -4361,7 +4368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="11" t="s">
         <v>321</v>
       </c>
@@ -4619,7 +4626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="9" t="s">
         <v>342</v>
       </c>
@@ -4627,12 +4634,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>127</v>
       </c>
@@ -4640,7 +4647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>128</v>
       </c>
@@ -4648,7 +4655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="9" t="s">
         <v>343</v>
       </c>
@@ -4656,7 +4663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="9" t="s">
         <v>344</v>
       </c>
@@ -4664,7 +4671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="11" t="s">
         <v>345</v>
       </c>
@@ -4672,7 +4679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>119</v>
       </c>
@@ -4680,7 +4687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>111</v>
       </c>
@@ -4688,7 +4695,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>123</v>
       </c>
@@ -4696,12 +4703,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A316" s="11" t="s">
         <v>183</v>
       </c>
@@ -4709,7 +4716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>82</v>
       </c>
@@ -4717,23 +4724,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A318" s="11" t="s">
         <v>184</v>
       </c>
       <c r="B318" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F318" s="3">
+      <c r="G318" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>45</v>
       </c>
@@ -4943,8 +4950,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A361" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J71:J80">
-    <sortCondition ref="J71:J80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K71:K80">
+    <sortCondition ref="K71:K80"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
     <cfRule type="duplicateValues" dxfId="19" priority="10"/>

</xml_diff>

<commit_message>
Updating FIX and PGR earnings
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756F46F1-3F4A-49F6-BC0F-5221F67BF855}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E1D705-8CB3-49B3-B1C0-E3BA92E3DF92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="383">
   <si>
     <t>SCVL</t>
   </si>
@@ -1170,6 +1170,9 @@
   </si>
   <si>
     <t>Last_Earnings_Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This keeps on going up now </t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1770,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1884,9 +1887,12 @@
         <v>13</v>
       </c>
       <c r="G6" s="3">
-        <v>43674</v>
+        <v>43714</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1898,7 +1904,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="3">
-        <v>43674</v>
+        <v>43714</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>139</v>
@@ -1912,9 +1918,12 @@
         <v>13</v>
       </c>
       <c r="G8" s="3">
-        <v>43676</v>
+        <v>43714</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating AAN AAPL ABCB ABG ABMD IIPR JAZZ MNST NCLH REGN
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="387">
   <si>
     <t>SCVL</t>
   </si>
@@ -1096,9 +1096,6 @@
     <t>ZUMZ</t>
   </si>
   <si>
-    <t>Overprices right now. Needs channel adjustment</t>
-  </si>
-  <si>
     <t xml:space="preserve">See the huge drop - Asking Ann about it </t>
   </si>
   <si>
@@ -1165,13 +1162,28 @@
     <t>Looks attracitve - Maybe tell Ann about it</t>
   </si>
   <si>
-    <t>The projections seem to have gone up</t>
-  </si>
-  <si>
     <t>The projections seem to have gone up - Why does the price not move up?</t>
   </si>
   <si>
     <t>Another one where the price does not move up?</t>
+  </si>
+  <si>
+    <t>Looks very interesting - Maybe ask Ann</t>
+  </si>
+  <si>
+    <t>The projections seem to have gone up. Ann has it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good chart - Just look </t>
+  </si>
+  <si>
+    <t>One of those stocks that remain flat while the earnings keep trending up…never catches the price channel</t>
+  </si>
+  <si>
+    <t>One of those stocks that have difficult patterrn to figure out when we could have bought</t>
+  </si>
+  <si>
+    <t>More price drop</t>
   </si>
 </sst>
 </file>
@@ -1769,7 +1781,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1791,7 +1803,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1803,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
@@ -1827,7 +1839,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1841,7 +1853,7 @@
         <v>43712</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>135</v>
@@ -1858,7 +1870,7 @@
         <v>43712</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1872,7 +1884,7 @@
         <v>43712</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1886,7 +1898,7 @@
         <v>43714</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>138</v>
@@ -1917,7 +1929,7 @@
         <v>43714</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>141</v>
@@ -1934,7 +1946,7 @@
         <v>43714</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1951,7 +1963,7 @@
         <v>43715</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>143</v>
@@ -1971,7 +1983,7 @@
         <v>43715</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>145</v>
@@ -1991,7 +2003,7 @@
         <v>43715</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2039,7 +2051,7 @@
         <v>43715</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2056,68 +2068,95 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C17" s="3">
+        <v>43684</v>
+      </c>
       <c r="D17" s="3">
-        <v>43686</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C18" s="3">
+        <v>43683</v>
+      </c>
       <c r="D18" s="3">
-        <v>43686</v>
+        <v>43715</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C19" s="3">
+        <v>43684</v>
+      </c>
       <c r="D19" s="3">
-        <v>43686</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C20" s="3">
+        <v>43685</v>
+      </c>
       <c r="D20" s="3">
-        <v>43686</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C21" s="3">
+        <v>43683</v>
+      </c>
       <c r="D21" s="3">
-        <v>43686</v>
+        <v>43715</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>181</v>
       </c>
@@ -2125,68 +2164,86 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C23" s="3">
+        <v>43671</v>
+      </c>
       <c r="D23" s="3">
-        <v>43689</v>
+        <v>43715</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>159</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C24" s="3">
+        <v>43676</v>
+      </c>
       <c r="D24" s="3">
-        <v>43689</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C25" s="3">
+        <v>43672</v>
+      </c>
       <c r="D25" s="3">
-        <v>43689</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C26" s="3">
+        <v>43672</v>
+      </c>
       <c r="D26" s="3">
-        <v>43689</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>182</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C27" s="3">
+        <v>43678</v>
+      </c>
       <c r="D27" s="3">
-        <v>43689</v>
+        <v>43715</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>183</v>
       </c>
@@ -2197,10 +2254,10 @@
         <v>43690</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>184</v>
       </c>
@@ -2211,10 +2268,10 @@
         <v>43690</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>185</v>
       </c>
@@ -2225,7 +2282,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>160</v>
       </c>
@@ -2236,7 +2293,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>186</v>
       </c>
@@ -2269,7 +2326,7 @@
         <v>43690</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,7 +2395,7 @@
         <v>43691</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2396,7 +2453,7 @@
         <v>43693</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2432,7 +2489,7 @@
         <v>43693</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2619,7 +2676,7 @@
         <v>43694</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2688,7 +2745,7 @@
         <v>43703</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2787,7 +2844,7 @@
         <v>43705</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2814,10 +2871,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="D83" s="3">
         <v>43698</v>
@@ -2856,7 +2913,7 @@
         <v>43706</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2881,7 +2938,7 @@
         <v>43706</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2966,7 +3023,7 @@
         <v>11</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2996,7 +3053,7 @@
         <v>224</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D99" s="3"/>
     </row>
@@ -3044,7 +3101,7 @@
         <v>43714</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3137,7 @@
         <v>43714</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding DRI DXPE EBF ECOL EPAY EPD EQIX ET ETFC EVR EW EXPD
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8812935-D97F-4EDE-8ECB-21925155DB43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="9195" yWindow="180" windowWidth="15900" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="392">
   <si>
     <t>SCVL</t>
   </si>
@@ -1184,12 +1185,27 @@
   </si>
   <si>
     <t>More price drop</t>
+  </si>
+  <si>
+    <t>Could not loacte in the emails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov fiscal - Has chart problems. </t>
+  </si>
+  <si>
+    <t>Keep an eye out - Earning are growing but the price ahs been cut alomost in half</t>
+  </si>
+  <si>
+    <t>Interseting chart - Earnings growing but price does not follow - Energy Compnay</t>
+  </si>
+  <si>
+    <t>Ann has it but the price has not moved - not sure why?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1775,13 +1791,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3147,6 +3163,12 @@
       <c r="B107" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C107" s="3">
+        <v>43636</v>
+      </c>
+      <c r="D107" s="3">
+        <v>43716</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
@@ -3155,6 +3177,12 @@
       <c r="B108" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C108" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D108" s="3">
+        <v>43716</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
@@ -3163,6 +3191,15 @@
       <c r="B109" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C109" s="3">
+        <v>43642</v>
+      </c>
+      <c r="D109" s="3">
+        <v>43716</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
@@ -3171,6 +3208,12 @@
       <c r="B110" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C110" s="3">
+        <v>43678</v>
+      </c>
+      <c r="D110" s="3">
+        <v>43716</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
@@ -3179,6 +3222,9 @@
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F111" s="2" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
@@ -3187,64 +3233,121 @@
       <c r="B112" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D112" s="3">
+        <v>43716</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>235</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D113" s="3">
+        <v>43716</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D114" s="3">
+        <v>43716</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>237</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115" s="3">
+        <v>43684</v>
+      </c>
+      <c r="D115" s="3">
+        <v>43716</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116" s="3">
+        <v>43664</v>
+      </c>
+      <c r="D116" s="3">
+        <v>43716</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117" s="3">
+        <v>43670</v>
+      </c>
+      <c r="D117" s="3">
+        <v>43716</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118" s="3">
+        <v>43659</v>
+      </c>
+      <c r="D118" s="3">
+        <v>43716</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>238</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D119" s="3">
+        <v>43716</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>39</v>
       </c>
@@ -3252,7 +3355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>239</v>
       </c>
@@ -3260,7 +3363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
         <v>240</v>
       </c>
@@ -3268,7 +3371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>55</v>
       </c>
@@ -3276,7 +3379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>64</v>
       </c>
@@ -3284,7 +3387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>166</v>
       </c>
@@ -3292,7 +3395,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>60</v>
       </c>
@@ -3300,7 +3403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>167</v>
       </c>
@@ -3308,7 +3411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>21</v>
       </c>
@@ -5038,8 +5141,8 @@
       <c r="H358" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A361"/>
-  <sortState ref="G71:G80">
+  <autoFilter ref="A1:A361" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G71:G80">
     <sortCondition ref="G71:G80"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
@@ -5078,7 +5181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
@@ -7752,7 +7855,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A331">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A331">
     <sortCondition ref="A1:A331"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Adding FAF FANG FB FCFS FDX FFIV FISV
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8812935-D97F-4EDE-8ECB-21925155DB43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA376195-3FBF-40FB-B07A-74F161AC814D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9195" yWindow="180" windowWidth="15900" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="394">
   <si>
     <t>SCVL</t>
   </si>
@@ -1200,6 +1200,12 @@
   </si>
   <si>
     <t>Ann has it but the price has not moved - not sure why?</t>
+  </si>
+  <si>
+    <t>Ann has it - The projections have come down - maybe buy later</t>
+  </si>
+  <si>
+    <t>Great Earnings growth - but too expensive right now</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1321,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1793,11 +1809,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J358"/>
+  <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3042,7 +3058,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>222</v>
       </c>
@@ -3053,7 +3069,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>223</v>
       </c>
@@ -3064,7 +3080,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>224</v>
       </c>
@@ -3073,7 +3089,7 @@
       </c>
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>22</v>
       </c>
@@ -3084,7 +3100,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>75</v>
       </c>
@@ -3095,7 +3111,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>225</v>
       </c>
@@ -3106,7 +3122,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>226</v>
       </c>
@@ -3120,7 +3136,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>227</v>
       </c>
@@ -3131,7 +3147,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>228</v>
       </c>
@@ -3142,7 +3158,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>133</v>
       </c>
@@ -3155,8 +3171,9 @@
       <c r="F106" s="2" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L106" s="11"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>229</v>
       </c>
@@ -3169,8 +3186,9 @@
       <c r="D107" s="3">
         <v>43716</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L107" s="9"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>230</v>
       </c>
@@ -3184,7 +3202,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>231</v>
       </c>
@@ -3201,7 +3219,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>232</v>
       </c>
@@ -3214,8 +3232,9 @@
       <c r="D110" s="3">
         <v>43716</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L110" s="11"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>233</v>
       </c>
@@ -3226,7 +3245,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>234</v>
       </c>
@@ -3242,8 +3261,9 @@
       <c r="F112" s="2" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L112" s="7"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>235</v>
       </c>
@@ -3257,7 +3277,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>236</v>
       </c>
@@ -3270,8 +3290,9 @@
       <c r="D114" s="3">
         <v>43716</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L114" s="11"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>237</v>
       </c>
@@ -3287,8 +3308,9 @@
       <c r="F115" s="2" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L115" s="9"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>103</v>
       </c>
@@ -3301,8 +3323,9 @@
       <c r="D116" s="3">
         <v>43716</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L116" s="11"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>73</v>
       </c>
@@ -3318,8 +3341,9 @@
       <c r="F117" s="2" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L117" s="11"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>76</v>
       </c>
@@ -3332,8 +3356,9 @@
       <c r="D118" s="3">
         <v>43716</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L118" s="11"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>238</v>
       </c>
@@ -3346,24 +3371,37 @@
       <c r="D119" s="3">
         <v>43716</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L119" s="11"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C120" s="3">
+        <v>43671</v>
+      </c>
+      <c r="D120" s="3">
+        <v>43717</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>239</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C121" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D121" s="3">
+        <v>43717</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
         <v>240</v>
       </c>
@@ -3371,39 +3409,66 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C123" s="3">
+        <v>43670</v>
+      </c>
+      <c r="D123" s="3">
+        <v>43717</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C124" s="3">
+        <v>43670</v>
+      </c>
+      <c r="D124" s="3">
+        <v>43717</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>166</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C125" s="3">
+        <v>43641</v>
+      </c>
+      <c r="D125" s="3">
+        <v>43717</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C126" s="3">
+        <v>43670</v>
+      </c>
+      <c r="D126" s="3">
+        <v>43717</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>167</v>
       </c>
@@ -3411,39 +3476,57 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128" s="3">
+        <v>43670</v>
+      </c>
+      <c r="D128" s="3">
+        <v>43717</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>241</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129" s="3">
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>242</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130" s="3">
+        <v>43700</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>243</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131" s="3">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>244</v>
       </c>
@@ -3451,23 +3534,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
         <v>245</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133" s="3">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>168</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134" s="3">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>246</v>
       </c>
@@ -3475,7 +3564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
         <v>247</v>
       </c>
@@ -3483,7 +3572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>169</v>
       </c>
@@ -3491,7 +3580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
         <v>248</v>
       </c>
@@ -3499,7 +3588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>27</v>
       </c>
@@ -3507,7 +3596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
         <v>249</v>
       </c>
@@ -3515,12 +3604,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
         <v>250</v>
       </c>
@@ -3528,7 +3617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>251</v>
       </c>
@@ -3536,7 +3625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>114</v>
       </c>
@@ -5146,33 +5235,36 @@
     <sortCondition ref="G71:G80"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
+    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A142:A339">
     <cfRule type="duplicateValues" dxfId="19" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A142:A339">
+  <conditionalFormatting sqref="H341:H343">
     <cfRule type="duplicateValues" dxfId="18" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H341:H343">
+  <conditionalFormatting sqref="H344">
     <cfRule type="duplicateValues" dxfId="17" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H344">
+  <conditionalFormatting sqref="H345:H347">
     <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H345:H347">
+  <conditionalFormatting sqref="H346:H347">
     <cfRule type="duplicateValues" dxfId="15" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H346:H347">
     <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H346:H347">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+  <conditionalFormatting sqref="H348:H358">
+    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H348:H358">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H348:H358">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L105:L119">
     <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding FIVE FL FORM FOXF FTNT
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA376195-3FBF-40FB-B07A-74F161AC814D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D9AAAC-FD27-4ADD-BACE-8A008EC817D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$361</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="396">
   <si>
     <t>SCVL</t>
   </si>
@@ -1206,6 +1207,12 @@
   </si>
   <si>
     <t>Great Earnings growth - but too expensive right now</t>
+  </si>
+  <si>
+    <t>Interesting - Could be a momentum play</t>
+  </si>
+  <si>
+    <t>Ann purchase - Should think about purchasing it</t>
   </si>
 </sst>
 </file>
@@ -1813,7 +1820,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F128" sqref="F128"/>
+      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3493,7 +3500,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>241</v>
       </c>
@@ -3503,8 +3510,11 @@
       <c r="C129" s="3">
         <v>43705</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>242</v>
       </c>
@@ -3514,8 +3524,11 @@
       <c r="C130" s="3">
         <v>43700</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>243</v>
       </c>
@@ -3525,8 +3538,14 @@
       <c r="C131" s="3">
         <v>43677</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="3">
+        <v>43718</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>244</v>
       </c>
@@ -3534,7 +3553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
         <v>245</v>
       </c>
@@ -3544,8 +3563,11 @@
       <c r="C133" s="3">
         <v>43677</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>168</v>
       </c>
@@ -3555,8 +3577,14 @@
       <c r="C134" s="3">
         <v>43678</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="3">
+        <v>43718</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>246</v>
       </c>
@@ -3564,7 +3592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
         <v>247</v>
       </c>
@@ -3572,7 +3600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>169</v>
       </c>
@@ -3580,7 +3608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
         <v>248</v>
       </c>
@@ -3588,7 +3616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>27</v>
       </c>
@@ -3596,7 +3624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
         <v>249</v>
       </c>
@@ -3604,12 +3632,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
         <v>250</v>
       </c>
@@ -3617,7 +3645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>251</v>
       </c>
@@ -3625,7 +3653,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Adding GNRC GOOGL GPC
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3BB659-2D21-4F96-9EC8-CCE12A465495}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F86C468-4B5D-4405-A530-3B4D73656363}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="397">
   <si>
     <t>SCVL</t>
   </si>
@@ -1213,6 +1213,9 @@
   </si>
   <si>
     <t>Ann purchase - Should think about purchasing it</t>
+  </si>
+  <si>
+    <t>Around 2014 - the black diamonds don'g match - found out because the projections line does not line up…need to see</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1823,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1867,1994 +1870,1916 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="3">
-        <v>43712</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C3" s="3">
+        <v>43671</v>
+      </c>
       <c r="D3" s="3">
-        <v>43712</v>
+        <v>43715</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>135</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
+      <c r="A4" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C4" s="3">
+        <v>43676</v>
+      </c>
       <c r="D4" s="3">
-        <v>43712</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>374</v>
+        <v>43715</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="3">
+        <v>43672</v>
+      </c>
       <c r="D5" s="3">
-        <v>43712</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>374</v>
+        <v>43715</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="3">
+        <v>43672</v>
+      </c>
       <c r="D6" s="3">
-        <v>43714</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>138</v>
+        <v>43715</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>136</v>
+      <c r="A7" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C7" s="3">
+        <v>43678</v>
+      </c>
       <c r="D7" s="3">
-        <v>43714</v>
+        <v>43715</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
+        <v>386</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>139</v>
+      <c r="A8" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="3">
-        <v>43714</v>
+        <v>43690</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>141</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>140</v>
+      <c r="A9" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <v>43714</v>
+        <v>43690</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>142</v>
+      <c r="A10" s="11" t="s">
+        <v>185</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
-        <v>43677</v>
-      </c>
       <c r="D10" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>143</v>
+        <v>43690</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>144</v>
+      <c r="A11" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3">
-        <v>43677</v>
-      </c>
       <c r="D11" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>145</v>
+        <v>43690</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>146</v>
+      <c r="A12" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
-        <v>43678</v>
-      </c>
       <c r="D12" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>380</v>
+        <v>43690</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3">
-        <v>43684</v>
-      </c>
       <c r="D13" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>148</v>
+        <v>43690</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>149</v>
+      <c r="A14" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3">
-        <v>43685</v>
-      </c>
       <c r="D14" s="3">
-        <v>43715</v>
+        <v>43690</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>150</v>
+      <c r="A15" s="9" t="s">
+        <v>188</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3">
-        <v>43679</v>
-      </c>
       <c r="D15" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>380</v>
+        <v>43690</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>151</v>
+      <c r="A16" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3">
-        <v>43683</v>
-      </c>
       <c r="D16" s="3">
-        <v>43715</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>152</v>
+        <v>43690</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="3">
-        <v>43684</v>
-      </c>
       <c r="D17" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>153</v>
+        <v>43690</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3">
-        <v>43683</v>
-      </c>
       <c r="D18" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43691</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3">
-        <v>43684</v>
-      </c>
       <c r="D19" s="3">
-        <v>43715</v>
-      </c>
+        <v>43712</v>
+      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>156</v>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>192</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="3">
-        <v>43685</v>
-      </c>
       <c r="D20" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>157</v>
+        <v>43691</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="3">
-        <v>43683</v>
-      </c>
       <c r="D21" s="3">
-        <v>43715</v>
+        <v>43691</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>181</v>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D22" s="3">
+        <v>43691</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="3">
-        <v>43671</v>
-      </c>
       <c r="D23" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43691</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3">
-        <v>43676</v>
-      </c>
       <c r="D24" s="3">
-        <v>43715</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>16</v>
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>65</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="3">
-        <v>43672</v>
-      </c>
       <c r="D25" s="3">
-        <v>43715</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="3">
-        <v>43672</v>
-      </c>
       <c r="D26" s="3">
-        <v>43715</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43693</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="3">
-        <v>43678</v>
-      </c>
       <c r="D27" s="3">
-        <v>43715</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="3">
-        <v>43690</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>184</v>
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>198</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="3">
-        <v>43690</v>
+        <v>43693</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="3">
-        <v>43690</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>160</v>
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="3">
-        <v>43690</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>186</v>
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>11</v>
+        <v>366</v>
       </c>
       <c r="D32" s="3">
-        <v>43690</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>59</v>
+      <c r="A33" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="3">
-        <v>43690</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="3">
-        <v>43690</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>360</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>188</v>
+      <c r="A35" s="11" t="s">
+        <v>201</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="3">
-        <v>43690</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>11</v>
+      <c r="A36" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D36" s="3">
-        <v>43690</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>190</v>
+      <c r="A37" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="3">
-        <v>43690</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>191</v>
+      <c r="A38" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="3">
-        <v>43691</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>192</v>
+      <c r="A39" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="3">
-        <v>43691</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>193</v>
+      <c r="A40" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="3">
-        <v>43691</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>361</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>194</v>
+      <c r="A41" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="3">
-        <v>43691</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="3">
-        <v>43691</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>195</v>
+      <c r="A43" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="3">
-        <v>43693</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>65</v>
+      <c r="A44" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="3">
-        <v>43693</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>58</v>
+      <c r="A45" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="3">
-        <v>43693</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>363</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>196</v>
+      <c r="A46" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="3">
-        <v>43693</v>
+        <v>43694</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>197</v>
+      <c r="A47" s="10" t="s">
+        <v>206</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="3">
-        <v>43693</v>
+        <v>43694</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>198</v>
+      <c r="A48" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="3">
-        <v>43693</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>199</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>208</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D49" s="3">
-        <v>43693</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>161</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="3">
-        <v>43693</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="3">
-        <v>43693</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="3">
-        <v>43693</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>201</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>211</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D53" s="3">
-        <v>43693</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>67</v>
+        <v>43703</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D54" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
-        <v>162</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>124</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D56" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>11</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D57" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>118</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>203</v>
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>90</v>
+        <v>43712</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D60" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>204</v>
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D61" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>30</v>
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>164</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D62" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>205</v>
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>215</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D63" s="3">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>71</v>
+        <v>43705</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D64" s="3">
-        <v>43694</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
-        <v>206</v>
+      <c r="A65" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C65" s="3">
+        <v>43678</v>
+      </c>
       <c r="D65" s="3">
-        <v>43694</v>
+        <v>43715</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
-        <v>207</v>
+      <c r="A66" s="18" t="s">
+        <v>165</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D66" s="3">
-        <v>43703</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>208</v>
+      <c r="A67" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D67" s="3">
-        <v>43703</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D68" s="3">
-        <v>43703</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
-        <v>68</v>
+      <c r="A69" s="11" t="s">
+        <v>218</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D69" s="3">
-        <v>43703</v>
+        <v>43706</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>210</v>
+      <c r="A70" s="9" t="s">
+        <v>219</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D70" s="3">
-        <v>43703</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>211</v>
+      <c r="A71" s="11" t="s">
+        <v>220</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D71" s="3">
-        <v>43703</v>
+        <v>43706</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D72" s="3">
-        <v>43703</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>163</v>
+      <c r="A73" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D73" s="3">
-        <v>43703</v>
+        <v>43706</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
-        <v>99</v>
+      <c r="A74" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D74" s="3">
-        <v>43703</v>
+        <v>43698</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
-        <v>29</v>
+      <c r="A75" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D75" s="3">
-        <v>43703</v>
+        <v>43713</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>213</v>
+      <c r="A76" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D76" s="3">
-        <v>43703</v>
+        <v>43713</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
-        <v>214</v>
+      <c r="A77" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D77" s="3">
-        <v>43705</v>
+        <v>43713</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>11</v>
+      <c r="A78" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D78" s="3">
-        <v>43705</v>
+        <v>43713</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
-        <v>164</v>
+      <c r="A79" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D79" s="3">
-        <v>43705</v>
+      <c r="F79" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
-        <v>215</v>
+      <c r="A80" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C80" s="3">
+        <v>43684</v>
+      </c>
       <c r="D80" s="3">
-        <v>43705</v>
+        <v>43715</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
-        <v>216</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>222</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D81" s="3">
-        <v>43705</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="18" t="s">
-        <v>165</v>
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D82" s="3">
-        <v>43698</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>365</v>
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>224</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D83" s="3">
-        <v>43698</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D84" s="3">
-        <v>43706</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>217</v>
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D85" s="3">
-        <v>43706</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
-        <v>218</v>
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>225</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D86" s="3">
-        <v>43706</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
-        <v>219</v>
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
+        <v>226</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D87" s="3">
-        <v>43706</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43714</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D88" s="3">
-        <v>43706</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
-        <v>221</v>
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D89" s="3">
-        <v>43706</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43714</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D90" s="3">
-        <v>43706</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>84</v>
+        <v>43714</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="L90" s="11"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C91" s="3">
+        <v>43636</v>
+      </c>
       <c r="D91" s="3">
-        <v>43698</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>130</v>
+        <v>43716</v>
+      </c>
+      <c r="L91" s="9"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C92" s="3">
+        <v>43683</v>
+      </c>
       <c r="D92" s="3">
-        <v>43713</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>129</v>
+        <v>43716</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C93" s="3">
+        <v>43642</v>
+      </c>
       <c r="D93" s="3">
-        <v>43713</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>57</v>
+        <v>43716</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>232</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C94" s="3">
+        <v>43678</v>
+      </c>
       <c r="D94" s="3">
-        <v>43713</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D95" s="3">
-        <v>43713</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43716</v>
+      </c>
+      <c r="L94" s="11"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>372</v>
+      <c r="C96" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D96" s="3">
+        <v>43715</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C97" s="3">
+        <v>43685</v>
+      </c>
       <c r="D97" s="3">
-        <v>43714</v>
-      </c>
+        <v>43716</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L97" s="7"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C98" s="3">
+        <v>43677</v>
+      </c>
       <c r="D98" s="3">
-        <v>43714</v>
+        <v>43716</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="D99" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C99" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D99" s="3">
+        <v>43716</v>
+      </c>
+      <c r="L99" s="11"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C100" s="3">
+        <v>43679</v>
+      </c>
       <c r="D100" s="3">
-        <v>43714</v>
+        <v>43715</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>75</v>
+      <c r="A101" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C101" s="3">
+        <v>43684</v>
+      </c>
       <c r="D101" s="3">
-        <v>43714</v>
-      </c>
+        <v>43716</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L101" s="9"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
-        <v>225</v>
+      <c r="A102" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C102" s="3">
+        <v>43664</v>
+      </c>
       <c r="D102" s="3">
-        <v>43714</v>
-      </c>
+        <v>43716</v>
+      </c>
+      <c r="L102" s="11"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
-        <v>226</v>
+      <c r="A103" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C103" s="3">
+        <v>43670</v>
+      </c>
       <c r="D103" s="3">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>375</v>
-      </c>
+        <v>391</v>
+      </c>
+      <c r="L103" s="11"/>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
-        <v>227</v>
+      <c r="A104" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C104" s="3">
+        <v>43659</v>
+      </c>
       <c r="D104" s="3">
-        <v>43714</v>
-      </c>
+        <v>43716</v>
+      </c>
+      <c r="L104" s="11"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
-        <v>228</v>
+      <c r="A105" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C105" s="3">
+        <v>43683</v>
+      </c>
       <c r="D105" s="3">
-        <v>43714</v>
-      </c>
+        <v>43716</v>
+      </c>
+      <c r="L105" s="11"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C106" s="3">
+        <v>43671</v>
+      </c>
       <c r="D106" s="3">
-        <v>43714</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="L106" s="11"/>
+        <v>43717</v>
+      </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="3">
-        <v>43636</v>
+        <v>43683</v>
       </c>
       <c r="D107" s="3">
-        <v>43716</v>
-      </c>
-      <c r="L107" s="9"/>
+        <v>43717</v>
+      </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C108" s="3">
-        <v>43683</v>
-      </c>
-      <c r="D108" s="3">
-        <v>43716</v>
-      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
-        <v>231</v>
+      <c r="A109" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C109" s="3">
-        <v>43642</v>
+        <v>43670</v>
       </c>
       <c r="D109" s="3">
-        <v>43716</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>388</v>
+        <v>43717</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
-        <v>232</v>
+      <c r="A110" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C110" s="3">
-        <v>43678</v>
+        <v>43670</v>
       </c>
       <c r="D110" s="3">
-        <v>43716</v>
-      </c>
-      <c r="L110" s="11"/>
+        <v>43717</v>
+      </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>233</v>
+        <v>166</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F111" s="2" t="s">
-        <v>387</v>
+      <c r="C111" s="3">
+        <v>43641</v>
+      </c>
+      <c r="D111" s="3">
+        <v>43717</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A112" s="11" t="s">
-        <v>234</v>
+      <c r="A112" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C112" s="3">
-        <v>43685</v>
+        <v>43670</v>
       </c>
       <c r="D112" s="3">
-        <v>43716</v>
+        <v>43717</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L112" s="7"/>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="11" t="s">
-        <v>235</v>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C113" s="3">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C114" s="3">
+        <v>43670</v>
+      </c>
+      <c r="D114" s="3">
+        <v>43717</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C115" s="3">
+        <v>43705</v>
+      </c>
+      <c r="D115" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" s="3">
+        <v>43714</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" s="3">
+        <v>43700</v>
+      </c>
+      <c r="D117" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D118" s="3">
+        <v>43715</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" s="3">
         <v>43677</v>
       </c>
-      <c r="D113" s="3">
-        <v>43716</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C114" s="3">
+      <c r="D119" s="3">
+        <v>43718</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C121" s="3">
         <v>43677</v>
       </c>
-      <c r="D114" s="3">
-        <v>43716</v>
-      </c>
-      <c r="L114" s="11"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C115" s="3">
-        <v>43684</v>
-      </c>
-      <c r="D115" s="3">
-        <v>43716</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="L115" s="9"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C116" s="3">
+      <c r="D121" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122" s="3">
+        <v>43678</v>
+      </c>
+      <c r="D122" s="3">
+        <v>43718</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D124" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" s="3">
+        <v>43676</v>
+      </c>
+      <c r="D125" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" s="3">
+        <v>43678</v>
+      </c>
+      <c r="D126" s="3">
+        <v>43718</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" s="3"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" s="3">
+        <v>43671</v>
+      </c>
+      <c r="D128" s="3">
+        <v>43718</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C129" s="3">
         <v>43664</v>
-      </c>
-      <c r="D116" s="3">
-        <v>43716</v>
-      </c>
-      <c r="L116" s="11"/>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C117" s="3">
-        <v>43670</v>
-      </c>
-      <c r="D117" s="3">
-        <v>43716</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="L117" s="11"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" s="3">
-        <v>43659</v>
-      </c>
-      <c r="D118" s="3">
-        <v>43716</v>
-      </c>
-      <c r="L118" s="11"/>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" s="3">
-        <v>43683</v>
-      </c>
-      <c r="D119" s="3">
-        <v>43716</v>
-      </c>
-      <c r="L119" s="11"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C120" s="3">
-        <v>43671</v>
-      </c>
-      <c r="D120" s="3">
-        <v>43717</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C121" s="3">
-        <v>43683</v>
-      </c>
-      <c r="D121" s="3">
-        <v>43717</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C123" s="3">
-        <v>43670</v>
-      </c>
-      <c r="D123" s="3">
-        <v>43717</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C124" s="3">
-        <v>43670</v>
-      </c>
-      <c r="D124" s="3">
-        <v>43717</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C125" s="3">
-        <v>43641</v>
-      </c>
-      <c r="D125" s="3">
-        <v>43717</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C126" s="3">
-        <v>43670</v>
-      </c>
-      <c r="D126" s="3">
-        <v>43717</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C128" s="3">
-        <v>43670</v>
-      </c>
-      <c r="D128" s="3">
-        <v>43717</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C129" s="3">
-        <v>43705</v>
       </c>
       <c r="D129" s="3">
         <v>43718</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="9" t="s">
-        <v>242</v>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="11" t="s">
+        <v>250</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C130" s="3">
-        <v>43700</v>
-      </c>
-      <c r="D130" s="3">
-        <v>43718</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C131" s="3">
-        <v>43677</v>
-      </c>
-      <c r="D131" s="3">
-        <v>43718</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="11" t="s">
-        <v>244</v>
+        <v>43699</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="11" t="s">
-        <v>245</v>
+      <c r="C132" s="3">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C133" s="3">
-        <v>43677</v>
-      </c>
-      <c r="D133" s="3">
-        <v>43718</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="11" t="s">
-        <v>168</v>
+        <v>43670</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C134" s="3">
-        <v>43678</v>
-      </c>
-      <c r="D134" s="3">
-        <v>43718</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="11" t="s">
-        <v>247</v>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C136" s="3">
-        <v>43677</v>
-      </c>
       <c r="D136" s="3">
-        <v>43718</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="9" t="s">
-        <v>169</v>
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="11" t="s">
+        <v>253</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C137" s="3">
-        <v>43676</v>
-      </c>
-      <c r="D137" s="3">
-        <v>43718</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C138" s="3">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C139" s="3"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C140" s="3">
-        <v>43671</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C141" s="3">
-        <v>43664</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C142" s="3">
-        <v>43676</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C143" s="3">
-        <v>43699</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C144" s="3">
-        <v>43664</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C145" s="3">
-        <v>43670</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>38</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="11" t="s">
+        <v>258</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="11" t="s">
-        <v>252</v>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="9" t="s">
-        <v>170</v>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C148" s="3">
+        <v>43684</v>
+      </c>
       <c r="D148" s="3">
-        <v>43698</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="11" t="s">
-        <v>253</v>
+        <v>43715</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="11" t="s">
-        <v>254</v>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="11" t="s">
-        <v>257</v>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="11" t="s">
-        <v>258</v>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
-        <v>23</v>
+      <c r="C158" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D158" s="3">
+        <v>43715</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="11" t="s">
+        <v>264</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="9" t="s">
-        <v>259</v>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="9" t="s">
-        <v>260</v>
+      <c r="A161" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>26</v>
+      <c r="A162" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="2" t="s">
-        <v>54</v>
+      <c r="A164" s="11" t="s">
+        <v>268</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="11" t="s">
-        <v>262</v>
+      <c r="A165" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>11</v>
@@ -3862,71 +3787,71 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D166" s="3">
+        <v>43698</v>
+      </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
-        <v>105</v>
+      <c r="A167" s="11" t="s">
+        <v>269</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="10" t="s">
-        <v>263</v>
+      <c r="A168" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="11" t="s">
-        <v>264</v>
+      <c r="A169" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="11" t="s">
-        <v>265</v>
+      <c r="A170" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>134</v>
+      <c r="A171" s="11" t="s">
+        <v>271</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="11" t="s">
-        <v>266</v>
+      <c r="A172" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>11</v>
+      <c r="A173" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="11" t="s">
-        <v>268</v>
+      <c r="A174" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>11</v>
@@ -3934,7 +3859,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>11</v>
@@ -3942,138 +3867,162 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D176" s="3">
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D180" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="10" t="s">
-        <v>272</v>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="11" t="s">
+        <v>277</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>31</v>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="11" t="s">
+        <v>278</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="11" t="s">
-        <v>273</v>
+      <c r="D186" s="3">
+        <v>43714</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D187" s="3">
+        <v>43714</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G187" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
-        <v>45</v>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="9" t="s">
-        <v>172</v>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C190" s="3">
+        <v>43684</v>
+      </c>
       <c r="D190" s="3">
-        <v>43698</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43715</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="11" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>36</v>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="9" t="s">
+        <v>282</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>11</v>
@@ -4081,7 +4030,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>11</v>
@@ -4089,23 +4038,23 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="11" t="s">
-        <v>278</v>
+      <c r="A195" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="11" t="s">
-        <v>279</v>
+      <c r="A196" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>11</v>
@@ -4113,47 +4062,50 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="11" t="s">
-        <v>281</v>
+      <c r="A198" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="9" t="s">
-        <v>282</v>
+      <c r="A199" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="D199" s="3">
+        <v>43698</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="11" t="s">
-        <v>284</v>
+      <c r="A201" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>116</v>
+      <c r="A202" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>11</v>
@@ -4161,7 +4113,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>11</v>
@@ -4169,420 +4121,477 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
-        <v>285</v>
+        <v>174</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
-        <v>104</v>
+      <c r="A205" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="11" t="s">
-        <v>173</v>
+      <c r="A206" s="9" t="s">
+        <v>289</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D206" s="3">
-        <v>43698</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="11" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>112</v>
+      <c r="A208" s="11" t="s">
+        <v>291</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="11" t="s">
-        <v>287</v>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C209" s="3">
+        <v>43685</v>
+      </c>
+      <c r="D209" s="3">
+        <v>43715</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="11" t="s">
-        <v>174</v>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="11" t="s">
-        <v>288</v>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="9" t="s">
-        <v>289</v>
+      <c r="C212" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D212" s="3">
+        <v>43715</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="G212" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="11" t="s">
-        <v>290</v>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214" s="9" t="s">
+        <v>292</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="11" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
-        <v>69</v>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216" s="11" t="s">
+        <v>294</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="9" t="s">
-        <v>292</v>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219" s="11" t="s">
+        <v>295</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="11" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
-        <v>111</v>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222" s="11" t="s">
+        <v>298</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="11" t="s">
-        <v>295</v>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="11" t="s">
-        <v>296</v>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
-        <v>51</v>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="11" t="s">
+        <v>300</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="9" t="s">
-        <v>175</v>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
-        <v>86</v>
+      <c r="D229" s="3">
+        <v>43714</v>
+      </c>
+      <c r="F229" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="11" t="s">
-        <v>299</v>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="9" t="s">
-        <v>301</v>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="11" t="s">
+        <v>303</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="9" t="s">
-        <v>302</v>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="11" t="s">
+        <v>176</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
-        <v>87</v>
+      <c r="D235" s="3">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="11" t="s">
+        <v>304</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="11" t="s">
-        <v>303</v>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D239" s="3">
-        <v>43698</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
-        <v>304</v>
+        <v>177</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="11" t="s">
-        <v>305</v>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D242" s="3">
+        <v>43712</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G242" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="11" t="s">
-        <v>177</v>
+        <v>306</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="2" t="s">
-        <v>50</v>
+      <c r="C245" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D245" s="3">
+        <v>43715</v>
+      </c>
+      <c r="F245" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G245" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="11" t="s">
-        <v>306</v>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="10" t="s">
+        <v>307</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="7" t="s">
-        <v>178</v>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="10" t="s">
-        <v>307</v>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="11" t="s">
+        <v>308</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="2" t="s">
-        <v>49</v>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="9" t="s">
+        <v>309</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="11" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="9" t="s">
-        <v>309</v>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="11" t="s">
-        <v>310</v>
+      <c r="C252" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D252" s="3">
+        <v>43715</v>
+      </c>
+      <c r="F252" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G252" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="2" t="s">
-        <v>98</v>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="11" t="s">
+        <v>311</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="11" t="s">
-        <v>312</v>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>11</v>
@@ -4590,7 +4599,7 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>11</v>
@@ -4598,7 +4607,7 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>11</v>
@@ -4606,31 +4615,31 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A260" s="2" t="s">
-        <v>35</v>
+      <c r="A260" s="9" t="s">
+        <v>313</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A261" s="9" t="s">
-        <v>313</v>
+      <c r="A261" s="11" t="s">
+        <v>314</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A262" s="11" t="s">
-        <v>314</v>
+      <c r="A262" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>11</v>
@@ -4638,7 +4647,7 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>11</v>
@@ -4646,7 +4655,7 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>11</v>
@@ -4654,23 +4663,23 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
-        <v>24</v>
+      <c r="A266" s="11" t="s">
+        <v>315</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A267" s="11" t="s">
-        <v>315</v>
+      <c r="A267" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>11</v>
@@ -4678,50 +4687,50 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F268" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
-        <v>0</v>
+      <c r="A269" s="11" t="s">
+        <v>316</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F269" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A270" s="11" t="s">
-        <v>316</v>
+      <c r="A270" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
-        <v>25</v>
+      <c r="A271" s="11" t="s">
+        <v>317</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A272" s="11" t="s">
-        <v>317</v>
+      <c r="A272" s="9" t="s">
+        <v>318</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="9" t="s">
-        <v>318</v>
+      <c r="A273" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>11</v>
@@ -4729,15 +4738,15 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="2" t="s">
-        <v>18</v>
+      <c r="A275" s="11" t="s">
+        <v>319</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>11</v>
@@ -4745,7 +4754,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>11</v>
@@ -4753,41 +4762,41 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>11</v>
+      <c r="A278" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="2" t="s">
-        <v>44</v>
+      <c r="A280" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="9" t="s">
-        <v>322</v>
+      <c r="A281" s="11" t="s">
+        <v>323</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="11" t="s">
-        <v>323</v>
+      <c r="A282" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>11</v>
@@ -4795,15 +4804,15 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="2" t="s">
-        <v>97</v>
+      <c r="A284" s="11" t="s">
+        <v>324</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>11</v>
@@ -4811,31 +4820,31 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="11" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="11" t="s">
-        <v>325</v>
+      <c r="A286" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="2" t="s">
-        <v>122</v>
+      <c r="A287" s="9" t="s">
+        <v>326</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="9" t="s">
-        <v>326</v>
+      <c r="A288" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>11</v>
@@ -4843,15 +4852,15 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="2" t="s">
-        <v>95</v>
+      <c r="A290" s="11" t="s">
+        <v>327</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>11</v>
@@ -4859,7 +4868,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>11</v>
@@ -4867,31 +4876,31 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="11" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="11" t="s">
-        <v>329</v>
+      <c r="A293" s="10" t="s">
+        <v>330</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="10" t="s">
-        <v>330</v>
+      <c r="A294" s="11" t="s">
+        <v>331</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="11" t="s">
-        <v>331</v>
+      <c r="A295" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>11</v>
@@ -4899,7 +4908,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>11</v>
@@ -4907,15 +4916,15 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="2" t="s">
-        <v>33</v>
+      <c r="A298" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>11</v>
@@ -4923,7 +4932,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>11</v>
@@ -4931,7 +4940,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>11</v>
@@ -4939,7 +4948,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>11</v>
@@ -4947,7 +4956,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>11</v>
@@ -4955,34 +4964,40 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="11" t="s">
-        <v>337</v>
+      <c r="A304" s="9" t="s">
+        <v>338</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A305" s="9" t="s">
-        <v>338</v>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D305" s="3">
+        <v>43712</v>
+      </c>
+      <c r="F305" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>125</v>
       </c>
@@ -4990,7 +5005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>126</v>
       </c>
@@ -4998,7 +5013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="9" t="s">
         <v>339</v>
       </c>
@@ -5006,7 +5021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="9" t="s">
         <v>340</v>
       </c>
@@ -5014,7 +5029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="11" t="s">
         <v>341</v>
       </c>
@@ -5022,7 +5037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>117</v>
       </c>
@@ -5030,7 +5045,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>109</v>
       </c>
@@ -5038,7 +5053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>121</v>
       </c>
@@ -5046,12 +5061,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="11" t="s">
         <v>179</v>
       </c>
@@ -5059,7 +5074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>80</v>
       </c>
@@ -5067,7 +5082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="11" t="s">
         <v>180</v>
       </c>
@@ -5078,12 +5093,12 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>43</v>
       </c>
@@ -5293,8 +5308,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A361" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G71:G80">
-    <sortCondition ref="G71:G80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L358">
+    <sortCondition ref="A2:A358"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
     <cfRule type="duplicateValues" dxfId="20" priority="11"/>

</xml_diff>

<commit_message>
Adding HBAN HCA HD HMSY HOFT HOMB HQY HSTM HUM HWC
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2EC123-F3B2-4635-B175-73DD2DECF257}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449F0841-1DB1-4D9F-9B07-DCE2D952B039}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$361</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1823,7 +1822,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D133" sqref="D133"/>
+      <selection pane="bottomLeft" activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3533,6 +3532,12 @@
       <c r="B134" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C134" s="3">
+        <v>43671</v>
+      </c>
+      <c r="D134" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
@@ -3541,6 +3546,12 @@
       <c r="B135" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C135" s="3">
+        <v>43676</v>
+      </c>
+      <c r="D135" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
@@ -3549,8 +3560,11 @@
       <c r="B136" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C136" s="3">
+        <v>43697</v>
+      </c>
       <c r="D136" s="3">
-        <v>43698</v>
+        <v>43722</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,6 +3574,12 @@
       <c r="B137" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C137" s="3">
+        <v>43679</v>
+      </c>
+      <c r="D137" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
@@ -3568,6 +3588,12 @@
       <c r="B138" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C138" s="3">
+        <v>43713</v>
+      </c>
+      <c r="D138" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
@@ -3576,6 +3602,12 @@
       <c r="B139" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C139" s="3">
+        <v>43664</v>
+      </c>
+      <c r="D139" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
@@ -3584,6 +3616,12 @@
       <c r="B140" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C140" s="3">
+        <v>43711</v>
+      </c>
+      <c r="D140" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
@@ -3592,6 +3630,12 @@
       <c r="B141" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C141" s="3">
+        <v>43668</v>
+      </c>
+      <c r="D141" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
@@ -3600,6 +3644,12 @@
       <c r="B142" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C142" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D142" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
@@ -3615,6 +3665,12 @@
       </c>
       <c r="B144" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C144" s="3">
+        <v>43662</v>
+      </c>
+      <c r="D144" s="3">
+        <v>43722</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding IBM IDXX IEX IIVI ILMN
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449F0841-1DB1-4D9F-9B07-DCE2D952B039}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976642EA-9ABB-4A1A-AF99-FEA27884C99A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="398">
   <si>
     <t>SCVL</t>
   </si>
@@ -1169,9 +1169,6 @@
     <t>Another one where the price does not move up?</t>
   </si>
   <si>
-    <t>Looks very interesting - Maybe ask Ann</t>
-  </si>
-  <si>
     <t>The projections seem to have gone up. Ann has it</t>
   </si>
   <si>
@@ -1215,6 +1212,12 @@
   </si>
   <si>
     <t>Around 2014 - the black diamonds don'g match - found out because the projections line does not line up…need to see</t>
+  </si>
+  <si>
+    <t>Probably chaff - Ann says analysts not interested in this company</t>
+  </si>
+  <si>
+    <t>Ann has it now</t>
   </si>
 </sst>
 </file>
@@ -1821,8 +1824,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D144" sqref="D144"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1893,7 @@
         <v>43715</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1949,7 +1952,7 @@
         <v>43715</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>357</v>
@@ -2959,7 +2962,7 @@
         <v>43716</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -2985,7 +2988,7 @@
         <v>11</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -3016,7 +3019,7 @@
         <v>43716</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L97" s="7"/>
     </row>
@@ -3080,7 +3083,7 @@
         <v>43716</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L101" s="9"/>
     </row>
@@ -3113,7 +3116,7 @@
         <v>43716</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L103" s="11"/>
     </row>
@@ -3239,7 +3242,7 @@
         <v>43717</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3264,7 +3267,7 @@
         <v>43717</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3340,7 +3343,7 @@
         <v>43718</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3379,7 +3382,7 @@
         <v>43718</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3455,7 +3458,7 @@
         <v>43718</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,6 +3680,12 @@
       <c r="A145" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="C145" s="3">
+        <v>43663</v>
+      </c>
+      <c r="D145" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="11" t="s">
@@ -3685,6 +3694,12 @@
       <c r="B146" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C146" s="3">
+        <v>43678</v>
+      </c>
+      <c r="D146" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
@@ -3693,6 +3708,12 @@
       <c r="B147" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C147" s="3">
+        <v>43671</v>
+      </c>
+      <c r="D147" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
@@ -3705,10 +3726,10 @@
         <v>43684</v>
       </c>
       <c r="D148" s="3">
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>381</v>
+        <v>397</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3718,6 +3739,12 @@
       <c r="B149" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C149" s="3">
+        <v>43690</v>
+      </c>
+      <c r="D149" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="s">
@@ -3726,11 +3753,20 @@
       <c r="B150" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C150" s="3">
+        <v>43675</v>
+      </c>
+      <c r="D150" s="3">
+        <v>43722</v>
+      </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="C151" s="3">
+        <v>43671</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
@@ -3739,6 +3775,9 @@
       <c r="B152" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C152" s="3">
+        <v>43699</v>
+      </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
@@ -3747,6 +3786,9 @@
       <c r="B153" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C153" s="3">
+        <v>43670</v>
+      </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
@@ -3755,6 +3797,9 @@
       <c r="B154" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C154" s="3">
+        <v>43676</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
@@ -3763,6 +3808,9 @@
       <c r="B155" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C155" s="3">
+        <v>43669</v>
+      </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
@@ -3771,6 +3819,9 @@
       <c r="B156" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C156" s="3">
+        <v>43664</v>
+      </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
@@ -3779,6 +3830,9 @@
       <c r="B157" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C157" s="3">
+        <v>43705</v>
+      </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
@@ -3791,7 +3845,7 @@
         <v>43683</v>
       </c>
       <c r="D158" s="3">
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>155</v>
@@ -3801,8 +3855,8 @@
       <c r="A159" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>11</v>
+      <c r="F159" s="2" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3812,48 +3866,60 @@
       <c r="B160" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C160" s="3">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C161" s="3">
+        <v>43662</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>266</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C162" s="3">
+        <v>43642</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F163" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F164" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C165" s="3">
+        <v>43669</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>66</v>
       </c>
@@ -3864,7 +3930,7 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="11" t="s">
         <v>269</v>
       </c>
@@ -3872,7 +3938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="9" t="s">
         <v>171</v>
       </c>
@@ -3880,7 +3946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
         <v>270</v>
       </c>
@@ -3888,7 +3954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>37</v>
       </c>
@@ -3896,7 +3962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>271</v>
       </c>
@@ -3904,7 +3970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>85</v>
       </c>
@@ -3912,12 +3978,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>272</v>
       </c>
@@ -3925,7 +3991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>31</v>
       </c>
@@ -3933,7 +3999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>53</v>
       </c>
@@ -4077,7 +4143,7 @@
         <v>43715</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -4241,7 +4307,7 @@
         <v>43715</v>
       </c>
       <c r="F209" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -4274,7 +4340,7 @@
         <v>43715</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G212" s="2" t="s">
         <v>143</v>

</xml_diff>

<commit_message>
Adding INTC INTU INVA IRBT IR ISRG ITRN
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976642EA-9ABB-4A1A-AF99-FEA27884C99A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97430862-81D5-4B17-822C-939D444261B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="400">
   <si>
     <t>SCVL</t>
   </si>
@@ -1218,6 +1218,12 @@
   </si>
   <si>
     <t>Ann has it now</t>
+  </si>
+  <si>
+    <t>Jul - works when the date is only till 2020 - Maybe there is some trick there????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNBC has just two more quarters of projections but Ann has 6 more </t>
   </si>
 </sst>
 </file>
@@ -1825,7 +1831,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D150" sqref="D150"/>
+      <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3726,7 +3732,7 @@
         <v>43684</v>
       </c>
       <c r="D148" s="3">
-        <v>43722</v>
+        <v>43723</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>397</v>
@@ -3743,7 +3749,7 @@
         <v>43690</v>
       </c>
       <c r="D149" s="3">
-        <v>43722</v>
+        <v>43723</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -3757,7 +3763,7 @@
         <v>43675</v>
       </c>
       <c r="D150" s="3">
-        <v>43722</v>
+        <v>43723</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -3767,6 +3773,9 @@
       <c r="C151" s="3">
         <v>43671</v>
       </c>
+      <c r="D151" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
@@ -3778,6 +3787,12 @@
       <c r="C152" s="3">
         <v>43699</v>
       </c>
+      <c r="D152" s="3">
+        <v>43723</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
@@ -3789,6 +3804,12 @@
       <c r="C153" s="3">
         <v>43670</v>
       </c>
+      <c r="D153" s="3">
+        <v>43723</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
@@ -3800,6 +3821,9 @@
       <c r="C154" s="3">
         <v>43676</v>
       </c>
+      <c r="D154" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
@@ -3811,6 +3835,9 @@
       <c r="C155" s="3">
         <v>43669</v>
       </c>
+      <c r="D155" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
@@ -3822,6 +3849,9 @@
       <c r="C156" s="3">
         <v>43664</v>
       </c>
+      <c r="D156" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
@@ -3832,6 +3862,9 @@
       </c>
       <c r="C157" s="3">
         <v>43705</v>
+      </c>
+      <c r="D157" s="3">
+        <v>43723</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding JEC JPM KBH KO
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97430862-81D5-4B17-822C-939D444261B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD39C80-6ADA-4C1E-A68B-F742553FF905}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,10 +14,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$361</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1831,7 +1837,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D157" sqref="D157"/>
+      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3902,6 +3908,9 @@
       <c r="C160" s="3">
         <v>43682</v>
       </c>
+      <c r="D160" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
@@ -3913,6 +3922,9 @@
       <c r="C161" s="3">
         <v>43662</v>
       </c>
+      <c r="D161" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
@@ -3924,6 +3936,9 @@
       <c r="C162" s="3">
         <v>43642</v>
       </c>
+      <c r="D162" s="3">
+        <v>43723</v>
+      </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
@@ -3950,6 +3965,9 @@
       </c>
       <c r="C165" s="3">
         <v>43669</v>
+      </c>
+      <c r="D165" s="3">
+        <v>43723</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding LAD LEN LFSU LGIH LH
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD39C80-6ADA-4C1E-A68B-F742553FF905}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D40639-970B-4366-A813-952E3C232E83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="400">
   <si>
     <t>SCVL</t>
   </si>
@@ -1314,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1341,6 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1836,8 +1837,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3971,14 +3972,17 @@
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
+      <c r="A166" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C166" s="3">
+        <v>43670</v>
+      </c>
       <c r="D166" s="3">
-        <v>43698</v>
+        <v>43724</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3988,6 +3992,12 @@
       <c r="B167" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C167" s="3">
+        <v>43641</v>
+      </c>
+      <c r="D167" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="9" t="s">
@@ -3996,6 +4006,12 @@
       <c r="B168" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C168" s="3">
+        <v>43677</v>
+      </c>
+      <c r="D168" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
@@ -4004,13 +4020,25 @@
       <c r="B169" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C169" s="3">
+        <v>43683</v>
+      </c>
+      <c r="D169" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C170" s="3">
+        <v>43671</v>
+      </c>
+      <c r="D170" s="3">
+        <v>43724</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4020,6 +4048,10 @@
       <c r="B171" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C171" s="3">
+        <v>43684</v>
+      </c>
+      <c r="D171" s="3"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
@@ -4028,11 +4060,17 @@
       <c r="B172" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C172" s="3">
+        <v>43669</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C173" s="3">
+        <v>43671</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
@@ -4041,6 +4079,9 @@
       <c r="B174" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C174" s="3">
+        <v>43683</v>
+      </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
@@ -4049,6 +4090,9 @@
       <c r="B175" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C175" s="3">
+        <v>43671</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
@@ -4057,6 +4101,9 @@
       <c r="B176" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C176" s="3">
+        <v>43670</v>
+      </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
@@ -4065,6 +4112,9 @@
       <c r="B177" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F177" s="2" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="11" t="s">
@@ -4073,6 +4123,9 @@
       <c r="B178" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C178" s="3">
+        <v>43713</v>
+      </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
@@ -4080,6 +4133,9 @@
       </c>
       <c r="B179" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C179" s="3">
+        <v>43671</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding LHCG LMT LOGM LOPE LPLA
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D40639-970B-4366-A813-952E3C232E83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59767EE3-5A94-4532-B041-E9BD1FC60234}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2885" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="401">
   <si>
     <t>SCVL</t>
   </si>
@@ -1230,6 +1230,9 @@
   </si>
   <si>
     <t xml:space="preserve">CNBC has just two more quarters of projections but Ann has 6 more </t>
+  </si>
+  <si>
+    <t>Ann has it</t>
   </si>
 </sst>
 </file>
@@ -1838,7 +1841,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
+      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3972,7 +3975,7 @@
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="20" t="s">
+      <c r="A166" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B166" s="2" t="s">
@@ -4028,7 +4031,7 @@
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="20" t="s">
+      <c r="A170" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B170" s="2" t="s">
@@ -4051,7 +4054,9 @@
       <c r="C171" s="3">
         <v>43684</v>
       </c>
-      <c r="D171" s="3"/>
+      <c r="D171" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
@@ -4063,6 +4068,9 @@
       <c r="C172" s="3">
         <v>43669</v>
       </c>
+      <c r="D172" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
@@ -4071,6 +4079,9 @@
       <c r="C173" s="3">
         <v>43671</v>
       </c>
+      <c r="D173" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
@@ -4082,9 +4093,12 @@
       <c r="C174" s="3">
         <v>43683</v>
       </c>
+      <c r="D174" s="3">
+        <v>43724</v>
+      </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+      <c r="A175" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B175" s="2" t="s">
@@ -4093,9 +4107,15 @@
       <c r="C175" s="3">
         <v>43671</v>
       </c>
+      <c r="D175" s="3">
+        <v>43724</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="20" t="s">
         <v>53</v>
       </c>
       <c r="B176" s="2" t="s">

</xml_diff>

<commit_message>
Adding LSTR LULU LUV
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59767EE3-5A94-4532-B041-E9BD1FC60234}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7B71C1-3AA2-4EFC-B5DA-5463217BA896}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3173" uniqueCount="403">
   <si>
     <t>SCVL</t>
   </si>
@@ -1233,6 +1233,12 @@
   </si>
   <si>
     <t>Ann has it</t>
+  </si>
+  <si>
+    <t>730/2019</t>
+  </si>
+  <si>
+    <t>May 29th - no chart after that?</t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1840,8 +1846,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4115,7 +4121,7 @@
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="20" t="s">
+      <c r="A176" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B176" s="2" t="s">
@@ -4123,6 +4129,9 @@
       </c>
       <c r="C176" s="3">
         <v>43670</v>
+      </c>
+      <c r="D176" s="3">
+        <v>43725</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -4146,6 +4155,9 @@
       <c r="C178" s="3">
         <v>43713</v>
       </c>
+      <c r="D178" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
@@ -4157,13 +4169,19 @@
       <c r="C179" s="3">
         <v>43671</v>
       </c>
+      <c r="D179" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="9" t="s">
+      <c r="A180" s="20" t="s">
         <v>172</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="D180" s="3">
         <v>43698</v>
@@ -4176,6 +4194,9 @@
       <c r="B181" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C181" s="3">
+        <v>43677</v>
+      </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
@@ -4184,6 +4205,9 @@
       <c r="B182" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C182" s="3">
+        <v>43671</v>
+      </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="11" t="s">
@@ -4192,6 +4216,9 @@
       <c r="B183" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C183" s="3">
+        <v>43677</v>
+      </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="11" t="s">
@@ -4200,6 +4227,9 @@
       <c r="B184" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C184" s="3">
+        <v>43676</v>
+      </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="11" t="s">
@@ -4208,6 +4238,9 @@
       <c r="B185" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C185" s="3">
+        <v>43707</v>
+      </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
@@ -4216,6 +4249,9 @@
       <c r="B186" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C186" s="3">
+        <v>43678</v>
+      </c>
       <c r="D186" s="3">
         <v>43714</v>
       </c>
@@ -4230,6 +4266,9 @@
       <c r="B187" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C187" s="3">
+        <v>43675</v>
+      </c>
       <c r="D187" s="3">
         <v>43714</v>
       </c>
@@ -4247,6 +4286,9 @@
       <c r="B188" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C188" s="3">
+        <v>43677</v>
+      </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="11" t="s">
@@ -4255,6 +4297,9 @@
       <c r="B189" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C189" s="3">
+        <v>43643</v>
+      </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
@@ -4280,6 +4325,9 @@
       <c r="B191" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F191" s="2" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="9" t="s">
@@ -4288,123 +4336,168 @@
       <c r="B192" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C192" s="3">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
         <v>283</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C193" s="3">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
         <v>284</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C194" s="3">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C195" s="3">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C196" s="3">
+        <v>43670</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
         <v>285</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C197" s="3">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C198" s="3">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="11" t="s">
         <v>173</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C199" s="3">
+        <v>43678</v>
+      </c>
       <c r="D199" s="3">
         <v>43698</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
         <v>286</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C200" s="3">
+        <v>43656</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C201" s="3">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="11" t="s">
         <v>287</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C202" s="3">
+        <v>43652</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C203" s="3">
+        <v>43669</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C204" s="3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="11" t="s">
         <v>288</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F205" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="9" t="s">
         <v>289</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C206" s="3">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="11" t="s">
         <v>290</v>
       </c>
@@ -4412,7 +4505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
         <v>291</v>
       </c>

</xml_diff>

<commit_message>
Adding MA MANT MAS MASI MDLZ MDT
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7B71C1-3AA2-4EFC-B5DA-5463217BA896}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1777728C-C37B-4870-AE3B-4A71CB213DAC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3173" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="403">
   <si>
     <t>SCVL</t>
   </si>
@@ -1847,7 +1847,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
+      <selection pane="bottomLeft" activeCell="F186" sqref="F186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4184,7 +4184,7 @@
         <v>401</v>
       </c>
       <c r="D180" s="3">
-        <v>43698</v>
+        <v>43725</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -4197,6 +4197,9 @@
       <c r="C181" s="3">
         <v>43677</v>
       </c>
+      <c r="D181" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
@@ -4208,6 +4211,9 @@
       <c r="C182" s="3">
         <v>43671</v>
       </c>
+      <c r="D182" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="11" t="s">
@@ -4219,6 +4225,9 @@
       <c r="C183" s="3">
         <v>43677</v>
       </c>
+      <c r="D183" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="11" t="s">
@@ -4230,6 +4239,9 @@
       <c r="C184" s="3">
         <v>43676</v>
       </c>
+      <c r="D184" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="11" t="s">
@@ -4240,6 +4252,9 @@
       </c>
       <c r="C185" s="3">
         <v>43707</v>
+      </c>
+      <c r="D185" s="3">
+        <v>43725</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding MEOH MKC MNST MPLX MPWR
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1777728C-C37B-4870-AE3B-4A71CB213DAC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE771FB3-953B-4EC0-9FBB-D362226B58ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="404">
   <si>
     <t>SCVL</t>
   </si>
@@ -1239,6 +1239,9 @@
   </si>
   <si>
     <t>May 29th - no chart after that?</t>
+  </si>
+  <si>
+    <t>This has coments in the chart - See how to incorporate</t>
   </si>
 </sst>
 </file>
@@ -1323,7 +1326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1350,7 +1353,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1847,7 +1849,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F186" sqref="F186"/>
+      <selection pane="bottomLeft" activeCell="F193" sqref="F193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4174,7 +4176,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="20" t="s">
+      <c r="A180" s="9" t="s">
         <v>172</v>
       </c>
       <c r="B180" s="2" t="s">
@@ -4295,7 +4297,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="11" t="s">
+      <c r="A188" s="17" t="s">
         <v>279</v>
       </c>
       <c r="B188" s="2" t="s">
@@ -4303,6 +4305,9 @@
       </c>
       <c r="C188" s="3">
         <v>43677</v>
+      </c>
+      <c r="D188" s="3">
+        <v>43725</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -4315,6 +4320,9 @@
       <c r="C189" s="3">
         <v>43643</v>
       </c>
+      <c r="D189" s="3">
+        <v>43725</v>
+      </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
@@ -4327,7 +4335,7 @@
         <v>43684</v>
       </c>
       <c r="D190" s="3">
-        <v>43715</v>
+        <v>43725</v>
       </c>
       <c r="F190" s="2" t="s">
         <v>382</v>
@@ -4354,9 +4362,15 @@
       <c r="C192" s="3">
         <v>43678</v>
       </c>
+      <c r="D192" s="3">
+        <v>43725</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="11" t="s">
+      <c r="A193" s="17" t="s">
         <v>283</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -4364,6 +4378,9 @@
       </c>
       <c r="C193" s="3">
         <v>43677</v>
+      </c>
+      <c r="D193" s="3">
+        <v>43725</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding MRK MSA MSCI MSFT MS
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE771FB3-953B-4EC0-9FBB-D362226B58ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB67FB72-C650-42EF-BD54-77FA462CC6AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="404">
   <si>
     <t>SCVL</t>
   </si>
@@ -1849,7 +1849,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F193" sqref="F193"/>
+      <selection pane="bottomLeft" activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4297,7 +4297,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="17" t="s">
+      <c r="A188" s="11" t="s">
         <v>279</v>
       </c>
       <c r="B188" s="2" t="s">
@@ -4370,7 +4370,7 @@
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="17" t="s">
+      <c r="A193" s="11" t="s">
         <v>283</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -4384,7 +4384,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="11" t="s">
+      <c r="A194" s="17" t="s">
         <v>284</v>
       </c>
       <c r="B194" s="2" t="s">
@@ -4392,6 +4392,9 @@
       </c>
       <c r="C194" s="3">
         <v>43676</v>
+      </c>
+      <c r="D194" s="3">
+        <v>43726</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -4404,6 +4407,9 @@
       <c r="C195" s="3">
         <v>43664</v>
       </c>
+      <c r="D195" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
@@ -4415,6 +4421,9 @@
       <c r="C196" s="3">
         <v>43670</v>
       </c>
+      <c r="D196" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
@@ -4426,6 +4435,9 @@
       <c r="C197" s="3">
         <v>43678</v>
       </c>
+      <c r="D197" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
@@ -4436,6 +4448,9 @@
       </c>
       <c r="C198" s="3">
         <v>43664</v>
+      </c>
+      <c r="D198" s="3">
+        <v>43726</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding MSI MSM MTB MTCH MTG MU MXIM
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB67FB72-C650-42EF-BD54-77FA462CC6AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4CBBC8-E2D5-4082-ADEF-E7C1A1468077}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="405">
   <si>
     <t>SCVL</t>
   </si>
@@ -1242,6 +1242,9 @@
   </si>
   <si>
     <t>This has coments in the chart - See how to incorporate</t>
+  </si>
+  <si>
+    <t>Ann has some comments in the chart</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1852,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D198" sqref="D198"/>
+      <selection pane="bottomLeft" activeCell="F205" sqref="F205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4384,7 +4387,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="17" t="s">
+      <c r="A194" s="11" t="s">
         <v>284</v>
       </c>
       <c r="B194" s="2" t="s">
@@ -4454,7 +4457,7 @@
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="11" t="s">
+      <c r="A199" s="17" t="s">
         <v>173</v>
       </c>
       <c r="B199" s="2" t="s">
@@ -4464,7 +4467,7 @@
         <v>43678</v>
       </c>
       <c r="D199" s="3">
-        <v>43698</v>
+        <v>43726</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -4477,6 +4480,9 @@
       <c r="C200" s="3">
         <v>43656</v>
       </c>
+      <c r="D200" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
@@ -4488,6 +4494,9 @@
       <c r="C201" s="3">
         <v>43664</v>
       </c>
+      <c r="D201" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="11" t="s">
@@ -4499,6 +4508,9 @@
       <c r="C202" s="3">
         <v>43652</v>
       </c>
+      <c r="D202" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
@@ -4510,6 +4522,9 @@
       <c r="C203" s="3">
         <v>43669</v>
       </c>
+      <c r="D203" s="3">
+        <v>43726</v>
+      </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
@@ -4521,6 +4536,12 @@
       <c r="C204" s="3">
         <v>43641</v>
       </c>
+      <c r="D204" s="3">
+        <v>43726</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="11" t="s">
@@ -4529,6 +4550,9 @@
       <c r="B205" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D205" s="3">
+        <v>43726</v>
+      </c>
       <c r="F205" s="2" t="s">
         <v>367</v>
       </c>
@@ -4542,6 +4566,9 @@
       </c>
       <c r="C206" s="3">
         <v>43676</v>
+      </c>
+      <c r="D206" s="3">
+        <v>43726</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More updates to earnings dates
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66CF187-E9CD-4317-9595-E282EB9FFD4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E4625-045B-490D-A227-3A2DE1C51A59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1841,8 +1841,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2312,6 +2312,9 @@
       <c r="B30" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C30" s="3">
+        <v>43712</v>
+      </c>
       <c r="D30" s="3">
         <v>43693</v>
       </c>
@@ -2323,6 +2326,9 @@
       <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C31" s="3">
+        <v>43720</v>
+      </c>
       <c r="D31" s="3">
         <v>43693</v>
       </c>
@@ -2344,6 +2350,9 @@
       </c>
       <c r="B33" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C33" s="3">
+        <v>43665</v>
       </c>
       <c r="D33" s="3">
         <v>43693</v>

</xml_diff>

<commit_message>
More dates updated in Mater Tracklist
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740E4625-045B-490D-A227-3A2DE1C51A59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0470677D-64E9-4CA3-8AD4-4B608BB8D44A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="408">
   <si>
     <t>SCVL</t>
   </si>
@@ -1242,13 +1242,25 @@
   </si>
   <si>
     <t>Ann has some comments in the chart</t>
+  </si>
+  <si>
+    <t>Hmm..Not seeing it now</t>
+  </si>
+  <si>
+    <t>This is an etf</t>
+  </si>
+  <si>
+    <t>ETF</t>
+  </si>
+  <si>
+    <t>Same as googl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1287,6 +1299,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1320,7 +1338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1346,6 +1364,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1840,9 +1860,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L358"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2365,6 +2385,9 @@
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C34" s="3">
+        <v>43648</v>
+      </c>
       <c r="D34" s="3">
         <v>43693</v>
       </c>
@@ -2376,6 +2399,9 @@
       <c r="B35" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C35" s="3">
+        <v>43684</v>
+      </c>
       <c r="D35" s="3">
         <v>43693</v>
       </c>
@@ -2384,6 +2410,9 @@
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="C36" s="3">
+        <v>43670</v>
+      </c>
       <c r="D36" s="3">
         <v>43694</v>
       </c>
@@ -2395,6 +2424,9 @@
       <c r="B37" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C37" s="3">
+        <v>43692</v>
+      </c>
       <c r="D37" s="3">
         <v>43694</v>
       </c>
@@ -2406,6 +2438,9 @@
       <c r="B38" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C38" s="3">
+        <v>43663</v>
+      </c>
       <c r="D38" s="3">
         <v>43694</v>
       </c>
@@ -2417,6 +2452,9 @@
       <c r="B39" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C39" s="3">
+        <v>43683</v>
+      </c>
       <c r="D39" s="3">
         <v>43694</v>
       </c>
@@ -2428,6 +2466,9 @@
       <c r="B40" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C40" s="3">
+        <v>43664</v>
+      </c>
       <c r="D40" s="3">
         <v>43694</v>
       </c>
@@ -2439,6 +2480,9 @@
       <c r="B41" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C41" s="3">
+        <v>43706</v>
+      </c>
       <c r="D41" s="3">
         <v>43694</v>
       </c>
@@ -2450,6 +2494,9 @@
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C42" s="3">
+        <v>43669</v>
+      </c>
       <c r="D42" s="3">
         <v>43694</v>
       </c>
@@ -2461,6 +2508,9 @@
       <c r="B43" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C43" s="3">
+        <v>43700</v>
+      </c>
       <c r="D43" s="3">
         <v>43694</v>
       </c>
@@ -2472,6 +2522,9 @@
       <c r="B44" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C44" s="3">
+        <v>43671</v>
+      </c>
       <c r="D44" s="3">
         <v>43694</v>
       </c>
@@ -2483,6 +2536,9 @@
       <c r="B45" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C45" s="3">
+        <v>43678</v>
+      </c>
       <c r="D45" s="3">
         <v>43694</v>
       </c>
@@ -2494,6 +2550,9 @@
       <c r="B46" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C46" s="3">
+        <v>43670</v>
+      </c>
       <c r="D46" s="3">
         <v>43694</v>
       </c>
@@ -2505,6 +2564,9 @@
       <c r="B47" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C47" s="3">
+        <v>43698</v>
+      </c>
       <c r="D47" s="3">
         <v>43694</v>
       </c>
@@ -2519,6 +2581,9 @@
       <c r="B48" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C48" s="3">
+        <v>43676</v>
+      </c>
       <c r="D48" s="3">
         <v>43703</v>
       </c>
@@ -2530,6 +2595,9 @@
       <c r="B49" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C49" s="3">
+        <v>43691</v>
+      </c>
       <c r="D49" s="3">
         <v>43703</v>
       </c>
@@ -2541,6 +2609,9 @@
       <c r="B50" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C50" s="3">
+        <v>43684</v>
+      </c>
       <c r="D50" s="3">
         <v>43703</v>
       </c>
@@ -2552,6 +2623,9 @@
       <c r="B51" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C51" s="3">
+        <v>43670</v>
+      </c>
       <c r="D51" s="3">
         <v>43703</v>
       </c>
@@ -2563,6 +2637,9 @@
       <c r="B52" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C52" s="3">
+        <v>43678</v>
+      </c>
       <c r="D52" s="3">
         <v>43703</v>
       </c>
@@ -2588,6 +2665,9 @@
       <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C54" s="3">
+        <v>43677</v>
+      </c>
       <c r="D54" s="3">
         <v>43703</v>
       </c>
@@ -2599,6 +2679,9 @@
       <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C55" s="3">
+        <v>43676</v>
+      </c>
       <c r="D55" s="3">
         <v>43703</v>
       </c>
@@ -2610,6 +2693,9 @@
       <c r="B56" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C56" s="3">
+        <v>43665</v>
+      </c>
       <c r="D56" s="3">
         <v>43703</v>
       </c>
@@ -2618,6 +2704,9 @@
       <c r="A57" s="15" t="s">
         <v>29</v>
       </c>
+      <c r="C57" s="3">
+        <v>43671</v>
+      </c>
       <c r="D57" s="3">
         <v>43703</v>
       </c>
@@ -2629,6 +2718,9 @@
       <c r="B58" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C58" s="3">
+        <v>43676</v>
+      </c>
       <c r="D58" s="3">
         <v>43703</v>
       </c>
@@ -2640,6 +2732,9 @@
       <c r="B59" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C59" s="3">
+        <v>43672</v>
+      </c>
       <c r="D59" s="3">
         <v>43712</v>
       </c>
@@ -2654,6 +2749,9 @@
       <c r="B60" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C60" s="3">
+        <v>43678</v>
+      </c>
       <c r="D60" s="3">
         <v>43705</v>
       </c>
@@ -2665,6 +2763,9 @@
       <c r="B61" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C61" s="3">
+        <v>43669</v>
+      </c>
       <c r="D61" s="3">
         <v>43705</v>
       </c>
@@ -2676,6 +2777,9 @@
       <c r="B62" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C62" s="3">
+        <v>43676</v>
+      </c>
       <c r="D62" s="3">
         <v>43705</v>
       </c>
@@ -2687,6 +2791,9 @@
       <c r="B63" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C63" s="3">
+        <v>43711</v>
+      </c>
       <c r="D63" s="3">
         <v>43705</v>
       </c>
@@ -2701,6 +2808,9 @@
       <c r="B64" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C64" s="3">
+        <v>43684</v>
+      </c>
       <c r="D64" s="3">
         <v>43705</v>
       </c>
@@ -2732,6 +2842,9 @@
       <c r="D66" s="3">
         <v>43698</v>
       </c>
+      <c r="F66" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
@@ -2740,6 +2853,9 @@
       <c r="B67" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C67" s="3">
+        <v>43662</v>
+      </c>
       <c r="D67" s="3">
         <v>43706</v>
       </c>
@@ -2751,6 +2867,9 @@
       <c r="B68" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C68" s="3">
+        <v>43713</v>
+      </c>
       <c r="D68" s="3">
         <v>43706</v>
       </c>
@@ -2762,6 +2881,9 @@
       <c r="B69" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C69" s="3">
+        <v>43699</v>
+      </c>
       <c r="D69" s="3">
         <v>43706</v>
       </c>
@@ -2776,6 +2898,9 @@
       <c r="B70" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C70" s="3">
+        <v>43678</v>
+      </c>
       <c r="D70" s="3">
         <v>43706</v>
       </c>
@@ -2787,6 +2912,9 @@
       <c r="B71" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C71" s="3">
+        <v>43676</v>
+      </c>
       <c r="D71" s="3">
         <v>43706</v>
       </c>
@@ -2801,6 +2929,9 @@
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C72" s="3">
+        <v>43691</v>
+      </c>
       <c r="D72" s="3">
         <v>43706</v>
       </c>
@@ -2812,6 +2943,9 @@
       <c r="B73" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C73" s="3">
+        <v>43669</v>
+      </c>
       <c r="D73" s="3">
         <v>43706</v>
       </c>
@@ -2823,6 +2957,9 @@
       <c r="B74" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C74" s="3">
+        <v>43669</v>
+      </c>
       <c r="D74" s="3">
         <v>43698</v>
       </c>
@@ -2834,6 +2971,9 @@
       <c r="B75" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C75" s="3">
+        <v>43662</v>
+      </c>
       <c r="D75" s="3">
         <v>43713</v>
       </c>
@@ -2845,6 +2985,9 @@
       <c r="B76" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C76" s="3">
+        <v>43662</v>
+      </c>
       <c r="D76" s="3">
         <v>43713</v>
       </c>
@@ -2856,6 +2999,9 @@
       <c r="B77" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C77" s="3">
+        <v>43670</v>
+      </c>
       <c r="D77" s="3">
         <v>43713</v>
       </c>
@@ -2864,6 +3010,9 @@
       <c r="A78" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="C78" s="3">
+        <v>43670</v>
+      </c>
       <c r="D78" s="3">
         <v>43713</v>
       </c>
@@ -2875,6 +3024,9 @@
       <c r="B79" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C79" s="3">
+        <v>43671</v>
+      </c>
       <c r="F79" s="2" t="s">
         <v>372</v>
       </c>
@@ -2903,6 +3055,9 @@
       <c r="B81" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C81" s="3">
+        <v>43697</v>
+      </c>
       <c r="D81" s="3">
         <v>43714</v>
       </c>
@@ -2914,6 +3069,9 @@
       <c r="B82" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C82" s="3">
+        <v>43498</v>
+      </c>
       <c r="D82" s="3">
         <v>43714</v>
       </c>
@@ -2925,6 +3083,9 @@
       <c r="B83" s="2" t="s">
         <v>366</v>
       </c>
+      <c r="C83" s="3">
+        <v>43693</v>
+      </c>
       <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -2934,6 +3095,9 @@
       <c r="B84" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C84" s="3">
+        <v>43671</v>
+      </c>
       <c r="D84" s="3">
         <v>43714</v>
       </c>
@@ -2945,6 +3109,9 @@
       <c r="B85" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C85" s="3">
+        <v>43669</v>
+      </c>
       <c r="D85" s="3">
         <v>43714</v>
       </c>
@@ -2956,6 +3123,9 @@
       <c r="B86" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C86" s="3">
+        <v>43706</v>
+      </c>
       <c r="D86" s="3">
         <v>43714</v>
       </c>
@@ -2967,6 +3137,9 @@
       <c r="B87" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C87" s="3">
+        <v>43676</v>
+      </c>
       <c r="D87" s="3">
         <v>43714</v>
       </c>
@@ -2981,6 +3154,9 @@
       <c r="B88" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C88" s="3">
+        <v>43683</v>
+      </c>
       <c r="D88" s="3">
         <v>43714</v>
       </c>
@@ -2992,6 +3168,9 @@
       <c r="B89" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C89" s="3">
+        <v>43678</v>
+      </c>
       <c r="D89" s="3">
         <v>43714</v>
       </c>
@@ -3003,6 +3182,9 @@
       <c r="B90" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C90" s="3">
+        <v>43662</v>
+      </c>
       <c r="D90" s="3">
         <v>43714</v>
       </c>
@@ -3019,7 +3201,7 @@
         <v>11</v>
       </c>
       <c r="C91" s="3">
-        <v>43636</v>
+        <v>43727</v>
       </c>
       <c r="D91" s="3">
         <v>43716</v>
@@ -3073,7 +3255,7 @@
       <c r="L94" s="11"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="16" t="s">
         <v>233</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -3277,6 +3459,9 @@
       <c r="B108" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C108" s="3">
+        <v>43566</v>
+      </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
@@ -3342,7 +3527,10 @@
         <v>167</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>11</v>
+        <v>406</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3383,6 +3571,9 @@
       <c r="B116" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C116" s="3">
+        <v>43671</v>
+      </c>
       <c r="D116" s="3">
         <v>43714</v>
       </c>
@@ -3439,11 +3630,14 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="11" t="s">
+      <c r="A120" s="16" t="s">
         <v>244</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3484,6 +3678,9 @@
       <c r="B123" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C123" s="3">
+        <v>43488</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
@@ -3528,13 +3725,16 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C127" s="3"/>
+      <c r="F127" s="2" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
@@ -3747,7 +3947,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="11" t="s">
+      <c r="A143" s="16" t="s">
         <v>257</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -4021,7 +4221,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="11" t="s">
+      <c r="A163" s="20" t="s">
         <v>267</v>
       </c>
       <c r="F163" s="2" t="s">
@@ -4029,7 +4229,7 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="11" t="s">
+      <c r="A164" s="20" t="s">
         <v>268</v>
       </c>
       <c r="F164" s="2" t="s">
@@ -4205,7 +4405,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="11" t="s">
+      <c r="A177" s="16" t="s">
         <v>273</v>
       </c>
       <c r="B177" s="2" t="s">
@@ -4410,7 +4610,7 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A191" s="11" t="s">
+      <c r="A191" s="16" t="s">
         <v>281</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -4609,7 +4809,7 @@
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="11" t="s">
+      <c r="A205" s="16" t="s">
         <v>288</v>
       </c>
       <c r="B205" s="2" t="s">

</xml_diff>

<commit_message>
NANO NATI NCLH NDAQ NFLX NMIH NSC NSP NSSC NTAP NUE NVR NXPI
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC37FF00-036E-43C5-9560-3D79564AB2CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96588F0-8F77-4E81-9B59-6B2DDA9BAA0E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="300" windowWidth="11550" windowHeight="16485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$361</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="410">
   <si>
     <t>SCVL</t>
   </si>
@@ -1254,6 +1255,12 @@
   </si>
   <si>
     <t>Same as googl</t>
+  </si>
+  <si>
+    <t>etf</t>
+  </si>
+  <si>
+    <t>Look promising</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1325,6 +1332,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1338,7 +1351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1376,6 +1389,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1871,8 +1887,8 @@
   <dimension ref="A1:L358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C239" sqref="C239"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F215" sqref="F215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4856,6 +4872,9 @@
       <c r="C207" s="24">
         <v>43676</v>
       </c>
+      <c r="D207" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
@@ -4867,6 +4886,9 @@
       <c r="C208" s="24">
         <v>43676</v>
       </c>
+      <c r="D208" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
@@ -4879,7 +4901,7 @@
         <v>43685</v>
       </c>
       <c r="D209" s="24">
-        <v>43715</v>
+        <v>43728</v>
       </c>
       <c r="F209" s="2" t="s">
         <v>383</v>
@@ -4895,6 +4917,9 @@
       <c r="C210" s="24">
         <v>43670</v>
       </c>
+      <c r="D210" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
@@ -4906,9 +4931,12 @@
       <c r="C211" s="24">
         <v>43663</v>
       </c>
+      <c r="D211" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
+      <c r="A212" s="15" t="s">
         <v>142</v>
       </c>
       <c r="B212" s="2" t="s">
@@ -4918,7 +4946,7 @@
         <v>43677</v>
       </c>
       <c r="D212" s="24">
-        <v>43715</v>
+        <v>43728</v>
       </c>
       <c r="F212" s="2" t="s">
         <v>381</v>
@@ -4928,7 +4956,7 @@
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
+      <c r="A213" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B213" s="2" t="s">
@@ -4936,6 +4964,9 @@
       </c>
       <c r="C213" s="24">
         <v>43670</v>
+      </c>
+      <c r="D213" s="24">
+        <v>43728</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -4948,6 +4979,12 @@
       <c r="C214" s="24">
         <v>43675</v>
       </c>
+      <c r="D214" s="24">
+        <v>43728</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="11" t="s">
@@ -4959,6 +4996,9 @@
       <c r="C215" s="24">
         <v>43711</v>
       </c>
+      <c r="D215" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="11" t="s">
@@ -4970,6 +5010,9 @@
       <c r="C216" s="24">
         <v>43691</v>
       </c>
+      <c r="D216" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
@@ -4981,6 +5024,9 @@
       <c r="C217" s="24">
         <v>43664</v>
       </c>
+      <c r="D217" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
@@ -4992,9 +5038,12 @@
       <c r="C218" s="24">
         <v>43668</v>
       </c>
+      <c r="D218" s="24">
+        <v>43728</v>
+      </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A219" s="11" t="s">
+      <c r="A219" s="26" t="s">
         <v>295</v>
       </c>
       <c r="B219" s="2" t="s">
@@ -5002,6 +5051,9 @@
       </c>
       <c r="C219" s="24">
         <v>43675</v>
+      </c>
+      <c r="D219" s="24">
+        <v>43728</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -5233,6 +5285,9 @@
       <c r="B241" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C241" s="24">
+        <v>43669</v>
+      </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
@@ -5241,6 +5296,9 @@
       <c r="B242" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C242" s="24">
+        <v>43672</v>
+      </c>
       <c r="D242" s="24">
         <v>43712</v>
       </c>
@@ -5258,9 +5316,12 @@
       <c r="B243" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C243" s="24">
+        <v>43670</v>
+      </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="11" t="s">
+      <c r="A244" s="16" t="s">
         <v>306</v>
       </c>
       <c r="B244" s="2" t="s">
@@ -5292,7 +5353,7 @@
         <v>178</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>11</v>
+        <v>408</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -5302,6 +5363,9 @@
       <c r="B247" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C247" s="24">
+        <v>43679</v>
+      </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
@@ -5310,9 +5374,12 @@
       <c r="B248" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C248" s="24">
+        <v>43670</v>
+      </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" s="11" t="s">
+      <c r="A249" s="16" t="s">
         <v>308</v>
       </c>
       <c r="B249" s="2" t="s">
@@ -5326,9 +5393,12 @@
       <c r="B250" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C250" s="24">
+        <v>43677</v>
+      </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A251" s="11" t="s">
+      <c r="A251" s="16" t="s">
         <v>310</v>
       </c>
       <c r="B251" s="2" t="s">
@@ -5362,6 +5432,9 @@
       <c r="B253" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C253" s="24">
+        <v>43665</v>
+      </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="11" t="s">
@@ -5370,6 +5443,9 @@
       <c r="B254" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C254" s="24">
+        <v>43719</v>
+      </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="11" t="s">
@@ -5378,6 +5454,9 @@
       <c r="B255" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C255" s="24">
+        <v>43683</v>
+      </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
@@ -5386,6 +5465,9 @@
       <c r="B256" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C256" s="24">
+        <v>43670</v>
+      </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
@@ -5394,6 +5476,9 @@
       <c r="B257" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C257" s="24">
+        <v>43306</v>
+      </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
@@ -5402,6 +5487,9 @@
       <c r="B258" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C258" s="24">
+        <v>43671</v>
+      </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
@@ -5410,6 +5498,9 @@
       <c r="B259" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C259" s="24">
+        <v>43671</v>
+      </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="9" t="s">
@@ -5418,6 +5509,9 @@
       <c r="B260" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C260" s="24">
+        <v>43699</v>
+      </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="11" t="s">
@@ -5426,6 +5520,9 @@
       <c r="B261" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C261" s="24">
+        <v>43678</v>
+      </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
@@ -5434,6 +5531,9 @@
       <c r="B262" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C262" s="24">
+        <v>43671</v>
+      </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
@@ -5442,6 +5542,9 @@
       <c r="B263" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C263" s="24">
+        <v>43670</v>
+      </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
@@ -5450,6 +5553,9 @@
       <c r="B264" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C264" s="24">
+        <v>43664</v>
+      </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
@@ -5458,6 +5564,9 @@
       <c r="B265" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C265" s="24">
+        <v>43671</v>
+      </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="11" t="s">
@@ -5466,6 +5575,9 @@
       <c r="B266" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C266" s="24">
+        <v>43674</v>
+      </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
@@ -5474,6 +5586,9 @@
       <c r="B267" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C267" s="24">
+        <v>43663</v>
+      </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
@@ -5482,6 +5597,9 @@
       <c r="B268" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C268" s="24">
+        <v>43705</v>
+      </c>
       <c r="F268" s="2" t="s">
         <v>2</v>
       </c>
@@ -5493,6 +5611,9 @@
       <c r="B269" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C269" s="24">
+        <v>43676</v>
+      </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
@@ -5501,6 +5622,9 @@
       <c r="B270" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C270" s="24">
+        <v>43671</v>
+      </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="11" t="s">
@@ -5509,6 +5633,9 @@
       <c r="B271" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C271" s="24">
+        <v>43677</v>
+      </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="9" t="s">
@@ -5517,255 +5644,348 @@
       <c r="B272" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C272" s="24">
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C273" s="24">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C274" s="24">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="11" t="s">
         <v>319</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C275" s="24">
+        <v>43699</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
         <v>320</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C276" s="24">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
         <v>321</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="2" t="s">
+      <c r="C277" s="24">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B279" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C279" s="24">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="9" t="s">
         <v>322</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C280" s="24">
+        <v>43679</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="11" t="s">
         <v>323</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C281" s="24">
+        <v>43674</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C282" s="24">
+        <v>43669</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C283" s="24">
+        <v>43665</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="11" t="s">
         <v>324</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="11" t="s">
+      <c r="C284" s="24">
+        <v>43689</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="16" t="s">
         <v>325</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C286" s="24">
+        <v>43663</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="9" t="s">
         <v>326</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C287" s="24">
+        <v>43683</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C288" s="24">
+        <v>43669</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C289" s="24">
+        <v>43668</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C290" s="24">
+        <v>43697</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
         <v>328</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="11" t="s">
+      <c r="C291" s="24">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="16" t="s">
         <v>329</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="10" t="s">
         <v>330</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C293" s="24">
+        <v>43503</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="11" t="s">
         <v>331</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C294" s="24">
+        <v>43697</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C295" s="24">
+        <v>43670</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C296" s="24">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C297" s="24">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="11" t="s">
         <v>332</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C298" s="24">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
         <v>333</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C299" s="24">
+        <v>43685</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
         <v>334</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C300" s="24">
+        <v>43699</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
         <v>335</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C301" s="24">
+        <v>43685</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
         <v>336</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C302" s="24">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
         <v>337</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C303" s="24">
+        <v>43478</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="9" t="s">
         <v>338</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C304" s="24">
+        <v>43686</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
@@ -5775,6 +5995,9 @@
       <c r="B305" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C305" s="24">
+        <v>43672</v>
+      </c>
       <c r="D305" s="24">
         <v>43712</v>
       </c>
@@ -5786,6 +6009,12 @@
       <c r="A306" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="B306" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C306" s="24">
+        <v>43639</v>
+      </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
@@ -5794,6 +6023,9 @@
       <c r="B307" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C307" s="24">
+        <v>43663</v>
+      </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
@@ -5802,6 +6034,9 @@
       <c r="B308" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C308" s="24">
+        <v>43663</v>
+      </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="9" t="s">
@@ -5810,6 +6045,9 @@
       <c r="B309" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C309" s="24">
+        <v>43504</v>
+      </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="9" t="s">
@@ -5818,6 +6056,9 @@
       <c r="B310" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C310" s="24">
+        <v>43685</v>
+      </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="11" t="s">
@@ -5826,6 +6067,9 @@
       <c r="B311" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C311" s="24">
+        <v>43706</v>
+      </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
@@ -5834,6 +6078,9 @@
       <c r="B312" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C312" s="24">
+        <v>43664</v>
+      </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
@@ -5842,6 +6089,9 @@
       <c r="B313" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C313" s="24">
+        <v>43664</v>
+      </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
@@ -5850,11 +6100,20 @@
       <c r="B314" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C314" s="24">
+        <v>43663</v>
+      </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="B315" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C315" s="24">
+        <v>43669</v>
+      </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="11" t="s">
@@ -5863,6 +6122,9 @@
       <c r="B316" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C316" s="24">
+        <v>43677</v>
+      </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
@@ -5871,6 +6133,9 @@
       <c r="B317" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C317" s="24">
+        <v>43669</v>
+      </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="11" t="s">
@@ -5879,6 +6144,9 @@
       <c r="B318" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C318" s="24">
+        <v>43704</v>
+      </c>
       <c r="D318" s="24">
         <v>43698</v>
       </c>
@@ -5887,135 +6155,195 @@
       <c r="A319" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="B319" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C319" s="24">
+        <v>43670</v>
+      </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B320" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C320" s="24">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C321" s="24">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="11" t="s">
         <v>342</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C322" s="24">
+        <v>43699</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
         <v>343</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C323" s="24">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="11" t="s">
         <v>344</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C324" s="24">
+        <v>43677</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="11" t="s">
         <v>345</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C325" s="24">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C326" s="24">
+        <v>43664</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
         <v>346</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C327" s="24">
+        <v>43697</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="11" t="s">
         <v>347</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C328" s="24">
+        <v>43675</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="11" t="s">
         <v>348</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C329" s="24">
+        <v>43635</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C330" s="24">
+        <v>43668</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="11" t="s">
         <v>349</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" s="9" t="s">
+      <c r="C331" s="24">
+        <v>43685</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" s="25" t="s">
         <v>350</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B333" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C333" s="24">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="12" t="s">
         <v>351</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C334" s="24">
+        <v>43676</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
         <v>352</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C335" s="24">
+        <v>43683</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
         <v>353</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C336" s="24">
+        <v>43676</v>
       </c>
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.25">
@@ -6025,6 +6353,9 @@
       <c r="B337" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C337" s="24">
+        <v>43602</v>
+      </c>
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
@@ -6033,6 +6364,9 @@
       <c r="B338" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C338" s="24">
+        <v>43683</v>
+      </c>
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="11" t="s">
@@ -6040,6 +6374,9 @@
       </c>
       <c r="B339" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C339" s="24">
+        <v>43713</v>
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating charts to current date
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96588F0-8F77-4E81-9B59-6B2DDA9BAA0E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179844E6-8246-43F8-98C6-CCE254ED7DFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$361</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="409">
   <si>
     <t>SCVL</t>
   </si>
@@ -1110,18 +1109,9 @@
     <t>Seems like a nice growth ahead - Ann's adjusted analyst lines are flatter than the actual analysts. Understand why</t>
   </si>
   <si>
-    <t>One stock that reports whose fiscal is Oct-Oct. Use this as an experiment case</t>
-  </si>
-  <si>
     <t xml:space="preserve">This does not plot correctly with xtick and xticklabels on…not sure what is wrong though. If plotted without labels, it plots correctly </t>
   </si>
   <si>
-    <t>Ann does not have this chart???</t>
-  </si>
-  <si>
-    <t>Not found???</t>
-  </si>
-  <si>
     <t>This one looks good</t>
   </si>
   <si>
@@ -1137,9 +1127,6 @@
     <t>Not found</t>
   </si>
   <si>
-    <t>Problem with the diamonds not matching with pink dots…Oct quarter….Need to figure out what is wroing</t>
-  </si>
-  <si>
     <t>Problem with the diamonds not matching with pink dots…Dec quarter….Need to figure out what is wroing</t>
   </si>
   <si>
@@ -1261,6 +1248,15 @@
   </si>
   <si>
     <t>Look promising</t>
+  </si>
+  <si>
+    <t>Foreign</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Price runs up too far of earnings - Can discuss</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1332,12 +1328,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1351,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1390,8 +1380,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1884,11 +1872,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L358"/>
+  <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F215" sqref="F215"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1899,10 +1887,11 @@
     <col min="5" max="5" width="12" style="2" customWidth="1"/>
     <col min="6" max="6" width="98.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="139.85546875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="14" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1910,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>5</v>
@@ -1922,19 +1911,22 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>181</v>
       </c>
@@ -1942,7 +1934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1956,10 +1948,10 @@
         <v>43715</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>159</v>
       </c>
@@ -1973,7 +1965,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1987,7 +1979,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2001,7 +1993,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>182</v>
       </c>
@@ -2015,13 +2007,13 @@
         <v>43715</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>183</v>
       </c>
@@ -2032,13 +2024,13 @@
         <v>43725</v>
       </c>
       <c r="D8" s="24">
-        <v>43690</v>
+        <v>43729</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>184</v>
       </c>
@@ -2049,13 +2041,10 @@
         <v>43698</v>
       </c>
       <c r="D9" s="24">
-        <v>43690</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>185</v>
       </c>
@@ -2069,7 +2058,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>160</v>
       </c>
@@ -2083,7 +2072,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>186</v>
       </c>
@@ -2097,7 +2086,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
@@ -2111,7 +2100,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>187</v>
       </c>
@@ -2125,10 +2114,10 @@
         <v>43690</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>188</v>
       </c>
@@ -2142,7 +2131,7 @@
         <v>43690</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>189</v>
       </c>
@@ -2153,7 +2142,7 @@
         <v>43692</v>
       </c>
       <c r="D16" s="24">
-        <v>43690</v>
+        <v>43728</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2199,7 +2188,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2227,10 +2216,7 @@
         <v>43706</v>
       </c>
       <c r="D21" s="24">
-        <v>43691</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>361</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2272,7 +2258,7 @@
         <v>43693</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2303,7 +2289,7 @@
         <v>43693</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,9 +2333,6 @@
       <c r="D29" s="24">
         <v>43693</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>362</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
@@ -2362,7 +2345,7 @@
         <v>43712</v>
       </c>
       <c r="D30" s="24">
-        <v>43693</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,21 +2359,21 @@
         <v>43720</v>
       </c>
       <c r="D31" s="24">
-        <v>43693</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D32" s="24">
         <v>43698</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>100</v>
       </c>
@@ -2404,7 +2387,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>200</v>
       </c>
@@ -2418,7 +2401,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>201</v>
       </c>
@@ -2432,7 +2415,7 @@
         <v>43693</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -2443,7 +2426,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>162</v>
       </c>
@@ -2457,7 +2440,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>124</v>
       </c>
@@ -2471,7 +2454,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>202</v>
       </c>
@@ -2485,7 +2468,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
@@ -2499,7 +2482,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>203</v>
       </c>
@@ -2510,10 +2493,10 @@
         <v>43706</v>
       </c>
       <c r="D41" s="24">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43729</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>90</v>
       </c>
@@ -2527,7 +2510,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>204</v>
       </c>
@@ -2541,7 +2524,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>30</v>
       </c>
@@ -2555,7 +2538,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>205</v>
       </c>
@@ -2569,7 +2552,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>71</v>
       </c>
@@ -2583,7 +2566,7 @@
         <v>43694</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>206</v>
       </c>
@@ -2594,13 +2577,16 @@
         <v>43698</v>
       </c>
       <c r="D47" s="24">
-        <v>43694</v>
+        <v>43729</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>207</v>
       </c>
@@ -2681,7 +2667,7 @@
         <v>43703</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2765,7 +2751,7 @@
         <v>43712</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2821,10 +2807,7 @@
         <v>43711</v>
       </c>
       <c r="D63" s="24">
-        <v>43705</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>368</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2855,7 +2838,7 @@
         <v>43715</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2869,7 +2852,7 @@
         <v>43698</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2897,7 +2880,10 @@
         <v>43713</v>
       </c>
       <c r="D68" s="24">
-        <v>43706</v>
+        <v>43729</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2914,7 +2900,7 @@
         <v>43706</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2945,7 +2931,7 @@
         <v>43706</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3054,7 +3040,7 @@
         <v>43671</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3074,7 +3060,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>222</v>
       </c>
@@ -3088,7 +3074,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>223</v>
       </c>
@@ -3102,19 +3088,19 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>224</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C83" s="24">
         <v>43693</v>
       </c>
       <c r="D83" s="24"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>22</v>
       </c>
@@ -3128,7 +3114,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>75</v>
       </c>
@@ -3142,7 +3128,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>225</v>
       </c>
@@ -3156,7 +3142,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>226</v>
       </c>
@@ -3170,10 +3156,10 @@
         <v>43714</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>227</v>
       </c>
@@ -3187,7 +3173,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>228</v>
       </c>
@@ -3201,7 +3187,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>133</v>
       </c>
@@ -3215,11 +3201,11 @@
         <v>43714</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="L90" s="11"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+      <c r="M90" s="11"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>229</v>
       </c>
@@ -3230,11 +3216,11 @@
         <v>43727</v>
       </c>
       <c r="D91" s="24">
-        <v>43716</v>
-      </c>
-      <c r="L91" s="9"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <v>43729</v>
+      </c>
+      <c r="M91" s="9"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>230</v>
       </c>
@@ -3248,7 +3234,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>231</v>
       </c>
@@ -3262,10 +3248,10 @@
         <v>43716</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>232</v>
       </c>
@@ -3278,9 +3264,9 @@
       <c r="D94" s="24">
         <v>43716</v>
       </c>
-      <c r="L94" s="11"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M94" s="11"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
         <v>233</v>
       </c>
@@ -3288,10 +3274,10 @@
         <v>11</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>149</v>
       </c>
@@ -3305,7 +3291,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>234</v>
       </c>
@@ -3319,11 +3305,11 @@
         <v>43716</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="L97" s="7"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+      <c r="M97" s="7"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>235</v>
       </c>
@@ -3337,7 +3323,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>236</v>
       </c>
@@ -3350,9 +3336,9 @@
       <c r="D99" s="24">
         <v>43716</v>
       </c>
-      <c r="L99" s="11"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M99" s="11"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>150</v>
       </c>
@@ -3366,10 +3352,10 @@
         <v>43715</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>237</v>
       </c>
@@ -3383,11 +3369,11 @@
         <v>43716</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="L101" s="9"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="M101" s="9"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>103</v>
       </c>
@@ -3400,9 +3386,9 @@
       <c r="D102" s="24">
         <v>43716</v>
       </c>
-      <c r="L102" s="11"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M102" s="11"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>73</v>
       </c>
@@ -3416,11 +3402,11 @@
         <v>43716</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="L103" s="11"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="M103" s="11"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>76</v>
       </c>
@@ -3433,9 +3419,9 @@
       <c r="D104" s="24">
         <v>43716</v>
       </c>
-      <c r="L104" s="11"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M104" s="11"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
         <v>238</v>
       </c>
@@ -3448,9 +3434,9 @@
       <c r="D105" s="24">
         <v>43716</v>
       </c>
-      <c r="L105" s="11"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M105" s="11"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>39</v>
       </c>
@@ -3464,7 +3450,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>239</v>
       </c>
@@ -3478,7 +3464,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>240</v>
       </c>
@@ -3489,7 +3475,7 @@
         <v>43566</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>55</v>
       </c>
@@ -3503,7 +3489,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>64</v>
       </c>
@@ -3517,7 +3503,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>166</v>
       </c>
@@ -3531,7 +3517,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>60</v>
       </c>
@@ -3545,7 +3531,7 @@
         <v>43717</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3553,10 +3539,10 @@
         <v>167</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3573,7 +3559,7 @@
         <v>43717</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3604,7 +3590,7 @@
         <v>43714</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>138</v>
@@ -3652,7 +3638,7 @@
         <v>43718</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3663,7 +3649,7 @@
         <v>11</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3694,7 +3680,7 @@
         <v>43718</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3759,7 +3745,7 @@
       </c>
       <c r="C127" s="24"/>
       <c r="F127" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3776,7 +3762,7 @@
         <v>43718</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4047,7 +4033,7 @@
         <v>43723</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -4103,7 +4089,7 @@
         <v>43723</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4120,7 +4106,7 @@
         <v>43723</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4201,7 +4187,7 @@
         <v>264</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4251,7 +4237,7 @@
         <v>267</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4259,7 +4245,7 @@
         <v>268</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4413,7 +4399,7 @@
         <v>43724</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4438,7 +4424,7 @@
         <v>11</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -4567,7 +4553,7 @@
         <v>43714</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -4584,7 +4570,7 @@
         <v>43714</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="G187" s="2" t="s">
         <v>141</v>
@@ -4632,7 +4618,7 @@
         <v>43725</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -4643,7 +4629,7 @@
         <v>11</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -4660,7 +4646,7 @@
         <v>43725</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -4831,7 +4817,7 @@
         <v>43726</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -4845,7 +4831,7 @@
         <v>43726</v>
       </c>
       <c r="F205" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -4904,7 +4890,7 @@
         <v>43728</v>
       </c>
       <c r="F209" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -4949,14 +4935,14 @@
         <v>43728</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G212" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A213" s="27" t="s">
+      <c r="A213" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B213" s="2" t="s">
@@ -4983,7 +4969,7 @@
         <v>43728</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -5043,7 +5029,7 @@
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A219" s="26" t="s">
+      <c r="A219" s="11" t="s">
         <v>295</v>
       </c>
       <c r="B219" s="2" t="s">
@@ -5303,7 +5289,7 @@
         <v>43712</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G242" s="2" t="s">
         <v>135</v>
@@ -5342,7 +5328,7 @@
         <v>43715</v>
       </c>
       <c r="F245" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G245" s="2" t="s">
         <v>145</v>
@@ -5353,7 +5339,7 @@
         <v>178</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -5419,7 +5405,7 @@
         <v>43715</v>
       </c>
       <c r="F252" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G252" s="2" t="s">
         <v>158</v>
@@ -6002,7 +5988,7 @@
         <v>43712</v>
       </c>
       <c r="F305" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
@@ -6148,7 +6134,7 @@
         <v>43704</v>
       </c>
       <c r="D318" s="24">
-        <v>43698</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
@@ -6346,7 +6332,7 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" s="11" t="s">
         <v>354</v>
       </c>
@@ -6357,7 +6343,7 @@
         <v>43602</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
         <v>355</v>
       </c>
@@ -6368,7 +6354,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" s="11" t="s">
         <v>356</v>
       </c>
@@ -6379,63 +6365,63 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H341" s="8"/>
-    </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H342" s="8"/>
-    </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H343" s="8"/>
-    </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H344" s="8"/>
-    </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H345" s="8"/>
-    </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H346" s="8"/>
-    </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H347" s="8"/>
-    </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H348" s="8"/>
-    </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H349" s="8"/>
-    </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H350" s="8"/>
-    </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H351" s="8"/>
-    </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H352" s="8"/>
-    </row>
-    <row r="353" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H353" s="8"/>
-    </row>
-    <row r="354" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H354" s="8"/>
-    </row>
-    <row r="355" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H355" s="8"/>
-    </row>
-    <row r="356" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H356" s="8"/>
-    </row>
-    <row r="357" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H357" s="8"/>
-    </row>
-    <row r="358" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H358" s="8"/>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I341" s="8"/>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I342" s="8"/>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I343" s="8"/>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I344" s="8"/>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I345" s="8"/>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I346" s="8"/>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I347" s="8"/>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I348" s="8"/>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I349" s="8"/>
+    </row>
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I350" s="8"/>
+    </row>
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I351" s="8"/>
+    </row>
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I352" s="8"/>
+    </row>
+    <row r="353" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I353" s="8"/>
+    </row>
+    <row r="354" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I354" s="8"/>
+    </row>
+    <row r="355" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I355" s="8"/>
+    </row>
+    <row r="356" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I356" s="8"/>
+    </row>
+    <row r="357" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I357" s="8"/>
+    </row>
+    <row r="358" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I358" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A361" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L358">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M358">
     <sortCondition ref="A2:A358"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
@@ -6444,31 +6430,31 @@
   <conditionalFormatting sqref="A142:A339">
     <cfRule type="duplicateValues" dxfId="19" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H341:H343">
+  <conditionalFormatting sqref="I341:I343">
     <cfRule type="duplicateValues" dxfId="18" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H344">
+  <conditionalFormatting sqref="I344">
     <cfRule type="duplicateValues" dxfId="17" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H345:H347">
+  <conditionalFormatting sqref="I345:I347">
     <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H346:H347">
+  <conditionalFormatting sqref="I346:I347">
     <cfRule type="duplicateValues" dxfId="15" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H346:H347">
+  <conditionalFormatting sqref="I346:I347">
     <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H348:H358">
+  <conditionalFormatting sqref="I348:I358">
     <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H348:H358">
+  <conditionalFormatting sqref="I348:I358">
     <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L105:L119">
+  <conditionalFormatting sqref="M105:M119">
     <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding OKE OLED OLLI ORLY
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179844E6-8246-43F8-98C6-CCE254ED7DFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC4D218-2B79-4FD1-BF02-96C6C50E7A13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1309,7 +1309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1328,6 +1328,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1341,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1380,6 +1386,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1875,8 +1883,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F222" sqref="F222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2339,7 @@
         <v>43697</v>
       </c>
       <c r="D29" s="24">
-        <v>43693</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2521,7 +2529,7 @@
         <v>43700</v>
       </c>
       <c r="D43" s="24">
-        <v>43694</v>
+        <v>43729</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -5043,7 +5051,7 @@
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="11" t="s">
+      <c r="A220" s="27" t="s">
         <v>296</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -5051,6 +5059,9 @@
       </c>
       <c r="C220" s="24">
         <v>43676</v>
+      </c>
+      <c r="D220" s="24">
+        <v>43729</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -5063,6 +5074,9 @@
       <c r="C221" s="24">
         <v>43678</v>
       </c>
+      <c r="D221" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="11" t="s">
@@ -5074,9 +5088,12 @@
       <c r="C222" s="24">
         <v>43705</v>
       </c>
+      <c r="D222" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
+      <c r="A223" s="26" t="s">
         <v>51</v>
       </c>
       <c r="B223" s="2" t="s">
@@ -5084,6 +5101,9 @@
       </c>
       <c r="C223" s="24">
         <v>43670</v>
+      </c>
+      <c r="D223" s="24">
+        <v>43729</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -5463,7 +5483,7 @@
         <v>11</v>
       </c>
       <c r="C257" s="24">
-        <v>43306</v>
+        <v>43671</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
@@ -5999,7 +6019,7 @@
         <v>11</v>
       </c>
       <c r="C306" s="24">
-        <v>43639</v>
+        <v>43669</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding PAYC PCAR PFE PFGC PGR PGTI PH PHM
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC4D218-2B79-4FD1-BF02-96C6C50E7A13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3799F926-B01A-4270-9909-D336D1929BF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="410">
   <si>
     <t>SCVL</t>
   </si>
@@ -1257,6 +1257,9 @@
   </si>
   <si>
     <t>Price runs up too far of earnings - Can discuss</t>
+  </si>
+  <si>
+    <t>CNBC does not have next year projections -- maybe temporary not available</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1386,7 +1389,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1883,8 +1885,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F222" sqref="F222"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F217" sqref="F217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5051,7 +5053,7 @@
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A220" s="27" t="s">
+      <c r="A220" s="11" t="s">
         <v>296</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -5093,7 +5095,7 @@
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="26" t="s">
+      <c r="A223" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B223" s="2" t="s">
@@ -5116,6 +5118,9 @@
       <c r="C224" s="24">
         <v>43676</v>
       </c>
+      <c r="D224" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
@@ -5127,6 +5132,9 @@
       <c r="C225" s="24">
         <v>43669</v>
       </c>
+      <c r="D225" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="19" t="s">
@@ -5143,6 +5151,12 @@
       <c r="C227" s="24">
         <v>43676</v>
       </c>
+      <c r="D227" s="24">
+        <v>43729</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="11" t="s">
@@ -5154,6 +5168,9 @@
       <c r="C228" s="24">
         <v>43691</v>
       </c>
+      <c r="D228" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
@@ -5166,7 +5183,7 @@
         <v>43673</v>
       </c>
       <c r="D229" s="24">
-        <v>43714</v>
+        <v>43729</v>
       </c>
       <c r="F229" s="2" t="s">
         <v>137</v>
@@ -5182,6 +5199,9 @@
       <c r="C230" s="24">
         <v>43678</v>
       </c>
+      <c r="D230" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="9" t="s">
@@ -5193,6 +5213,9 @@
       <c r="C231" s="24">
         <v>43678</v>
       </c>
+      <c r="D231" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
@@ -5204,6 +5227,9 @@
       <c r="C232" s="24">
         <v>43669</v>
       </c>
+      <c r="D232" s="24">
+        <v>43729</v>
+      </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="19" t="s">
@@ -5211,7 +5237,7 @@
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="11" t="s">
+      <c r="A234" s="26" t="s">
         <v>303</v>
       </c>
       <c r="B234" s="2" t="s">

</xml_diff>

<commit_message>
Adding PLD PLNT POOL PRLB PRU PSB PSXP PYPL
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3799F926-B01A-4270-9909-D336D1929BF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F5968-7538-4176-9FC4-5952611D7EC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="412">
   <si>
     <t>SCVL</t>
   </si>
@@ -1260,6 +1260,12 @@
   </si>
   <si>
     <t>CNBC does not have next year projections -- maybe temporary not available</t>
+  </si>
+  <si>
+    <t>Need latest</t>
+  </si>
+  <si>
+    <t>CNBC does not have next year projections -- maybe temporary not available - Is Ann doing something different</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1331,12 +1337,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1350,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1389,7 +1389,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1886,7 +1885,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F217" sqref="F217"/>
+      <selection pane="bottomLeft" activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5237,7 +5236,7 @@
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="26" t="s">
+      <c r="A234" s="11" t="s">
         <v>303</v>
       </c>
       <c r="B234" s="2" t="s">
@@ -5245,6 +5244,9 @@
       </c>
       <c r="C234" s="24">
         <v>43662</v>
+      </c>
+      <c r="D234" s="24">
+        <v>43730</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -5258,11 +5260,11 @@
         <v>43684</v>
       </c>
       <c r="D235" s="24">
-        <v>43698</v>
+        <v>43730</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="11" t="s">
+      <c r="A236" s="16" t="s">
         <v>304</v>
       </c>
       <c r="B236" s="2" t="s">
@@ -5270,6 +5272,9 @@
       </c>
       <c r="C236" s="24">
         <v>43532</v>
+      </c>
+      <c r="F236" s="2" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -5290,6 +5295,9 @@
       <c r="C238" s="24">
         <v>43664</v>
       </c>
+      <c r="D238" s="24">
+        <v>43730</v>
+      </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
@@ -5298,6 +5306,9 @@
       <c r="C239" s="24">
         <v>43671</v>
       </c>
+      <c r="D239" s="24">
+        <v>43730</v>
+      </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
@@ -5309,6 +5320,9 @@
       <c r="C240" s="24">
         <v>43677</v>
       </c>
+      <c r="D240" s="24">
+        <v>43730</v>
+      </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
@@ -5320,6 +5334,12 @@
       <c r="C241" s="24">
         <v>43669</v>
       </c>
+      <c r="D241" s="24">
+        <v>43730</v>
+      </c>
+      <c r="F241" s="2" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
@@ -5332,7 +5352,7 @@
         <v>43672</v>
       </c>
       <c r="D242" s="24">
-        <v>43712</v>
+        <v>43730</v>
       </c>
       <c r="F242" s="2" t="s">
         <v>370</v>
@@ -5350,6 +5370,9 @@
       </c>
       <c r="C243" s="24">
         <v>43670</v>
+      </c>
+      <c r="D243" s="24">
+        <v>43730</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding QDEL QLYS RACE RCKY RDWR REGN RF
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F5968-7538-4176-9FC4-5952611D7EC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329B14A8-FC93-42DE-84DA-FEDDECE1C9DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="412">
   <si>
     <t>SCVL</t>
   </si>
@@ -1318,7 +1318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1337,6 +1337,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1350,7 +1356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1389,6 +1395,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1884,8 +1892,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B244" sqref="B244"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5376,11 +5384,17 @@
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="16" t="s">
+      <c r="A244" s="26" t="s">
         <v>306</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C244" s="24">
+        <v>43593</v>
+      </c>
+      <c r="D244" s="24">
+        <v>43730</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -5394,7 +5408,7 @@
         <v>43677</v>
       </c>
       <c r="D245" s="24">
-        <v>43715</v>
+        <v>43730</v>
       </c>
       <c r="F245" s="2" t="s">
         <v>375</v>
@@ -5421,6 +5435,9 @@
       <c r="C247" s="24">
         <v>43679</v>
       </c>
+      <c r="D247" s="24">
+        <v>43730</v>
+      </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
@@ -5432,6 +5449,9 @@
       <c r="C248" s="24">
         <v>43670</v>
       </c>
+      <c r="D248" s="24">
+        <v>43730</v>
+      </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="16" t="s">
@@ -5440,6 +5460,9 @@
       <c r="B249" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F249" s="2" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="9" t="s">
@@ -5451,6 +5474,9 @@
       <c r="C250" s="24">
         <v>43677</v>
       </c>
+      <c r="D250" s="24">
+        <v>43730</v>
+      </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="16" t="s">
@@ -5459,6 +5485,10 @@
       <c r="B251" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D251" s="24"/>
+      <c r="F251" s="2" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
@@ -5471,7 +5501,7 @@
         <v>43683</v>
       </c>
       <c r="D252" s="24">
-        <v>43715</v>
+        <v>43730</v>
       </c>
       <c r="F252" s="2" t="s">
         <v>371</v>
@@ -5481,7 +5511,7 @@
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="2" t="s">
+      <c r="A253" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B253" s="2" t="s">
@@ -5489,6 +5519,9 @@
       </c>
       <c r="C253" s="24">
         <v>43665</v>
+      </c>
+      <c r="D253" s="24">
+        <v>43730</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding RHP RJ RJF RMD ROK ROP ROST RP RTN RUSHA
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329B14A8-FC93-42DE-84DA-FEDDECE1C9DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA43919-22A6-40FF-9782-DBE65C917906}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1339,7 +1339,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1892,8 +1892,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D252" sqref="D252"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5384,7 +5384,7 @@
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" s="26" t="s">
+      <c r="A244" s="11" t="s">
         <v>306</v>
       </c>
       <c r="B244" s="2" t="s">
@@ -5511,7 +5511,7 @@
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="27" t="s">
+      <c r="A253" s="15" t="s">
         <v>98</v>
       </c>
       <c r="B253" s="2" t="s">
@@ -5525,7 +5525,7 @@
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="11" t="s">
+      <c r="A254" s="26" t="s">
         <v>311</v>
       </c>
       <c r="B254" s="2" t="s">
@@ -5533,6 +5533,9 @@
       </c>
       <c r="C254" s="24">
         <v>43719</v>
+      </c>
+      <c r="D254" s="24">
+        <v>43730</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -5545,6 +5548,9 @@
       <c r="C255" s="24">
         <v>43683</v>
       </c>
+      <c r="D255" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
@@ -5556,6 +5562,9 @@
       <c r="C256" s="24">
         <v>43670</v>
       </c>
+      <c r="D256" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
@@ -5567,6 +5576,9 @@
       <c r="C257" s="24">
         <v>43671</v>
       </c>
+      <c r="D257" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
@@ -5578,6 +5590,9 @@
       <c r="C258" s="24">
         <v>43671</v>
       </c>
+      <c r="D258" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
@@ -5589,6 +5604,9 @@
       <c r="C259" s="24">
         <v>43671</v>
       </c>
+      <c r="D259" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="9" t="s">
@@ -5600,6 +5618,9 @@
       <c r="C260" s="24">
         <v>43699</v>
       </c>
+      <c r="D260" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="11" t="s">
@@ -5611,6 +5632,9 @@
       <c r="C261" s="24">
         <v>43678</v>
       </c>
+      <c r="D261" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
@@ -5622,9 +5646,12 @@
       <c r="C262" s="24">
         <v>43671</v>
       </c>
+      <c r="D262" s="24">
+        <v>43732</v>
+      </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A263" s="2" t="s">
+      <c r="A263" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B263" s="2" t="s">
@@ -5632,6 +5659,9 @@
       </c>
       <c r="C263" s="24">
         <v>43670</v>
+      </c>
+      <c r="D263" s="24">
+        <v>43732</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
@@ -6527,37 +6557,37 @@
     <sortCondition ref="A2:A358"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
-    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:A339">
-    <cfRule type="duplicateValues" dxfId="19" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I341:I343">
-    <cfRule type="duplicateValues" dxfId="18" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I344">
-    <cfRule type="duplicateValues" dxfId="17" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I345:I347">
-    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I346:I347">
-    <cfRule type="duplicateValues" dxfId="15" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I346:I347">
-    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I348:I358">
-    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I348:I358">
-    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M105:M119">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9243,34 +9273,34 @@
     <sortCondition ref="A1:A331"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H4">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H8">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136:B330">
-    <cfRule type="duplicateValues" dxfId="0" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding SBNY SBUX SCCO SCHW SCVL
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA43919-22A6-40FF-9782-DBE65C917906}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBBEEA-25D8-4304-A9BB-E4A953E5630D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1892,8 +1892,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D264" sqref="D264"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D268" sqref="D268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5674,6 +5674,9 @@
       <c r="C264" s="24">
         <v>43664</v>
       </c>
+      <c r="D264" s="24">
+        <v>43733</v>
+      </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
@@ -5685,6 +5688,9 @@
       <c r="C265" s="24">
         <v>43671</v>
       </c>
+      <c r="D265" s="24">
+        <v>43733</v>
+      </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="11" t="s">
@@ -5696,6 +5702,9 @@
       <c r="C266" s="24">
         <v>43674</v>
       </c>
+      <c r="D266" s="24">
+        <v>43733</v>
+      </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
@@ -5707,6 +5716,9 @@
       <c r="C267" s="24">
         <v>43663</v>
       </c>
+      <c r="D267" s="24">
+        <v>43733</v>
+      </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
@@ -5717,6 +5729,9 @@
       </c>
       <c r="C268" s="24">
         <v>43705</v>
+      </c>
+      <c r="D268" s="24">
+        <v>43733</v>
       </c>
       <c r="F268" s="2" t="s">
         <v>2</v>
@@ -6557,37 +6572,37 @@
     <sortCondition ref="A2:A358"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
-    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:A339">
-    <cfRule type="duplicateValues" dxfId="20" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I341:I343">
-    <cfRule type="duplicateValues" dxfId="19" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I344">
-    <cfRule type="duplicateValues" dxfId="18" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I345:I347">
-    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I346:I347">
-    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I346:I347">
-    <cfRule type="duplicateValues" dxfId="15" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I348:I358">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I348:I358">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M105:M119">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9273,34 +9288,34 @@
     <sortCondition ref="A1:A331"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H4">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H8">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H8">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136:B330">
-    <cfRule type="duplicateValues" dxfId="2" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding SIRI SIVB SKYW SMTC SNA
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBBEEA-25D8-4304-A9BB-E4A953E5630D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60321AFF-3332-443E-8345-69999D5B350C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1356,7 +1356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1396,7 +1396,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1893,7 +1892,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D268" sqref="D268"/>
+      <selection pane="bottomLeft" activeCell="D273" sqref="D273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5525,7 +5524,7 @@
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="26" t="s">
+      <c r="A254" s="11" t="s">
         <v>311</v>
       </c>
       <c r="B254" s="2" t="s">
@@ -5651,7 +5650,7 @@
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A263" s="27" t="s">
+      <c r="A263" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B263" s="2" t="s">
@@ -5738,7 +5737,7 @@
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A269" s="11" t="s">
+      <c r="A269" s="26" t="s">
         <v>316</v>
       </c>
       <c r="B269" s="2" t="s">
@@ -5746,6 +5745,9 @@
       </c>
       <c r="C269" s="24">
         <v>43676</v>
+      </c>
+      <c r="D269" s="24">
+        <v>43734</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
@@ -5758,6 +5760,9 @@
       <c r="C270" s="24">
         <v>43671</v>
       </c>
+      <c r="D270" s="24">
+        <v>43734</v>
+      </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="11" t="s">
@@ -5769,6 +5774,9 @@
       <c r="C271" s="24">
         <v>43677</v>
       </c>
+      <c r="D271" s="24">
+        <v>43734</v>
+      </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="9" t="s">
@@ -5780,8 +5788,11 @@
       <c r="C272" s="24">
         <v>43705</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D272" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>115</v>
       </c>
@@ -5791,8 +5802,11 @@
       <c r="C273" s="24">
         <v>43664</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D273" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>18</v>
       </c>
@@ -5803,7 +5817,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="11" t="s">
         <v>319</v>
       </c>
@@ -5814,7 +5828,7 @@
         <v>43699</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
         <v>320</v>
       </c>
@@ -5825,7 +5839,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
         <v>321</v>
       </c>
@@ -5836,12 +5850,12 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>44</v>
       </c>
@@ -5852,7 +5866,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="9" t="s">
         <v>322</v>
       </c>
@@ -5863,7 +5877,7 @@
         <v>43679</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="11" t="s">
         <v>323</v>
       </c>
@@ -5874,7 +5888,7 @@
         <v>43674</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>92</v>
       </c>
@@ -5885,7 +5899,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>97</v>
       </c>
@@ -5896,7 +5910,7 @@
         <v>43665</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="11" t="s">
         <v>324</v>
       </c>
@@ -5907,7 +5921,7 @@
         <v>43689</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="16" t="s">
         <v>325</v>
       </c>
@@ -5915,7 +5929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>122</v>
       </c>
@@ -5926,7 +5940,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="9" t="s">
         <v>326</v>
       </c>
@@ -5937,7 +5951,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Adding SNBR SNPS SRCI ST STM STX STZ SWK SXT SYY
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60321AFF-3332-443E-8345-69999D5B350C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0AB47D-A103-44A7-8981-42F4005E96F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="413">
   <si>
     <t>SCVL</t>
   </si>
@@ -1266,6 +1266,9 @@
   </si>
   <si>
     <t>CNBC does not have next year projections -- maybe temporary not available - Is Ann doing something different</t>
+  </si>
+  <si>
+    <t>Need to adjust the EPS</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1398,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1891,8 +1894,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D273" sqref="D273"/>
+      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F282" sqref="F282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5737,7 +5740,7 @@
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A269" s="26" t="s">
+      <c r="A269" s="11" t="s">
         <v>316</v>
       </c>
       <c r="B269" s="2" t="s">
@@ -5792,7 +5795,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>115</v>
       </c>
@@ -5806,8 +5809,8 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="2" t="s">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B274" s="2" t="s">
@@ -5816,8 +5819,11 @@
       <c r="C274" s="24">
         <v>43671</v>
       </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D274" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="11" t="s">
         <v>319</v>
       </c>
@@ -5827,8 +5833,11 @@
       <c r="C275" s="24">
         <v>43699</v>
       </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D275" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
         <v>320</v>
       </c>
@@ -5838,8 +5847,11 @@
       <c r="C276" s="24">
         <v>43677</v>
       </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D276" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
         <v>321</v>
       </c>
@@ -5849,14 +5861,18 @@
       <c r="C277" s="24">
         <v>43676</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D277" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="19" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="2" t="s">
+      <c r="D278" s="24"/>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B279" s="2" t="s">
@@ -5865,8 +5881,11 @@
       <c r="C279" s="24">
         <v>43671</v>
       </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D279" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="9" t="s">
         <v>322</v>
       </c>
@@ -5876,8 +5895,11 @@
       <c r="C280" s="24">
         <v>43679</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D280" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="11" t="s">
         <v>323</v>
       </c>
@@ -5887,8 +5909,11 @@
       <c r="C281" s="24">
         <v>43674</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D281" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>92</v>
       </c>
@@ -5898,8 +5923,14 @@
       <c r="C282" s="24">
         <v>43669</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D282" s="24">
+        <v>43734</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>97</v>
       </c>
@@ -5909,8 +5940,11 @@
       <c r="C283" s="24">
         <v>43665</v>
       </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D283" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="11" t="s">
         <v>324</v>
       </c>
@@ -5920,8 +5954,11 @@
       <c r="C284" s="24">
         <v>43689</v>
       </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D284" s="24">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="16" t="s">
         <v>325</v>
       </c>
@@ -5929,7 +5966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>122</v>
       </c>
@@ -5940,7 +5977,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="9" t="s">
         <v>326</v>
       </c>
@@ -5951,7 +5988,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Adding TCBI TDG TER TESS TJX
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0AB47D-A103-44A7-8981-42F4005E96F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C2992-F2CF-4E5B-9825-49CC2FB9BD2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1894,8 +1894,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F282" sqref="F282"/>
+      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D290" sqref="D290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5976,6 +5976,9 @@
       <c r="C286" s="24">
         <v>43663</v>
       </c>
+      <c r="D286" s="24">
+        <v>43735</v>
+      </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="9" t="s">
@@ -5987,6 +5990,9 @@
       <c r="C287" s="24">
         <v>43683</v>
       </c>
+      <c r="D287" s="24">
+        <v>43735</v>
+      </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
@@ -5998,8 +6004,11 @@
       <c r="C288" s="24">
         <v>43669</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D288" s="24">
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>95</v>
       </c>
@@ -6009,8 +6018,11 @@
       <c r="C289" s="24">
         <v>43668</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D289" s="24">
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="11" t="s">
         <v>327</v>
       </c>
@@ -6020,8 +6032,11 @@
       <c r="C290" s="24">
         <v>43697</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D290" s="24">
+        <v>43735</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
         <v>328</v>
       </c>
@@ -6032,7 +6047,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="16" t="s">
         <v>329</v>
       </c>
@@ -6040,7 +6055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="10" t="s">
         <v>330</v>
       </c>
@@ -6051,7 +6066,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="11" t="s">
         <v>331</v>
       </c>
@@ -6062,7 +6077,7 @@
         <v>43697</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>61</v>
       </c>
@@ -6073,7 +6088,7 @@
         <v>43670</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>91</v>
       </c>
@@ -6084,7 +6099,7 @@
         <v>43698</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>33</v>
       </c>
@@ -6095,7 +6110,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="11" t="s">
         <v>332</v>
       </c>
@@ -6106,7 +6121,7 @@
         <v>43682</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
         <v>333</v>
       </c>
@@ -6117,7 +6132,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
         <v>334</v>
       </c>
@@ -6128,7 +6143,7 @@
         <v>43699</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
         <v>335</v>
       </c>
@@ -6139,7 +6154,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
         <v>336</v>
       </c>
@@ -6150,7 +6165,7 @@
         <v>43677</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
         <v>337</v>
       </c>
@@ -6161,7 +6176,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="9" t="s">
         <v>338</v>
       </c>

</xml_diff>

<commit_message>
Adding TKR TOL TROW TRU TSCO
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C2992-F2CF-4E5B-9825-49CC2FB9BD2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED9C29-3ECE-4147-97BE-0E4B0180B3AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1359,7 +1359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1399,6 +1399,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1895,7 +1896,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D290" sqref="D290"/>
+      <selection pane="bottomLeft" activeCell="D294" sqref="D294:D297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6046,6 +6047,9 @@
       <c r="C291" s="24">
         <v>43677</v>
       </c>
+      <c r="D291" s="24">
+        <v>43735</v>
+      </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="16" t="s">
@@ -6056,7 +6060,7 @@
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="10" t="s">
+      <c r="A293" s="27" t="s">
         <v>330</v>
       </c>
       <c r="B293" s="2" t="s">
@@ -6076,6 +6080,9 @@
       <c r="C294" s="24">
         <v>43697</v>
       </c>
+      <c r="D294" s="24">
+        <v>43735</v>
+      </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
@@ -6087,6 +6094,9 @@
       <c r="C295" s="24">
         <v>43670</v>
       </c>
+      <c r="D295" s="24">
+        <v>43735</v>
+      </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
@@ -6098,6 +6108,9 @@
       <c r="C296" s="24">
         <v>43698</v>
       </c>
+      <c r="D296" s="24">
+        <v>43735</v>
+      </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
@@ -6108,6 +6121,9 @@
       </c>
       <c r="C297" s="24">
         <v>43671</v>
+      </c>
+      <c r="D297" s="24">
+        <v>43735</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding TSN TSS TTC TTD TTEK TWIN TWTR TXN TXT
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED9C29-3ECE-4147-97BE-0E4B0180B3AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C920885-E685-4CE9-8F76-B9C2CBC174C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="415">
   <si>
     <t>SCVL</t>
   </si>
@@ -1269,6 +1269,12 @@
   </si>
   <si>
     <t>Need to adjust the EPS</t>
+  </si>
+  <si>
+    <t>Not found on CNBC?</t>
+  </si>
+  <si>
+    <t>Keep an eye on it</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1346,6 +1352,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1359,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1400,6 +1418,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1896,7 +1916,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D294" sqref="D294:D297"/>
+      <selection pane="bottomLeft" activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6009,7 +6029,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>95</v>
       </c>
@@ -6023,7 +6043,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="11" t="s">
         <v>327</v>
       </c>
@@ -6037,7 +6057,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
         <v>328</v>
       </c>
@@ -6051,7 +6071,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="16" t="s">
         <v>329</v>
       </c>
@@ -6059,7 +6079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="27" t="s">
         <v>330</v>
       </c>
@@ -6070,7 +6090,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="11" t="s">
         <v>331</v>
       </c>
@@ -6084,7 +6104,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>61</v>
       </c>
@@ -6098,7 +6118,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>91</v>
       </c>
@@ -6112,7 +6132,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>33</v>
       </c>
@@ -6126,8 +6146,8 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A298" s="11" t="s">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="28" t="s">
         <v>332</v>
       </c>
       <c r="B298" s="2" t="s">
@@ -6136,9 +6156,12 @@
       <c r="C298" s="24">
         <v>43682</v>
       </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A299" s="11" t="s">
+      <c r="D298" s="24">
+        <v>43736</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="29" t="s">
         <v>333</v>
       </c>
       <c r="B299" s="2" t="s">
@@ -6147,8 +6170,14 @@
       <c r="C299" s="24">
         <v>43685</v>
       </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D299" s="24">
+        <v>43736</v>
+      </c>
+      <c r="F299" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
         <v>334</v>
       </c>
@@ -6158,8 +6187,11 @@
       <c r="C300" s="24">
         <v>43699</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D300" s="24">
+        <v>43736</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
         <v>335</v>
       </c>
@@ -6169,8 +6201,14 @@
       <c r="C301" s="24">
         <v>43685</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D301" s="24">
+        <v>43736</v>
+      </c>
+      <c r="F301" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
         <v>336</v>
       </c>
@@ -6180,9 +6218,12 @@
       <c r="C302" s="24">
         <v>43677</v>
       </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A303" s="11" t="s">
+      <c r="D302" s="24">
+        <v>43736</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="16" t="s">
         <v>337</v>
       </c>
       <c r="B303" s="2" t="s">
@@ -6192,7 +6233,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="9" t="s">
         <v>338</v>
       </c>
@@ -6201,6 +6242,9 @@
       </c>
       <c r="C304" s="24">
         <v>43686</v>
+      </c>
+      <c r="D304" s="24">
+        <v>43736</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
@@ -6214,7 +6258,7 @@
         <v>43672</v>
       </c>
       <c r="D305" s="24">
-        <v>43712</v>
+        <v>43736</v>
       </c>
       <c r="F305" s="2" t="s">
         <v>370</v>
@@ -6230,6 +6274,9 @@
       <c r="C306" s="24">
         <v>43669</v>
       </c>
+      <c r="D306" s="24">
+        <v>43736</v>
+      </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
@@ -6240,6 +6287,9 @@
       </c>
       <c r="C307" s="24">
         <v>43663</v>
+      </c>
+      <c r="D307" s="24">
+        <v>43736</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding UAL UFPT ULTA UNH UNP
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C920885-E685-4CE9-8F76-B9C2CBC174C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86FFF8-330D-4C4F-8129-13E61BBE6F66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="416">
   <si>
     <t>SCVL</t>
   </si>
@@ -1275,6 +1275,9 @@
   </si>
   <si>
     <t>Keep an eye on it</t>
+  </si>
+  <si>
+    <t>Feb updated???</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1364,6 +1367,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1377,7 +1386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1417,9 +1426,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1915,8 +1925,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D305" sqref="D305"/>
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D314" sqref="D314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6080,7 +6090,7 @@
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A293" s="27" t="s">
+      <c r="A293" s="30" t="s">
         <v>330</v>
       </c>
       <c r="B293" s="2" t="s">
@@ -6147,7 +6157,7 @@
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A298" s="28" t="s">
+      <c r="A298" s="11" t="s">
         <v>332</v>
       </c>
       <c r="B298" s="2" t="s">
@@ -6161,7 +6171,7 @@
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A299" s="29" t="s">
+      <c r="A299" s="27" t="s">
         <v>333</v>
       </c>
       <c r="B299" s="2" t="s">
@@ -6293,7 +6303,7 @@
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A308" s="2" t="s">
+      <c r="A308" s="28" t="s">
         <v>126</v>
       </c>
       <c r="B308" s="2" t="s">
@@ -6302,9 +6312,12 @@
       <c r="C308" s="24">
         <v>43663</v>
       </c>
+      <c r="D308" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A309" s="9" t="s">
+      <c r="A309" s="29" t="s">
         <v>339</v>
       </c>
       <c r="B309" s="2" t="s">
@@ -6312,6 +6325,9 @@
       </c>
       <c r="C309" s="24">
         <v>43504</v>
+      </c>
+      <c r="F309" s="2" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
@@ -6324,6 +6340,9 @@
       <c r="C310" s="24">
         <v>43685</v>
       </c>
+      <c r="D310" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="11" t="s">
@@ -6335,6 +6354,9 @@
       <c r="C311" s="24">
         <v>43706</v>
       </c>
+      <c r="D311" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
@@ -6346,6 +6368,9 @@
       <c r="C312" s="24">
         <v>43664</v>
       </c>
+      <c r="D312" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
@@ -6356,6 +6381,9 @@
       </c>
       <c r="C313" s="24">
         <v>43664</v>
+      </c>
+      <c r="D313" s="24">
+        <v>43737</v>
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding URI USNA UVE V VEEV
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86FFF8-330D-4C4F-8129-13E61BBE6F66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFED8DE-49F2-4502-A502-8136BACC0DCF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1357,12 +1357,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1370,6 +1364,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1426,10 +1426,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1926,7 +1926,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D314" sqref="D314"/>
+      <selection pane="bottomLeft" activeCell="D318" sqref="D318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6090,7 +6090,7 @@
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A293" s="30" t="s">
+      <c r="A293" s="29" t="s">
         <v>330</v>
       </c>
       <c r="B293" s="2" t="s">
@@ -6303,7 +6303,7 @@
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A308" s="28" t="s">
+      <c r="A308" s="15" t="s">
         <v>126</v>
       </c>
       <c r="B308" s="2" t="s">
@@ -6317,7 +6317,7 @@
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A309" s="29" t="s">
+      <c r="A309" s="28" t="s">
         <v>339</v>
       </c>
       <c r="B309" s="2" t="s">
@@ -6387,7 +6387,7 @@
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A314" s="2" t="s">
+      <c r="A314" s="30" t="s">
         <v>121</v>
       </c>
       <c r="B314" s="2" t="s">
@@ -6395,6 +6395,9 @@
       </c>
       <c r="C314" s="24">
         <v>43663</v>
+      </c>
+      <c r="D314" s="24">
+        <v>43737</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
@@ -6407,6 +6410,9 @@
       <c r="C315" s="24">
         <v>43669</v>
       </c>
+      <c r="D315" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="11" t="s">
@@ -6418,6 +6424,9 @@
       <c r="C316" s="24">
         <v>43677</v>
       </c>
+      <c r="D316" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
@@ -6429,6 +6438,9 @@
       <c r="C317" s="24">
         <v>43669</v>
       </c>
+      <c r="D317" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="11" t="s">
@@ -6441,7 +6453,7 @@
         <v>43704</v>
       </c>
       <c r="D318" s="24">
-        <v>43729</v>
+        <v>43737</v>
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding VFC VLO VMC VMW VNOM VRTX VSH
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFED8DE-49F2-4502-A502-8136BACC0DCF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2962D911-1F99-4E0C-B9DC-61CC2EBABD84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1926,7 +1926,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D318" sqref="D318"/>
+      <selection pane="bottomLeft" activeCell="D326" sqref="D326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6387,7 +6387,7 @@
       </c>
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A314" s="30" t="s">
+      <c r="A314" s="15" t="s">
         <v>121</v>
       </c>
       <c r="B314" s="2" t="s">
@@ -6457,7 +6457,7 @@
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A319" s="2" t="s">
+      <c r="A319" s="30" t="s">
         <v>70</v>
       </c>
       <c r="B319" s="2" t="s">
@@ -6465,6 +6465,9 @@
       </c>
       <c r="C319" s="24">
         <v>43670</v>
+      </c>
+      <c r="D319" s="24">
+        <v>43737</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
@@ -6477,8 +6480,11 @@
       <c r="C320" s="24">
         <v>43671</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D320" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>32</v>
       </c>
@@ -6488,8 +6494,11 @@
       <c r="C321" s="24">
         <v>43671</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D321" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="11" t="s">
         <v>342</v>
       </c>
@@ -6499,8 +6508,11 @@
       <c r="C322" s="24">
         <v>43699</v>
       </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D322" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
         <v>343</v>
       </c>
@@ -6510,8 +6522,11 @@
       <c r="C323" s="24">
         <v>43676</v>
       </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D323" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="11" t="s">
         <v>344</v>
       </c>
@@ -6521,8 +6536,11 @@
       <c r="C324" s="24">
         <v>43677</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D324" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="11" t="s">
         <v>345</v>
       </c>
@@ -6532,8 +6550,11 @@
       <c r="C325" s="24">
         <v>43676</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D325" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>101</v>
       </c>
@@ -6544,7 +6565,7 @@
         <v>43664</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
         <v>346</v>
       </c>
@@ -6555,7 +6576,7 @@
         <v>43697</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="11" t="s">
         <v>347</v>
       </c>
@@ -6566,7 +6587,7 @@
         <v>43675</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="11" t="s">
         <v>348</v>
       </c>
@@ -6577,7 +6598,7 @@
         <v>43635</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>93</v>
       </c>
@@ -6588,7 +6609,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" s="11" t="s">
         <v>349</v>
       </c>
@@ -6599,7 +6620,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" s="25" t="s">
         <v>350</v>
       </c>
@@ -6607,7 +6628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>42</v>
       </c>
@@ -6618,7 +6639,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" s="12" t="s">
         <v>351</v>
       </c>
@@ -6629,7 +6650,7 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
         <v>352</v>
       </c>
@@ -6640,7 +6661,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
         <v>353</v>
       </c>

</xml_diff>

<commit_message>
Adding WAL WB WCN WGO WINA WLFC
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2962D911-1F99-4E0C-B9DC-61CC2EBABD84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831F1107-6E9D-40BC-877E-89A98F228B92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="417">
   <si>
     <t>SCVL</t>
   </si>
@@ -1278,6 +1278,9 @@
   </si>
   <si>
     <t>Feb updated???</t>
+  </si>
+  <si>
+    <t>No projections on CNBC</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1430,6 +1433,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1926,7 +1931,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D326" sqref="D326"/>
+      <selection pane="bottomLeft" activeCell="F322" sqref="F322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6457,7 +6462,7 @@
       </c>
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A319" s="30" t="s">
+      <c r="A319" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B319" s="2" t="s">
@@ -6484,7 +6489,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>32</v>
       </c>
@@ -6498,7 +6503,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="11" t="s">
         <v>342</v>
       </c>
@@ -6512,7 +6517,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
         <v>343</v>
       </c>
@@ -6526,7 +6531,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="11" t="s">
         <v>344</v>
       </c>
@@ -6540,7 +6545,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="11" t="s">
         <v>345</v>
       </c>
@@ -6554,8 +6559,8 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="s">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" s="30" t="s">
         <v>101</v>
       </c>
       <c r="B326" s="2" t="s">
@@ -6564,8 +6569,11 @@
       <c r="C326" s="24">
         <v>43664</v>
       </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D326" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
         <v>346</v>
       </c>
@@ -6575,8 +6583,11 @@
       <c r="C327" s="24">
         <v>43697</v>
       </c>
-    </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D327" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="11" t="s">
         <v>347</v>
       </c>
@@ -6586,8 +6597,11 @@
       <c r="C328" s="24">
         <v>43675</v>
       </c>
-    </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D328" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="11" t="s">
         <v>348</v>
       </c>
@@ -6597,9 +6611,12 @@
       <c r="C329" s="24">
         <v>43635</v>
       </c>
-    </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A330" s="2" t="s">
+      <c r="D329" s="24">
+        <v>43737</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="31" t="s">
         <v>93</v>
       </c>
       <c r="B330" s="2" t="s">
@@ -6608,9 +6625,15 @@
       <c r="C330" s="24">
         <v>43668</v>
       </c>
-    </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="11" t="s">
+      <c r="D330" s="24">
+        <v>43737</v>
+      </c>
+      <c r="F330" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" s="32" t="s">
         <v>349</v>
       </c>
       <c r="B331" s="2" t="s">
@@ -6619,8 +6642,14 @@
       <c r="C331" s="24">
         <v>43685</v>
       </c>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D331" s="24">
+        <v>43737</v>
+      </c>
+      <c r="F331" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="25" t="s">
         <v>350</v>
       </c>
@@ -6628,7 +6657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>42</v>
       </c>
@@ -6639,7 +6668,7 @@
         <v>43671</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="12" t="s">
         <v>351</v>
       </c>
@@ -6650,7 +6679,7 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
         <v>352</v>
       </c>
@@ -6661,7 +6690,7 @@
         <v>43683</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
         <v>353</v>
       </c>

</xml_diff>

<commit_message>
Adding WM WYND WYNN ZBRA ZTS ZUMZ
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831F1107-6E9D-40BC-877E-89A98F228B92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F142708F-0760-4EC5-A3BF-4A96F7634D4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="418">
   <si>
     <t>SCVL</t>
   </si>
@@ -1281,6 +1281,9 @@
   </si>
   <si>
     <t>No projections on CNBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yahoo has historical data missing - maybe temporary </t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1370,12 +1373,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1389,7 +1386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1432,7 +1429,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1931,7 +1927,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F322" sqref="F322"/>
+      <selection pane="bottomLeft" activeCell="F340" sqref="F340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6560,7 +6556,7 @@
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A326" s="30" t="s">
+      <c r="A326" s="15" t="s">
         <v>101</v>
       </c>
       <c r="B326" s="2" t="s">
@@ -6616,7 +6612,7 @@
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A330" s="31" t="s">
+      <c r="A330" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B330" s="2" t="s">
@@ -6633,7 +6629,7 @@
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A331" s="32" t="s">
+      <c r="A331" s="31" t="s">
         <v>349</v>
       </c>
       <c r="B331" s="2" t="s">
@@ -6667,6 +6663,9 @@
       <c r="C333" s="24">
         <v>43671</v>
       </c>
+      <c r="D333" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="12" t="s">
@@ -6678,6 +6677,9 @@
       <c r="C334" s="24">
         <v>43676</v>
       </c>
+      <c r="D334" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
@@ -6689,6 +6691,9 @@
       <c r="C335" s="24">
         <v>43683</v>
       </c>
+      <c r="D335" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
@@ -6700,9 +6705,12 @@
       <c r="C336" s="24">
         <v>43676</v>
       </c>
+      <c r="D336" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A337" s="11" t="s">
+      <c r="A337" s="16" t="s">
         <v>354</v>
       </c>
       <c r="B337" s="2" t="s">
@@ -6711,6 +6719,7 @@
       <c r="C337" s="24">
         <v>43602</v>
       </c>
+      <c r="D337" s="24"/>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
@@ -6722,6 +6731,9 @@
       <c r="C338" s="24">
         <v>43683</v>
       </c>
+      <c r="D338" s="24">
+        <v>43737</v>
+      </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" s="11" t="s">
@@ -6732,6 +6744,12 @@
       </c>
       <c r="C339" s="24">
         <v>43713</v>
+      </c>
+      <c r="D339" s="24">
+        <v>43737</v>
+      </c>
+      <c r="F339" s="2" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding KBH MU after earnings
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F142708F-0760-4EC5-A3BF-4A96F7634D4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF84CC7-1570-4B32-AE9C-487CD931F8A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1926,8 +1926,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F340" sqref="F340"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4277,10 +4277,10 @@
         <v>11</v>
       </c>
       <c r="C162" s="24">
-        <v>43642</v>
+        <v>43733</v>
       </c>
       <c r="D162" s="24">
-        <v>43723</v>
+        <v>43738</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4834,7 +4834,7 @@
         <v>11</v>
       </c>
       <c r="C202" s="24">
-        <v>43652</v>
+        <v>43683</v>
       </c>
       <c r="D202" s="24">
         <v>43726</v>
@@ -4862,10 +4862,10 @@
         <v>11</v>
       </c>
       <c r="C204" s="24">
-        <v>43641</v>
+        <v>43735</v>
       </c>
       <c r="D204" s="24">
-        <v>43726</v>
+        <v>43738</v>
       </c>
       <c r="F204" s="2" t="s">
         <v>399</v>

</xml_diff>

<commit_message>
Adding RECN and updating COST CTAS
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D281D-ABDD-430A-AEB7-53A98B2902FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83748FA5-6CA1-49AF-BA2D-EEA33B0D8136}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="433">
   <si>
     <t>SCVL</t>
   </si>
@@ -1229,9 +1229,6 @@
     <t>Ann has some comments in the chart</t>
   </si>
   <si>
-    <t>Hmm..Not seeing it now</t>
-  </si>
-  <si>
     <t>This is an etf</t>
   </si>
   <si>
@@ -1329,6 +1326,9 @@
   </si>
   <si>
     <t>Ask Ann why huge price increse in 2014-2016 and then a huge drop without any corresponding big jump or big drop in earnings…Is the market looking at some other metric</t>
+  </si>
+  <si>
+    <t>CNBC has no projections - just actual earnings…Where is Ann Getting future projections from?</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1863,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G188" sqref="G188"/>
+      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G246" sqref="G246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1902,7 +1902,7 @@
         <v>368</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -2389,7 +2389,7 @@
         <v>43740</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>360</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2839,11 +2839,11 @@
       <c r="B66" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C66" s="19">
+        <v>43741</v>
+      </c>
       <c r="D66" s="19">
-        <v>43698</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>399</v>
+        <v>43745</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
         <v>43729</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2989,10 +2989,10 @@
         <v>11</v>
       </c>
       <c r="C76" s="19">
-        <v>43662</v>
+        <v>43732</v>
       </c>
       <c r="D76" s="19">
-        <v>43713</v>
+        <v>43745</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -3530,10 +3530,10 @@
         <v>166</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3736,7 +3736,7 @@
       </c>
       <c r="C127" s="19"/>
       <c r="F127" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4960,7 +4960,7 @@
         <v>43728</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>43729</v>
       </c>
       <c r="F227" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>43532</v>
       </c>
       <c r="F236" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -5320,7 +5320,7 @@
         <v>43730</v>
       </c>
       <c r="F241" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -5396,7 +5396,7 @@
         <v>177</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -5453,15 +5453,20 @@
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A251" s="11" t="s">
+      <c r="A251" s="12" t="s">
         <v>309</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D251" s="19"/>
+      <c r="C251" s="19">
+        <v>43740</v>
+      </c>
+      <c r="D251" s="19">
+        <v>43745</v>
+      </c>
       <c r="F251" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -5899,7 +5904,7 @@
         <v>43734</v>
       </c>
       <c r="F282" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6125,7 +6130,7 @@
         <v>43736</v>
       </c>
       <c r="F299" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
@@ -6156,7 +6161,7 @@
         <v>43736</v>
       </c>
       <c r="F301" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
@@ -6268,7 +6273,7 @@
         <v>43504</v>
       </c>
       <c r="F309" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
@@ -6565,7 +6570,7 @@
         <v>43737</v>
       </c>
       <c r="F330" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6582,7 +6587,7 @@
         <v>43737</v>
       </c>
       <c r="F331" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6689,12 +6694,12 @@
         <v>43737</v>
       </c>
       <c r="F339" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>11</v>
@@ -6708,23 +6713,21 @@
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" s="29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C341" s="19">
-        <v>43304</v>
-      </c>
+      <c r="C341" s="19"/>
       <c r="D341" s="19"/>
       <c r="F341" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I341" s="5"/>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>11</v>
@@ -6736,7 +6739,7 @@
         <v>43739</v>
       </c>
       <c r="F342" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I342" s="5"/>
     </row>
@@ -6846,67 +6849,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating AGCO ALB ALGN ALOT ALSN AL AME AMOT ANET ANSS ANTM
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83748FA5-6CA1-49AF-BA2D-EEA33B0D8136}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BECC29-C511-4939-9173-533FAE4A8DA6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="433">
   <si>
     <t>SCVL</t>
   </si>
@@ -1106,9 +1106,6 @@
     <t>Seems like a nice growth ahead - Ann's adjusted analyst lines are flatter than the actual analysts. Understand why</t>
   </si>
   <si>
-    <t xml:space="preserve">This does not plot correctly with xtick and xticklabels on…not sure what is wrong though. If plotted without labels, it plots correctly </t>
-  </si>
-  <si>
     <t>This one looks good</t>
   </si>
   <si>
@@ -1329,6 +1326,9 @@
   </si>
   <si>
     <t>CNBC has no projections - just actual earnings…Where is Ann Getting future projections from?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formly known as Atro-Med Inc -- Need to put that in text box </t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1468,6 +1468,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1863,8 +1866,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G246" sqref="G246"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1887,7 +1890,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>5</v>
@@ -1899,10 +1902,10 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -1936,7 +1939,7 @@
         <v>43715</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1995,7 +1998,7 @@
         <v>43715</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>356</v>
@@ -2042,8 +2045,8 @@
       <c r="C10" s="19">
         <v>43676</v>
       </c>
-      <c r="D10" s="19">
-        <v>43690</v>
+      <c r="D10" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2056,8 +2059,8 @@
       <c r="C11" s="19">
         <v>43685</v>
       </c>
-      <c r="D11" s="19">
-        <v>43690</v>
+      <c r="D11" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2070,8 +2073,8 @@
       <c r="C12" s="19">
         <v>43684</v>
       </c>
-      <c r="D12" s="19">
-        <v>43690</v>
+      <c r="D12" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2084,8 +2087,8 @@
       <c r="C13" s="19">
         <v>43670</v>
       </c>
-      <c r="D13" s="19">
-        <v>43690</v>
+      <c r="D13" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2098,11 +2101,11 @@
       <c r="C14" s="19">
         <v>43674</v>
       </c>
-      <c r="D14" s="19">
-        <v>43690</v>
+      <c r="D14" s="30">
+        <v>43745</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>358</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2115,8 +2118,8 @@
       <c r="C15" s="19">
         <v>43677</v>
       </c>
-      <c r="D15" s="19">
-        <v>43690</v>
+      <c r="D15" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2143,8 +2146,8 @@
       <c r="C17" s="19">
         <v>43676</v>
       </c>
-      <c r="D17" s="19">
-        <v>43690</v>
+      <c r="D17" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,8 +2160,8 @@
       <c r="C18" s="19">
         <v>43678</v>
       </c>
-      <c r="D18" s="19">
-        <v>43691</v>
+      <c r="D18" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2176,7 +2179,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2189,8 +2192,8 @@
       <c r="C20" s="19">
         <v>43678</v>
       </c>
-      <c r="D20" s="19">
-        <v>43691</v>
+      <c r="D20" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2217,8 +2220,8 @@
       <c r="C22" s="19">
         <v>43682</v>
       </c>
-      <c r="D22" s="19">
-        <v>43691</v>
+      <c r="D22" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2231,8 +2234,8 @@
       <c r="C23" s="19">
         <v>43670</v>
       </c>
-      <c r="D23" s="19">
-        <v>43691</v>
+      <c r="D23" s="30">
+        <v>43745</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2246,7 +2249,7 @@
         <v>43693</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2277,7 +2280,7 @@
         <v>43693</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2352,10 +2355,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="D32" s="19">
         <v>43698</v>
@@ -2389,7 +2392,7 @@
         <v>43740</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2571,10 +2574,10 @@
         <v>43729</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,7 +2661,7 @@
         <v>43703</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2742,7 +2745,7 @@
         <v>43712</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2829,7 +2832,7 @@
         <v>43715</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2874,7 +2877,7 @@
         <v>43729</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2891,7 +2894,7 @@
         <v>43706</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,7 +2925,7 @@
         <v>43706</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3031,7 +3034,7 @@
         <v>43671</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3084,7 +3087,7 @@
         <v>223</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C83" s="19">
         <v>43693</v>
@@ -3147,7 +3150,7 @@
         <v>43714</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -3192,7 +3195,7 @@
         <v>43714</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M90" s="8"/>
     </row>
@@ -3239,7 +3242,7 @@
         <v>43716</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -3265,7 +3268,7 @@
         <v>11</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -3296,7 +3299,7 @@
         <v>43716</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M97" s="4"/>
     </row>
@@ -3343,7 +3346,7 @@
         <v>43715</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -3360,7 +3363,7 @@
         <v>43716</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M101" s="6"/>
     </row>
@@ -3393,7 +3396,7 @@
         <v>43716</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M103" s="8"/>
     </row>
@@ -3522,7 +3525,7 @@
         <v>43717</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3530,10 +3533,10 @@
         <v>166</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3550,7 +3553,7 @@
         <v>43717</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3581,7 +3584,7 @@
         <v>43714</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>137</v>
@@ -3629,7 +3632,7 @@
         <v>43718</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3640,7 +3643,7 @@
         <v>11</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3671,7 +3674,7 @@
         <v>43718</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3736,7 +3739,7 @@
       </c>
       <c r="C127" s="19"/>
       <c r="F127" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3753,7 +3756,7 @@
         <v>43718</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4024,7 +4027,7 @@
         <v>43723</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -4080,7 +4083,7 @@
         <v>43723</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4097,7 +4100,7 @@
         <v>43723</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4178,7 +4181,7 @@
         <v>263</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4228,7 +4231,7 @@
         <v>266</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4236,7 +4239,7 @@
         <v>267</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4390,7 +4393,7 @@
         <v>43724</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4415,7 +4418,7 @@
         <v>11</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -4544,7 +4547,7 @@
         <v>43714</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -4561,7 +4564,7 @@
         <v>43714</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G187" s="2" t="s">
         <v>140</v>
@@ -4609,7 +4612,7 @@
         <v>43725</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -4620,7 +4623,7 @@
         <v>11</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -4637,7 +4640,7 @@
         <v>43725</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -4808,7 +4811,7 @@
         <v>43738</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -4822,7 +4825,7 @@
         <v>43726</v>
       </c>
       <c r="F205" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -4881,7 +4884,7 @@
         <v>43728</v>
       </c>
       <c r="F209" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -4926,7 +4929,7 @@
         <v>43728</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G212" s="2" t="s">
         <v>142</v>
@@ -4960,7 +4963,7 @@
         <v>43728</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -5136,7 +5139,7 @@
         <v>43729</v>
       </c>
       <c r="F227" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,7 +5259,7 @@
         <v>43532</v>
       </c>
       <c r="F236" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -5320,7 +5323,7 @@
         <v>43730</v>
       </c>
       <c r="F241" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -5337,7 +5340,7 @@
         <v>43730</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G242" s="2" t="s">
         <v>134</v>
@@ -5385,7 +5388,7 @@
         <v>43730</v>
       </c>
       <c r="F245" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G245" s="2" t="s">
         <v>144</v>
@@ -5396,7 +5399,7 @@
         <v>177</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -5435,7 +5438,7 @@
         <v>11</v>
       </c>
       <c r="F249" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -5466,7 +5469,7 @@
         <v>43745</v>
       </c>
       <c r="F251" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -5483,7 +5486,7 @@
         <v>43730</v>
       </c>
       <c r="F252" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G252" s="2" t="s">
         <v>157</v>
@@ -5904,7 +5907,7 @@
         <v>43734</v>
       </c>
       <c r="F282" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6130,7 +6133,7 @@
         <v>43736</v>
       </c>
       <c r="F299" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
@@ -6161,7 +6164,7 @@
         <v>43736</v>
       </c>
       <c r="F301" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
@@ -6217,7 +6220,7 @@
         <v>43736</v>
       </c>
       <c r="F305" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
@@ -6273,7 +6276,7 @@
         <v>43504</v>
       </c>
       <c r="F309" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
@@ -6570,7 +6573,7 @@
         <v>43737</v>
       </c>
       <c r="F330" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
@@ -6587,7 +6590,7 @@
         <v>43737</v>
       </c>
       <c r="F331" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
@@ -6694,12 +6697,12 @@
         <v>43737</v>
       </c>
       <c r="F339" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>11</v>
@@ -6713,7 +6716,7 @@
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>11</v>
@@ -6721,13 +6724,13 @@
       <c r="C341" s="19"/>
       <c r="D341" s="19"/>
       <c r="F341" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I341" s="5"/>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" s="28" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>11</v>
@@ -6739,7 +6742,7 @@
         <v>43739</v>
       </c>
       <c r="F342" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I342" s="5"/>
     </row>
@@ -6849,67 +6852,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating AOS APH ASGN ATHM ATVI AXP BAC BR BOOM
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BECC29-C511-4939-9173-533FAE4A8DA6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBC09AF-16AE-4F43-9871-00C479A77023}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$352</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="433">
   <si>
     <t>SCVL</t>
   </si>
@@ -1867,7 +1868,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2245,11 +2246,11 @@
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="19">
-        <v>43693</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>362</v>
+      <c r="C24" s="19">
+        <v>43676</v>
+      </c>
+      <c r="D24" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2262,8 +2263,8 @@
       <c r="C25" s="19">
         <v>43670</v>
       </c>
-      <c r="D25" s="19">
-        <v>43693</v>
+      <c r="D25" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2276,8 +2277,8 @@
       <c r="C26" s="19">
         <v>43670</v>
       </c>
-      <c r="D26" s="19">
-        <v>43693</v>
+      <c r="D26" s="30">
+        <v>43746</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>358</v>
@@ -2293,8 +2294,8 @@
       <c r="C27" s="19">
         <v>43684</v>
       </c>
-      <c r="D27" s="19">
-        <v>43693</v>
+      <c r="D27" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,8 +2308,8 @@
       <c r="C28" s="19">
         <v>43685</v>
       </c>
-      <c r="D28" s="19">
-        <v>43693</v>
+      <c r="D28" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2374,8 +2375,8 @@
       <c r="C33" s="19">
         <v>43665</v>
       </c>
-      <c r="D33" s="19">
-        <v>43693</v>
+      <c r="D33" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2405,8 +2406,8 @@
       <c r="C35" s="19">
         <v>43684</v>
       </c>
-      <c r="D35" s="19">
-        <v>43693</v>
+      <c r="D35" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2444,8 +2445,8 @@
       <c r="C38" s="19">
         <v>43663</v>
       </c>
-      <c r="D38" s="19">
-        <v>43694</v>
+      <c r="D38" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2528,8 +2529,8 @@
       <c r="C44" s="19">
         <v>43671</v>
       </c>
-      <c r="D44" s="19">
-        <v>43694</v>
+      <c r="D44" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2542,8 +2543,8 @@
       <c r="C45" s="19">
         <v>43678</v>
       </c>
-      <c r="D45" s="19">
-        <v>43694</v>
+      <c r="D45" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating BABA BA BBST BBT BIIB BSX
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBC09AF-16AE-4F43-9871-00C479A77023}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769A4391-D428-44EA-B705-DABA47D4456A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="433">
   <si>
     <t>SCVL</t>
   </si>
@@ -1867,8 +1867,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2417,8 +2417,8 @@
       <c r="C36" s="19">
         <v>43670</v>
       </c>
-      <c r="D36" s="19">
-        <v>43694</v>
+      <c r="D36" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2431,8 +2431,8 @@
       <c r="C37" s="19">
         <v>43692</v>
       </c>
-      <c r="D37" s="19">
-        <v>43694</v>
+      <c r="D37" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2459,8 +2459,8 @@
       <c r="C39" s="19">
         <v>43683</v>
       </c>
-      <c r="D39" s="19">
-        <v>43694</v>
+      <c r="D39" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2473,8 +2473,8 @@
       <c r="C40" s="19">
         <v>43664</v>
       </c>
-      <c r="D40" s="19">
-        <v>43694</v>
+      <c r="D40" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2501,8 +2501,8 @@
       <c r="C42" s="19">
         <v>43669</v>
       </c>
-      <c r="D42" s="19">
-        <v>43694</v>
+      <c r="D42" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2557,8 +2557,8 @@
       <c r="C46" s="19">
         <v>43670</v>
       </c>
-      <c r="D46" s="19">
-        <v>43694</v>
+      <c r="D46" s="30">
+        <v>43746</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating AX CDW CSGP
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769A4391-D428-44EA-B705-DABA47D4456A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E2BF60-77CA-4D77-AC8C-7DFBDFBF60CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="433">
   <si>
     <t>SCVL</t>
   </si>
@@ -1867,8 +1867,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2361,8 +2361,11 @@
       <c r="B32" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="C32" s="19">
+        <v>43676</v>
+      </c>
       <c r="D32" s="19">
-        <v>43698</v>
+        <v>43746</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,9 +2661,7 @@
       <c r="B53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="19">
-        <v>43703</v>
-      </c>
+      <c r="D53" s="19"/>
       <c r="F53" s="2" t="s">
         <v>362</v>
       </c>
@@ -2676,7 +2677,7 @@
         <v>43677</v>
       </c>
       <c r="D54" s="19">
-        <v>43703</v>
+        <v>43746</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2968,7 +2969,7 @@
         <v>43669</v>
       </c>
       <c r="D74" s="19">
-        <v>43698</v>
+        <v>43746</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updatig  CLEG CFG CHE CHRW
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2AEDB-C26C-4C15-83E6-A915514C0472}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BD3996-8C12-4FA4-9535-1EF92760C161}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1381,7 +1381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1418,12 +1418,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1437,7 +1431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1479,9 +1473,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1880,7 +1871,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57:D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2620,7 +2611,7 @@
       <c r="C49" s="19">
         <v>43676</v>
       </c>
-      <c r="D49" s="31">
+      <c r="D49" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2634,7 +2625,7 @@
       <c r="C50" s="19">
         <v>43691</v>
       </c>
-      <c r="D50" s="31">
+      <c r="D50" s="30">
         <v>43747</v>
       </c>
       <c r="F50" s="2" t="s">
@@ -2651,7 +2642,7 @@
       <c r="C51" s="19">
         <v>43684</v>
       </c>
-      <c r="D51" s="31">
+      <c r="D51" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2665,7 +2656,7 @@
       <c r="C52" s="19">
         <v>43670</v>
       </c>
-      <c r="D52" s="31">
+      <c r="D52" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2679,7 +2670,7 @@
       <c r="C53" s="19">
         <v>43678</v>
       </c>
-      <c r="D53" s="31">
+      <c r="D53" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2733,7 +2724,7 @@
       <c r="C57" s="19">
         <v>43676</v>
       </c>
-      <c r="D57" s="31">
+      <c r="D57" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2747,7 +2738,7 @@
       <c r="C58" s="19">
         <v>43665</v>
       </c>
-      <c r="D58" s="31">
+      <c r="D58" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2758,7 +2749,7 @@
       <c r="C59" s="19">
         <v>43671</v>
       </c>
-      <c r="D59" s="31">
+      <c r="D59" s="30">
         <v>43747</v>
       </c>
     </row>
@@ -2772,7 +2763,7 @@
       <c r="C60" s="19">
         <v>43676</v>
       </c>
-      <c r="D60" s="31">
+      <c r="D60" s="30">
         <v>43747</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating HWC JPM MA SCHW SNBR UAL UNH
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2588463A-96DA-4F67-8A26-298AD20426DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C65DD7C-595A-4E25-A85B-0934672657F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$352</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1882,8 +1881,8 @@
   <dimension ref="A1:M358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E276" sqref="E276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4019,10 +4018,10 @@
         <v>11</v>
       </c>
       <c r="C146" s="19">
-        <v>43662</v>
+        <v>43753</v>
       </c>
       <c r="D146" s="19">
-        <v>43722</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -4257,10 +4256,10 @@
         <v>11</v>
       </c>
       <c r="C163" s="19">
-        <v>43662</v>
+        <v>43753</v>
       </c>
       <c r="D163" s="19">
-        <v>43723</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -5747,10 +5746,10 @@
         <v>11</v>
       </c>
       <c r="C269" s="19">
-        <v>43663</v>
+        <v>43753</v>
       </c>
       <c r="D269" s="19">
-        <v>43733</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
@@ -5848,10 +5847,10 @@
         <v>11</v>
       </c>
       <c r="C276" s="19">
-        <v>43671</v>
+        <v>43753</v>
       </c>
       <c r="D276" s="19">
-        <v>43734</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -6310,10 +6309,10 @@
         <v>11</v>
       </c>
       <c r="C310" s="19">
-        <v>43663</v>
+        <v>43753</v>
       </c>
       <c r="D310" s="19">
-        <v>43737</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
@@ -6366,10 +6365,10 @@
         <v>11</v>
       </c>
       <c r="C314" s="19">
-        <v>43664</v>
+        <v>43753</v>
       </c>
       <c r="D314" s="19">
-        <v>43737</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More tickers are updated
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE60BF1-6B7F-4EC5-BC8E-D8A6AA52322C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12BBDDF-07C0-4A2F-BA04-EAAAE6C28A37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$A$352</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="441">
   <si>
     <t>SCVL</t>
   </si>
@@ -1344,6 +1345,15 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>Is_Foreign</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -1897,11 +1907,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N358"/>
+  <dimension ref="A1:O358"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A306" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C309" sqref="C309"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1910,13 +1920,14 @@
     <col min="3" max="3" width="12.28515625" style="18" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="18" customWidth="1"/>
     <col min="5" max="6" width="12" style="2" customWidth="1"/>
-    <col min="7" max="7" width="98.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="139.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="15.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="98.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="139.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1935,26 +1946,29 @@
       <c r="F1" s="34" t="s">
         <v>436</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="34" t="s">
+        <v>439</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>336</v>
       </c>
@@ -1965,7 +1979,7 @@
         <v>43478</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>245</v>
       </c>
@@ -1976,7 +1990,7 @@
         <v>43488</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>222</v>
       </c>
@@ -1990,7 +2004,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>329</v>
       </c>
@@ -2001,7 +2015,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>338</v>
       </c>
@@ -2011,11 +2025,11 @@
       <c r="C6" s="19">
         <v>43504</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>303</v>
       </c>
@@ -2025,11 +2039,11 @@
       <c r="C7" s="19">
         <v>43532</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>239</v>
       </c>
@@ -2040,7 +2054,7 @@
         <v>43566</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>305</v>
       </c>
@@ -2054,7 +2068,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>353</v>
       </c>
@@ -2066,7 +2080,7 @@
       </c>
       <c r="D10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>347</v>
       </c>
@@ -2080,7 +2094,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>230</v>
       </c>
@@ -2093,11 +2107,11 @@
       <c r="D12" s="19">
         <v>43716</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>285</v>
       </c>
@@ -2105,13 +2119,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="19">
-        <v>43656</v>
+        <v>43762</v>
       </c>
       <c r="D13" s="19">
         <v>43726</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>76</v>
       </c>
@@ -2119,14 +2133,14 @@
         <v>11</v>
       </c>
       <c r="C14" s="19">
-        <v>43659</v>
+        <v>43761</v>
       </c>
       <c r="D14" s="19">
         <v>43716</v>
       </c>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>130</v>
       </c>
@@ -2134,13 +2148,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="19">
-        <v>43662</v>
+        <v>43761</v>
       </c>
       <c r="D15" s="30">
         <v>43749</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>129</v>
       </c>
@@ -2154,7 +2171,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>132</v>
       </c>
@@ -2167,12 +2184,12 @@
       <c r="D17" s="19">
         <v>43714</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>302</v>
       </c>
@@ -2186,7 +2203,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>119</v>
       </c>
@@ -2197,7 +2214,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>122</v>
       </c>
@@ -2211,7 +2228,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>124</v>
       </c>
@@ -2225,7 +2242,7 @@
         <v>43736</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>121</v>
       </c>
@@ -2239,7 +2256,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>118</v>
       </c>
@@ -2253,7 +2270,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>103</v>
       </c>
@@ -2266,9 +2283,9 @@
       <c r="D24" s="19">
         <v>43716</v>
       </c>
-      <c r="N24" s="8"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="8"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>107</v>
       </c>
@@ -2279,7 +2296,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>114</v>
       </c>
@@ -2293,7 +2310,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>113</v>
       </c>
@@ -2307,7 +2324,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2321,7 +2338,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>116</v>
       </c>
@@ -2335,7 +2352,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -2343,13 +2360,13 @@
         <v>11</v>
       </c>
       <c r="C30" s="19">
-        <v>43664</v>
+        <v>43761</v>
       </c>
       <c r="D30" s="19">
         <v>43726</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>112</v>
       </c>
@@ -2363,7 +2380,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>111</v>
       </c>
@@ -2377,7 +2394,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>110</v>
       </c>
@@ -2391,7 +2408,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>106</v>
       </c>
@@ -2405,7 +2422,7 @@
         <v>43733</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>115</v>
       </c>
@@ -2419,7 +2436,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>109</v>
       </c>
@@ -2433,7 +2450,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>101</v>
       </c>
@@ -2447,7 +2464,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>100</v>
       </c>
@@ -2461,7 +2478,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>99</v>
       </c>
@@ -2475,7 +2492,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>98</v>
       </c>
@@ -2489,7 +2506,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>97</v>
       </c>
@@ -2503,7 +2520,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>96</v>
       </c>
@@ -2517,7 +2534,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>94</v>
       </c>
@@ -2531,7 +2548,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>95</v>
       </c>
@@ -2545,7 +2562,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>93</v>
       </c>
@@ -2558,11 +2575,11 @@
       <c r="D45" s="19">
         <v>43737</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2576,7 +2593,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>83</v>
       </c>
@@ -2593,7 +2610,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>74</v>
       </c>
@@ -2610,7 +2627,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>84</v>
       </c>
@@ -2627,7 +2644,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>75</v>
       </c>
@@ -2644,7 +2661,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>82</v>
       </c>
@@ -2658,7 +2675,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>89</v>
       </c>
@@ -2672,7 +2689,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>85</v>
       </c>
@@ -2686,7 +2703,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>88</v>
       </c>
@@ -2700,7 +2717,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>86</v>
       </c>
@@ -2714,7 +2731,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>87</v>
       </c>
@@ -2728,7 +2745,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>77</v>
       </c>
@@ -2741,11 +2758,11 @@
       <c r="D57" s="19">
         <v>43730</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>92</v>
       </c>
@@ -2758,11 +2775,11 @@
       <c r="D58" s="19">
         <v>43734</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>78</v>
       </c>
@@ -2776,7 +2793,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>79</v>
       </c>
@@ -2790,7 +2807,7 @@
         <v>43736</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>81</v>
       </c>
@@ -2804,7 +2821,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>80</v>
       </c>
@@ -2818,7 +2835,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>59</v>
       </c>
@@ -2832,7 +2849,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>72</v>
       </c>
@@ -2846,7 +2863,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>65</v>
       </c>
@@ -2860,7 +2877,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>58</v>
       </c>
@@ -2873,11 +2890,11 @@
       <c r="D66" s="30">
         <v>43746</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
@@ -2888,7 +2905,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>71</v>
       </c>
@@ -2902,7 +2919,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>68</v>
       </c>
@@ -2918,8 +2935,11 @@
       <c r="F69" s="2" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G69" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>57</v>
       </c>
@@ -2933,7 +2953,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>56</v>
       </c>
@@ -2944,7 +2964,7 @@
         <v>43713</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>73</v>
       </c>
@@ -2957,12 +2977,12 @@
       <c r="D72" s="19">
         <v>43716</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="N72" s="8"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" s="8"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>55</v>
       </c>
@@ -2976,7 +2996,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>64</v>
       </c>
@@ -2990,7 +3010,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>60</v>
       </c>
@@ -2998,16 +3018,16 @@
         <v>11</v>
       </c>
       <c r="C75" s="19">
-        <v>43670</v>
+        <v>43761</v>
       </c>
       <c r="D75" s="19">
         <v>43717</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="H75" s="2" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>21</v>
       </c>
@@ -3020,11 +3040,11 @@
       <c r="D76" s="19">
         <v>43717</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>63</v>
       </c>
@@ -3038,7 +3058,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>54</v>
       </c>
@@ -3051,11 +3071,11 @@
       <c r="D78" s="19">
         <v>43723</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>66</v>
       </c>
@@ -3069,7 +3089,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>53</v>
       </c>
@@ -3083,7 +3103,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>52</v>
       </c>
@@ -3091,13 +3111,13 @@
         <v>11</v>
       </c>
       <c r="C81" s="19">
-        <v>43670</v>
+        <v>43761</v>
       </c>
       <c r="D81" s="19">
         <v>43726</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>69</v>
       </c>
@@ -3105,13 +3125,13 @@
         <v>11</v>
       </c>
       <c r="C82" s="19">
-        <v>43670</v>
+        <v>43761</v>
       </c>
       <c r="D82" s="19">
         <v>43728</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>62</v>
       </c>
@@ -3127,8 +3147,11 @@
       <c r="F83" s="2" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>51</v>
       </c>
@@ -3136,13 +3159,13 @@
         <v>11</v>
       </c>
       <c r="C84" s="19">
-        <v>43670</v>
+        <v>43761</v>
       </c>
       <c r="D84" s="19">
         <v>43729</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>50</v>
       </c>
@@ -3150,13 +3173,13 @@
         <v>11</v>
       </c>
       <c r="C85" s="19">
-        <v>43670</v>
+        <v>43761</v>
       </c>
       <c r="D85" s="19">
         <v>43730</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>49</v>
       </c>
@@ -3170,7 +3193,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>48</v>
       </c>
@@ -3178,13 +3201,13 @@
         <v>11</v>
       </c>
       <c r="C87" s="19">
-        <v>43670</v>
+        <v>43761</v>
       </c>
       <c r="D87" s="19">
         <v>43732</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>47</v>
       </c>
@@ -3198,7 +3221,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>61</v>
       </c>
@@ -3212,7 +3235,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>70</v>
       </c>
@@ -3226,7 +3249,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>40</v>
       </c>
@@ -3239,11 +3262,11 @@
       <c r="D91" s="19">
         <v>43715</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="H91" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>4</v>
       </c>
@@ -3258,11 +3281,12 @@
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
-      <c r="G92" s="2" t="s">
+      <c r="G92" s="3"/>
+      <c r="H92" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>30</v>
       </c>
@@ -3276,7 +3300,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>29</v>
       </c>
@@ -3287,7 +3311,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>28</v>
       </c>
@@ -3297,11 +3321,11 @@
       <c r="C95" s="19">
         <v>43671</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="H95" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>22</v>
       </c>
@@ -3315,7 +3339,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>39</v>
       </c>
@@ -3323,13 +3347,13 @@
         <v>11</v>
       </c>
       <c r="C97" s="19">
-        <v>43671</v>
+        <v>43762</v>
       </c>
       <c r="D97" s="19">
         <v>43717</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>17</v>
       </c>
@@ -3342,14 +3366,14 @@
       <c r="D98" s="19">
         <v>43714</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="H98" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="I98" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>248</v>
       </c>
@@ -3362,11 +3386,11 @@
       <c r="D99" s="19">
         <v>43718</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="H99" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>38</v>
       </c>
@@ -3374,13 +3398,13 @@
         <v>11</v>
       </c>
       <c r="C100" s="19">
-        <v>43671</v>
+        <v>43762</v>
       </c>
       <c r="D100" s="19">
         <v>43722</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>23</v>
       </c>
@@ -3394,7 +3418,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>26</v>
       </c>
@@ -3405,7 +3429,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>37</v>
       </c>
@@ -3419,7 +3443,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>20</v>
       </c>
@@ -3430,7 +3454,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
         <v>31</v>
       </c>
@@ -3443,11 +3467,11 @@
       <c r="D105" s="19">
         <v>43724</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="H105" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>45</v>
       </c>
@@ -3461,7 +3485,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>36</v>
       </c>
@@ -3475,7 +3499,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>46</v>
       </c>
@@ -3486,7 +3510,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>19</v>
       </c>
@@ -3500,7 +3524,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>41</v>
       </c>
@@ -3514,7 +3538,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>35</v>
       </c>
@@ -3528,7 +3552,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>34</v>
       </c>
@@ -3542,7 +3566,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>24</v>
       </c>
@@ -3556,7 +3580,7 @@
         <v>43733</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>25</v>
       </c>
@@ -3570,7 +3594,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="21" t="s">
         <v>44</v>
       </c>
@@ -3584,7 +3608,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>33</v>
       </c>
@@ -3598,7 +3622,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>43</v>
       </c>
@@ -3612,7 +3636,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>32</v>
       </c>
@@ -3626,7 +3650,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>42</v>
       </c>
@@ -3640,7 +3664,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>16</v>
       </c>
@@ -3654,7 +3678,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>15</v>
       </c>
@@ -3668,7 +3692,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>14</v>
       </c>
@@ -3681,11 +3705,11 @@
       <c r="D122" s="19">
         <v>43712</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="H122" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>12</v>
       </c>
@@ -3698,14 +3722,14 @@
       <c r="D123" s="19">
         <v>43730</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="H123" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="H123" s="2" t="s">
+      <c r="I123" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>13</v>
       </c>
@@ -3718,11 +3742,11 @@
       <c r="D124" s="19">
         <v>43736</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="H124" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
         <v>186</v>
       </c>
@@ -3735,11 +3759,11 @@
       <c r="D125" s="30">
         <v>43745</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="H125" s="2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
         <v>314</v>
       </c>
@@ -3753,7 +3777,7 @@
         <v>43733</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
         <v>322</v>
       </c>
@@ -3767,7 +3791,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>259</v>
       </c>
@@ -3781,7 +3805,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>138</v>
       </c>
@@ -3794,14 +3818,14 @@
       <c r="D129" s="19">
         <v>43714</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="H129" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="H129" s="2" t="s">
+      <c r="I129" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>291</v>
       </c>
@@ -3814,11 +3838,11 @@
       <c r="D130" s="19">
         <v>43728</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="H130" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>294</v>
       </c>
@@ -3832,7 +3856,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>346</v>
       </c>
@@ -3846,7 +3870,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>158</v>
       </c>
@@ -3860,7 +3884,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
         <v>184</v>
       </c>
@@ -3874,7 +3898,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>189</v>
       </c>
@@ -3888,7 +3912,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>194</v>
       </c>
@@ -3902,7 +3926,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>360</v>
       </c>
@@ -3916,7 +3940,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>206</v>
       </c>
@@ -3930,7 +3954,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>162</v>
       </c>
@@ -3944,7 +3968,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
         <v>212</v>
       </c>
@@ -3958,7 +3982,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>163</v>
       </c>
@@ -3972,7 +3996,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
         <v>219</v>
       </c>
@@ -3985,11 +4009,11 @@
       <c r="D142" s="30">
         <v>43749</v>
       </c>
-      <c r="G142" s="2" t="s">
+      <c r="H142" s="2" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>225</v>
       </c>
@@ -4002,11 +4026,11 @@
       <c r="D143" s="19">
         <v>43714</v>
       </c>
-      <c r="G143" s="2" t="s">
+      <c r="H143" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>168</v>
       </c>
@@ -4020,7 +4044,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
         <v>249</v>
       </c>
@@ -4034,7 +4058,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>251</v>
       </c>
@@ -4048,7 +4072,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
         <v>261</v>
       </c>
@@ -4062,7 +4086,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>171</v>
       </c>
@@ -4076,7 +4100,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
         <v>276</v>
       </c>
@@ -4090,7 +4114,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
         <v>283</v>
       </c>
@@ -4104,7 +4128,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>288</v>
       </c>
@@ -4118,7 +4142,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>289</v>
       </c>
@@ -4132,7 +4156,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>290</v>
       </c>
@@ -4146,7 +4170,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>295</v>
       </c>
@@ -4160,7 +4184,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>174</v>
       </c>
@@ -4174,7 +4198,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>298</v>
       </c>
@@ -4187,11 +4211,11 @@
       <c r="D156" s="19">
         <v>43729</v>
       </c>
-      <c r="G156" s="2" t="s">
+      <c r="H156" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>315</v>
       </c>
@@ -4205,7 +4229,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>320</v>
       </c>
@@ -4219,7 +4243,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>342</v>
       </c>
@@ -4233,7 +4257,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>344</v>
       </c>
@@ -4247,7 +4271,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" s="9" t="s">
         <v>350</v>
       </c>
@@ -4261,7 +4285,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
         <v>352</v>
       </c>
@@ -4275,7 +4299,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>187</v>
       </c>
@@ -4289,7 +4313,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
         <v>211</v>
       </c>
@@ -4303,7 +4327,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
         <v>234</v>
       </c>
@@ -4317,7 +4341,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
         <v>235</v>
       </c>
@@ -4330,9 +4354,9 @@
       <c r="D166" s="19">
         <v>43716</v>
       </c>
-      <c r="N166" s="8"/>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O166" s="8"/>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
         <v>242</v>
       </c>
@@ -4345,11 +4369,11 @@
       <c r="D167" s="19">
         <v>43718</v>
       </c>
-      <c r="G167" s="2" t="s">
+      <c r="H167" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
         <v>244</v>
       </c>
@@ -4363,7 +4387,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
         <v>246</v>
       </c>
@@ -4377,7 +4401,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
         <v>255</v>
       </c>
@@ -4391,7 +4415,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>170</v>
       </c>
@@ -4405,7 +4429,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
         <v>274</v>
       </c>
@@ -4419,7 +4443,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
         <v>275</v>
       </c>
@@ -4433,7 +4457,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" s="8" t="s">
         <v>278</v>
       </c>
@@ -4447,7 +4471,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
         <v>282</v>
       </c>
@@ -4463,8 +4487,11 @@
       <c r="F175" s="2" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G175" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" s="10" t="s">
         <v>141</v>
       </c>
@@ -4477,14 +4504,14 @@
       <c r="D176" s="19">
         <v>43728</v>
       </c>
-      <c r="G176" s="2" t="s">
+      <c r="H176" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="H176" s="2" t="s">
+      <c r="I176" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="8" t="s">
         <v>176</v>
       </c>
@@ -4498,7 +4525,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>143</v>
       </c>
@@ -4511,14 +4538,14 @@
       <c r="D178" s="19">
         <v>43730</v>
       </c>
-      <c r="G178" s="2" t="s">
+      <c r="H178" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="H178" s="2" t="s">
+      <c r="I178" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>308</v>
       </c>
@@ -4532,7 +4559,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="8" t="s">
         <v>316</v>
       </c>
@@ -4546,7 +4573,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="8" t="s">
         <v>319</v>
       </c>
@@ -4560,7 +4587,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="8" t="s">
         <v>327</v>
       </c>
@@ -4574,7 +4601,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="8" t="s">
         <v>335</v>
       </c>
@@ -4588,7 +4615,7 @@
         <v>43736</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="8" t="s">
         <v>178</v>
       </c>
@@ -4602,7 +4629,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
         <v>343</v>
       </c>
@@ -4616,7 +4643,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="8" t="s">
         <v>181</v>
       </c>
@@ -4629,14 +4656,14 @@
       <c r="D186" s="19">
         <v>43715</v>
       </c>
-      <c r="G186" s="2" t="s">
+      <c r="H186" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="H186" s="2" t="s">
+      <c r="I186" s="2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="8" t="s">
         <v>190</v>
       </c>
@@ -4650,7 +4677,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>191</v>
       </c>
@@ -4664,7 +4691,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="8" t="s">
         <v>204</v>
       </c>
@@ -4678,7 +4705,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
         <v>209</v>
       </c>
@@ -4692,7 +4719,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>213</v>
       </c>
@@ -4706,7 +4733,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>145</v>
       </c>
@@ -4719,11 +4746,11 @@
       <c r="D192" s="19">
         <v>43715</v>
       </c>
-      <c r="G192" s="2" t="s">
+      <c r="H192" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
         <v>218</v>
       </c>
@@ -4737,7 +4764,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>227</v>
       </c>
@@ -4751,7 +4778,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
         <v>231</v>
       </c>
@@ -4764,9 +4791,9 @@
       <c r="D195" s="19">
         <v>43716</v>
       </c>
-      <c r="N195" s="8"/>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O195" s="8"/>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
         <v>167</v>
       </c>
@@ -4779,11 +4806,11 @@
       <c r="D196" s="19">
         <v>43718</v>
       </c>
-      <c r="G196" s="2" t="s">
+      <c r="H196" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" s="8" t="s">
         <v>247</v>
       </c>
@@ -4797,7 +4824,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
         <v>257</v>
       </c>
@@ -4811,7 +4838,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>281</v>
       </c>
@@ -4824,11 +4851,11 @@
       <c r="D199" s="19">
         <v>43725</v>
       </c>
-      <c r="G199" s="2" t="s">
+      <c r="H199" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
         <v>284</v>
       </c>
@@ -4842,7 +4869,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" s="11" t="s">
         <v>172</v>
       </c>
@@ -4856,7 +4883,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
         <v>296</v>
       </c>
@@ -4870,7 +4897,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
         <v>300</v>
       </c>
@@ -4884,7 +4911,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
         <v>301</v>
       </c>
@@ -4898,7 +4925,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" s="8" t="s">
         <v>313</v>
       </c>
@@ -4912,7 +4939,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>149</v>
       </c>
@@ -4925,11 +4952,11 @@
       <c r="D206" s="19">
         <v>43715</v>
       </c>
-      <c r="G206" s="2" t="s">
+      <c r="H206" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" s="8" t="s">
         <v>252</v>
       </c>
@@ -4943,7 +4970,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>306</v>
       </c>
@@ -4957,7 +4984,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
         <v>321</v>
       </c>
@@ -4971,7 +4998,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
         <v>193</v>
       </c>
@@ -4985,7 +5012,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" s="8" t="s">
         <v>264</v>
       </c>
@@ -4999,7 +5026,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
         <v>331</v>
       </c>
@@ -5013,7 +5040,7 @@
         <v>43736</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
         <v>201</v>
       </c>
@@ -5027,7 +5054,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
         <v>226</v>
       </c>
@@ -5041,7 +5068,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
         <v>229</v>
       </c>
@@ -5055,7 +5082,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
         <v>237</v>
       </c>
@@ -5068,9 +5095,9 @@
       <c r="D216" s="19">
         <v>43716</v>
       </c>
-      <c r="N216" s="8"/>
-    </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O216" s="8"/>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
         <v>238</v>
       </c>
@@ -5084,7 +5111,7 @@
         <v>43717</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>150</v>
       </c>
@@ -5098,7 +5125,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>152</v>
       </c>
@@ -5111,11 +5138,11 @@
       <c r="D219" s="19">
         <v>43722</v>
       </c>
-      <c r="G219" s="2" t="s">
+      <c r="H219" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
         <v>269</v>
       </c>
@@ -5129,7 +5156,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
         <v>271</v>
       </c>
@@ -5143,7 +5170,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" s="8" t="s">
         <v>286</v>
       </c>
@@ -5157,7 +5184,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>156</v>
       </c>
@@ -5170,14 +5197,14 @@
       <c r="D223" s="19">
         <v>43730</v>
       </c>
-      <c r="G223" s="2" t="s">
+      <c r="H223" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="H223" s="2" t="s">
+      <c r="I223" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" s="8" t="s">
         <v>311</v>
       </c>
@@ -5191,7 +5218,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
         <v>325</v>
       </c>
@@ -5205,7 +5232,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" s="8" t="s">
         <v>351</v>
       </c>
@@ -5219,7 +5246,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" s="8" t="s">
         <v>354</v>
       </c>
@@ -5233,7 +5260,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
         <v>185</v>
       </c>
@@ -5247,7 +5274,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" s="8" t="s">
         <v>195</v>
       </c>
@@ -5261,7 +5288,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" s="8" t="s">
         <v>200</v>
       </c>
@@ -5275,7 +5302,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" s="8" t="s">
         <v>208</v>
       </c>
@@ -5289,7 +5316,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" s="12" t="s">
         <v>215</v>
       </c>
@@ -5303,7 +5330,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>146</v>
       </c>
@@ -5316,11 +5343,11 @@
       <c r="D233" s="19">
         <v>43715</v>
       </c>
-      <c r="G233" s="2" t="s">
+      <c r="H233" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" s="8" t="s">
         <v>236</v>
       </c>
@@ -5333,12 +5360,12 @@
       <c r="D234" s="19">
         <v>43716</v>
       </c>
-      <c r="G234" s="2" t="s">
+      <c r="H234" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="N234" s="6"/>
-    </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O234" s="6"/>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>151</v>
       </c>
@@ -5351,11 +5378,11 @@
       <c r="D235" s="19">
         <v>43723</v>
       </c>
-      <c r="G235" s="2" t="s">
+      <c r="H235" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
         <v>270</v>
       </c>
@@ -5369,7 +5396,7 @@
         <v>43724</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>153</v>
       </c>
@@ -5382,11 +5409,11 @@
       <c r="D237" s="19">
         <v>43725</v>
       </c>
-      <c r="G237" s="2" t="s">
+      <c r="H237" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" s="8" t="s">
         <v>175</v>
       </c>
@@ -5400,7 +5427,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" s="8" t="s">
         <v>159</v>
       </c>
@@ -5414,7 +5441,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" s="8" t="s">
         <v>196</v>
       </c>
@@ -5428,7 +5455,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>148</v>
       </c>
@@ -5442,7 +5469,7 @@
         <v>43715</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A242" s="8" t="s">
         <v>233</v>
       </c>
@@ -5455,12 +5482,12 @@
       <c r="D242" s="19">
         <v>43716</v>
       </c>
-      <c r="G242" s="2" t="s">
+      <c r="H242" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="N242" s="4"/>
-    </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O242" s="4"/>
+    </row>
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>155</v>
       </c>
@@ -5473,11 +5500,11 @@
       <c r="D243" s="19">
         <v>43728</v>
       </c>
-      <c r="G243" s="2" t="s">
+      <c r="H243" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A244" s="22" t="s">
         <v>332</v>
       </c>
@@ -5490,11 +5517,11 @@
       <c r="D244" s="19">
         <v>43736</v>
       </c>
-      <c r="G244" s="2" t="s">
+      <c r="H244" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A245" s="8" t="s">
         <v>334</v>
       </c>
@@ -5507,11 +5534,11 @@
       <c r="D245" s="19">
         <v>43736</v>
       </c>
-      <c r="G245" s="2" t="s">
+      <c r="H245" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
         <v>339</v>
       </c>
@@ -5525,7 +5552,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A247" s="26" t="s">
         <v>348</v>
       </c>
@@ -5538,11 +5565,11 @@
       <c r="D247" s="19">
         <v>43737</v>
       </c>
-      <c r="G247" s="2" t="s">
+      <c r="H247" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
         <v>337</v>
       </c>
@@ -5556,7 +5583,7 @@
         <v>43736</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A249" s="8" t="s">
         <v>323</v>
       </c>
@@ -5570,7 +5597,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
         <v>258</v>
       </c>
@@ -5584,7 +5611,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A251" s="7" t="s">
         <v>207</v>
       </c>
@@ -5597,11 +5624,11 @@
       <c r="D251" s="30">
         <v>43747</v>
       </c>
-      <c r="G251" s="2" t="s">
+      <c r="H251" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A252" s="8" t="s">
         <v>220</v>
       </c>
@@ -5614,11 +5641,11 @@
       <c r="D252" s="30">
         <v>43749</v>
       </c>
-      <c r="G252" s="2" t="s">
+      <c r="H252" s="2" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A253" s="8" t="s">
         <v>293</v>
       </c>
@@ -5632,7 +5659,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" s="8" t="s">
         <v>299</v>
       </c>
@@ -5646,7 +5673,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A255" s="8" t="s">
         <v>188</v>
       </c>
@@ -5660,7 +5687,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A256" s="7" t="s">
         <v>161</v>
       </c>
@@ -5674,7 +5701,7 @@
         <v>43746</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="8" t="s">
         <v>223</v>
       </c>
@@ -5686,7 +5713,7 @@
       </c>
       <c r="D257" s="19"/>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="8" t="s">
         <v>197</v>
       </c>
@@ -5700,7 +5727,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="6" t="s">
         <v>169</v>
       </c>
@@ -5714,7 +5741,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="8" t="s">
         <v>326</v>
       </c>
@@ -5728,7 +5755,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="8" t="s">
         <v>330</v>
       </c>
@@ -5742,7 +5769,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="8" t="s">
         <v>345</v>
       </c>
@@ -5756,7 +5783,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
         <v>183</v>
       </c>
@@ -5770,7 +5797,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
         <v>205</v>
       </c>
@@ -5783,14 +5810,14 @@
       <c r="D264" s="19">
         <v>43729</v>
       </c>
-      <c r="G264" s="2" t="s">
+      <c r="H264" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="I264" s="2" t="s">
+      <c r="J264" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>91</v>
       </c>
@@ -5804,7 +5831,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="8" t="s">
         <v>217</v>
       </c>
@@ -5817,11 +5844,11 @@
       <c r="D266" s="30">
         <v>43749</v>
       </c>
-      <c r="G266" s="2" t="s">
+      <c r="H266" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="8" t="s">
         <v>250</v>
       </c>
@@ -5835,7 +5862,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="8" t="s">
         <v>260</v>
       </c>
@@ -5848,11 +5875,11 @@
       <c r="D268" s="19">
         <v>43723</v>
       </c>
-      <c r="G268" s="2" t="s">
+      <c r="H268" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>312</v>
       </c>
@@ -5866,7 +5893,7 @@
         <v>43732</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="8" t="s">
         <v>318</v>
       </c>
@@ -5880,7 +5907,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="8" t="s">
         <v>333</v>
       </c>
@@ -5894,7 +5921,7 @@
         <v>43736</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="8" t="s">
         <v>341</v>
       </c>
@@ -5908,7 +5935,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="8" t="s">
         <v>203</v>
       </c>
@@ -5922,7 +5949,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
         <v>241</v>
       </c>
@@ -5936,7 +5963,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="8" t="s">
         <v>179</v>
       </c>
@@ -5950,7 +5977,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="8" t="s">
         <v>240</v>
       </c>
@@ -5964,7 +5991,7 @@
         <v>43718</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
         <v>262</v>
       </c>
@@ -5978,7 +6005,7 @@
         <v>43723</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="8" t="s">
         <v>297</v>
       </c>
@@ -5992,7 +6019,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>0</v>
       </c>
@@ -6005,11 +6032,11 @@
       <c r="D279" s="19">
         <v>43733</v>
       </c>
-      <c r="G279" s="2" t="s">
+      <c r="H279" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>317</v>
       </c>
@@ -6023,7 +6050,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="8" t="s">
         <v>192</v>
       </c>
@@ -6037,7 +6064,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="8" t="s">
         <v>202</v>
       </c>
@@ -6051,7 +6078,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>224</v>
       </c>
@@ -6065,7 +6092,7 @@
         <v>43714</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="8" t="s">
         <v>340</v>
       </c>
@@ -6079,7 +6106,7 @@
         <v>43737</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="8" t="s">
         <v>277</v>
       </c>
@@ -6093,7 +6120,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>139</v>
       </c>
@@ -6106,11 +6133,11 @@
       <c r="D286" s="19">
         <v>43714</v>
       </c>
-      <c r="G286" s="2" t="s">
+      <c r="H286" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
         <v>214</v>
       </c>
@@ -6124,7 +6151,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="8" t="s">
         <v>254</v>
       </c>
@@ -6138,7 +6165,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A289" s="8" t="s">
         <v>292</v>
       </c>
@@ -6152,7 +6179,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A290" s="8" t="s">
         <v>198</v>
       </c>
@@ -6166,7 +6193,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A291" s="8" t="s">
         <v>216</v>
       </c>
@@ -6179,11 +6206,11 @@
       <c r="D291" s="19">
         <v>43729</v>
       </c>
-      <c r="G291" s="2" t="s">
+      <c r="H291" s="2" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A292" s="8" t="s">
         <v>253</v>
       </c>
@@ -6197,7 +6224,7 @@
         <v>43722</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A293" s="8" t="s">
         <v>273</v>
       </c>
@@ -6211,7 +6238,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A294" s="8" t="s">
         <v>355</v>
       </c>
@@ -6224,11 +6251,11 @@
       <c r="D294" s="19">
         <v>43737</v>
       </c>
-      <c r="G294" s="2" t="s">
+      <c r="H294" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A295" s="8" t="s">
         <v>310</v>
       </c>
@@ -6242,7 +6269,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A296" s="7" t="s">
         <v>160</v>
       </c>
@@ -6256,7 +6283,7 @@
         <v>43729</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A297" s="28" t="s">
         <v>413</v>
       </c>
@@ -6270,7 +6297,7 @@
         <v>43739</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A298" s="8" t="s">
         <v>182</v>
       </c>
@@ -6283,11 +6310,11 @@
       <c r="D298" s="19">
         <v>43729</v>
       </c>
-      <c r="G298" s="2" t="s">
+      <c r="H298" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A299" s="8" t="s">
         <v>165</v>
       </c>
@@ -6301,7 +6328,7 @@
         <v>43726</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A300" s="28" t="s">
         <v>424</v>
       </c>
@@ -6314,12 +6341,12 @@
       <c r="D300" s="19">
         <v>43739</v>
       </c>
-      <c r="G300" s="2" t="s">
+      <c r="H300" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="J300" s="5"/>
-    </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K300" s="5"/>
+    </row>
+    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A301" s="8" t="s">
         <v>228</v>
       </c>
@@ -6332,9 +6359,9 @@
       <c r="D301" s="19">
         <v>43729</v>
       </c>
-      <c r="N301" s="6"/>
-    </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O301" s="6"/>
+    </row>
+    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>128</v>
       </c>
@@ -6348,7 +6375,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A303" s="8" t="s">
         <v>265</v>
       </c>
@@ -6362,7 +6389,7 @@
         <v>43738</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A304" s="8" t="s">
         <v>173</v>
       </c>
@@ -6375,11 +6402,11 @@
       <c r="D304" s="19">
         <v>43738</v>
       </c>
-      <c r="G304" s="2" t="s">
+      <c r="H304" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="8" t="s">
         <v>279</v>
       </c>
@@ -6393,7 +6420,7 @@
         <v>43740</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="8" t="s">
         <v>199</v>
       </c>
@@ -6406,11 +6433,11 @@
       <c r="D306" s="19">
         <v>43740</v>
       </c>
-      <c r="G306" s="2" t="s">
+      <c r="H306" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="8" t="s">
         <v>268</v>
       </c>
@@ -6424,7 +6451,7 @@
         <v>43740</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="12" t="s">
         <v>309</v>
       </c>
@@ -6437,11 +6464,11 @@
       <c r="D308" s="19">
         <v>43745</v>
       </c>
-      <c r="G308" s="2" t="s">
+      <c r="H308" s="2" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="12" t="s">
         <v>164</v>
       </c>
@@ -6455,7 +6482,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" s="8" t="s">
         <v>221</v>
       </c>
@@ -6469,7 +6496,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>127</v>
       </c>
@@ -6483,7 +6510,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>133</v>
       </c>
@@ -6497,7 +6524,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>126</v>
       </c>
@@ -6511,7 +6538,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" s="10" t="s">
         <v>18</v>
       </c>
@@ -6525,7 +6552,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" s="10" t="s">
         <v>125</v>
       </c>
@@ -6539,7 +6566,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>117</v>
       </c>
@@ -6553,7 +6580,7 @@
         <v>43754</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>123</v>
       </c>
@@ -6567,7 +6594,7 @@
         <v>43765</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>120</v>
       </c>
@@ -6581,7 +6608,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>135</v>
       </c>
@@ -6594,11 +6621,11 @@
       <c r="D319" s="19">
         <v>43766</v>
       </c>
-      <c r="G319" s="2" t="s">
+      <c r="H319" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" s="8" t="s">
         <v>180</v>
       </c>
@@ -6606,7 +6633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="8" t="s">
         <v>210</v>
       </c>
@@ -6617,11 +6644,11 @@
         <v>43754</v>
       </c>
       <c r="D321" s="19"/>
-      <c r="G321" s="2" t="s">
+      <c r="H321" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="33" t="s">
         <v>415</v>
       </c>
@@ -6632,45 +6659,45 @@
         <v>43760</v>
       </c>
       <c r="D322" s="19"/>
-      <c r="G322" s="2" t="s">
+      <c r="H322" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="J322" s="5"/>
-    </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A323" s="11" t="s">
+      <c r="K322" s="5"/>
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A323" s="8" t="s">
         <v>232</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G323" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H323" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="G324" s="2" t="s">
+      <c r="H324" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="11" t="s">
         <v>243</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G325" s="2" t="s">
+      <c r="H325" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="14" t="s">
         <v>27</v>
       </c>
@@ -6678,11 +6705,11 @@
         <v>11</v>
       </c>
       <c r="C326" s="19"/>
-      <c r="G326" s="2" t="s">
+      <c r="H326" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
         <v>256</v>
       </c>
@@ -6690,15 +6717,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="G328" s="2" t="s">
+      <c r="H328" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="32" t="s">
         <v>266</v>
       </c>
@@ -6708,41 +6735,41 @@
       <c r="C329" s="19">
         <v>43754</v>
       </c>
-      <c r="G329" s="2" t="s">
+      <c r="H329" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="G330" s="2" t="s">
+      <c r="H330" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="11" t="s">
         <v>272</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G331" s="2" t="s">
+      <c r="H331" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="11" t="s">
         <v>280</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G332" s="2" t="s">
+      <c r="H332" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="11" t="s">
         <v>287</v>
       </c>
@@ -6752,21 +6779,21 @@
       <c r="D333" s="19">
         <v>43726</v>
       </c>
-      <c r="G333" s="2" t="s">
+      <c r="H333" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="16" t="s">
         <v>304</v>
       </c>
@@ -6774,7 +6801,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="4" t="s">
         <v>177</v>
       </c>
@@ -6782,24 +6809,24 @@
         <v>399</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
         <v>307</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G338" s="2" t="s">
+      <c r="H338" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="14" t="s">
         <v>108</v>
       </c>
       <c r="D339" s="19"/>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="11" t="s">
         <v>324</v>
       </c>
@@ -6807,7 +6834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="11" t="s">
         <v>328</v>
       </c>
@@ -6815,7 +6842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="20" t="s">
         <v>349</v>
       </c>
@@ -6823,7 +6850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>423</v>
       </c>
@@ -6836,56 +6863,68 @@
       <c r="D343" s="19">
         <v>43838</v>
       </c>
-      <c r="J343" s="5"/>
-    </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J344" s="5"/>
-    </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J345" s="5"/>
-    </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J346" s="5"/>
-    </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J347" s="5"/>
-    </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J348" s="5"/>
-    </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J349" s="5"/>
-    </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J350" s="5"/>
-    </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J351" s="5"/>
-    </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J352" s="5"/>
-    </row>
-    <row r="353" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J353" s="5"/>
-    </row>
-    <row r="354" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J354" s="5"/>
-    </row>
-    <row r="355" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J355" s="5"/>
-    </row>
-    <row r="356" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J356" s="5"/>
-    </row>
-    <row r="357" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J357" s="5"/>
-    </row>
-    <row r="358" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J358" s="5"/>
+      <c r="K343" s="5"/>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A344" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C344" s="19">
+        <v>43761</v>
+      </c>
+      <c r="D344" s="19">
+        <v>43838</v>
+      </c>
+      <c r="K344" s="5"/>
+    </row>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K345" s="5"/>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K346" s="5"/>
+    </row>
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K347" s="5"/>
+    </row>
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K348" s="5"/>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K349" s="5"/>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K350" s="5"/>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K351" s="5"/>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K352" s="5"/>
+    </row>
+    <row r="353" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K353" s="5"/>
+    </row>
+    <row r="354" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K354" s="5"/>
+    </row>
+    <row r="355" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K355" s="5"/>
+    </row>
+    <row r="356" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K356" s="5"/>
+    </row>
+    <row r="357" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K357" s="5"/>
+    </row>
+    <row r="358" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K358" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A352" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N358">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O358">
     <sortCondition ref="C2:C358"/>
   </sortState>
   <conditionalFormatting sqref="A142:A339">
@@ -6894,31 +6933,31 @@
   <conditionalFormatting sqref="A142:A339">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J341:J343">
+  <conditionalFormatting sqref="K341:K343">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J344">
+  <conditionalFormatting sqref="K344">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J345:J347">
+  <conditionalFormatting sqref="K345:K347">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J346:J347">
+  <conditionalFormatting sqref="K346:K347">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J346:J347">
+  <conditionalFormatting sqref="K346:K347">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J348:J358">
+  <conditionalFormatting sqref="K348:K358">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J348:J358">
+  <conditionalFormatting sqref="K348:K358">
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N105:N119">
+  <conditionalFormatting sqref="O105:O119">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RECN renamed to RGP
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAEAA36-8221-4B3B-987E-7462D685C85C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393CB95C-655C-4E58-98A3-E18CB38D3866}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72465" yWindow="135" windowWidth="13920" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Main!$A$1:$M$292</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="558">
   <si>
     <t>SCVL</t>
   </si>
@@ -1704,6 +1703,9 @@
   </si>
   <si>
     <t>SNX</t>
+  </si>
+  <si>
+    <t>RGP</t>
   </si>
 </sst>
 </file>
@@ -3906,8 +3908,8 @@
   <dimension ref="A1:M410"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C336" sqref="C336"/>
+      <pane ySplit="1" topLeftCell="A303" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A316" sqref="A316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8218,7 +8220,7 @@
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" s="18" t="s">
-        <v>300</v>
+        <v>557</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
HIIQ changed to BFYT
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DA8756-66EB-4FA1-AA44-B17BA8D5C70A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E8A980-12A5-480F-B518-D6A4A9768841}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72450" yWindow="90" windowWidth="13920" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73425" yWindow="90" windowWidth="12945" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="560">
   <si>
     <t>SCVL</t>
   </si>
@@ -1709,6 +1709,9 @@
   </si>
   <si>
     <t>BAX</t>
+  </si>
+  <si>
+    <t>BFYT</t>
   </si>
 </sst>
 </file>
@@ -3911,8 +3914,8 @@
   <dimension ref="A1:M411"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A402" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A412" sqref="A412"/>
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6414,7 +6417,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="10" t="s">
-        <v>446</v>
+        <v>559</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
More updtes and adding JNJ
</commit_message>
<xml_diff>
--- a/User_Files/Master_Tracklist.xlsx
+++ b/User_Files/Master_Tracklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E8A980-12A5-480F-B518-D6A4A9768841}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDDFD18-593B-4A48-9F63-DB39355D9A0A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73425" yWindow="90" windowWidth="12945" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73080" yWindow="150" windowWidth="12720" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="561">
   <si>
     <t>SCVL</t>
   </si>
@@ -1712,6 +1712,9 @@
   </si>
   <si>
     <t>BFYT</t>
+  </si>
+  <si>
+    <t>JNJ</t>
   </si>
 </sst>
 </file>
@@ -3911,11 +3914,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M411"/>
+  <dimension ref="A1:M412"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A180" sqref="A180"/>
+      <pane ySplit="1" topLeftCell="A396" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A413" sqref="A413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9411,6 +9414,14 @@
         <v>556</v>
       </c>
       <c r="B411" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A412" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="B412" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>